<commit_message>
Ajustes titulos de escaleta
Ajustes escaleta
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado06/guion11/ESCALETA MA_06_11_CO.xlsx
+++ b/fuentes/contenidos/grado06/guion11/ESCALETA MA_06_11_CO.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11595"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="30180" windowHeight="13260"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja2" sheetId="2" r:id="rId1"/>
@@ -13,12 +13,17 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja2!$K$1:$K$284</definedName>
   </definedNames>
-  <calcPr calcId="144525" iterateCount="2" iterateDelta="10"/>
+  <calcPr calcId="140001" iterateCount="2" iterateDelta="10" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="506" uniqueCount="216">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="506" uniqueCount="215">
   <si>
     <t>Asignatura</t>
   </si>
@@ -402,12 +407,6 @@
     <t>La clasificación de los polígonos</t>
   </si>
   <si>
-    <t>Clasifica polígonos:según la medida de sus  ángulos</t>
-  </si>
-  <si>
-    <t>Clasifica polígonos:según la medida de sus lados</t>
-  </si>
-  <si>
     <t>Clasifica polígonos</t>
   </si>
   <si>
@@ -432,9 +431,6 @@
     <t>Refuerza tu aprendizaje: Los triángulos</t>
   </si>
   <si>
-    <t>¿Qué sabes de los cuadriláteros?</t>
-  </si>
-  <si>
     <t xml:space="preserve">Identifica cuadriláteros </t>
   </si>
   <si>
@@ -573,9 +569,6 @@
     <t>Actividades sobre Los triángulos</t>
   </si>
   <si>
-    <t>Actividad para emitir juicios sobre afirmaciones sobre los caudriláteros</t>
-  </si>
-  <si>
     <t xml:space="preserve">Actividad para caracterizar cuadriláteros </t>
   </si>
   <si>
@@ -591,9 +584,6 @@
     <t xml:space="preserve">Actividad que plantea asociar diferentes posiciones relativas de una cirdunferencia respecto a rectas u otra circunferencia </t>
   </si>
   <si>
-    <t>Refuerza tu aprendixaje: Los cuadriláteros</t>
-  </si>
-  <si>
     <t>Actividad que propone aplicar los pasos necesarios para reconocer y relacionar los elementos de la circunferencia</t>
   </si>
   <si>
@@ -667,6 +657,18 @@
   </si>
   <si>
     <t>RM_01_01_CO</t>
+  </si>
+  <si>
+    <t>Clasifica polígonos según la medida de sus  ángulos</t>
+  </si>
+  <si>
+    <t>Clasifica polígonos según la medida de sus lados</t>
+  </si>
+  <si>
+    <t>Actividad para emitir juicios sobre afirmaciones relacionadas con los cuadriláteros</t>
+  </si>
+  <si>
+    <t>Reconoce información sobre los cuadriláteros</t>
   </si>
 </sst>
 </file>
@@ -804,97 +806,97 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="double">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="hair">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="hair">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom style="hair">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="hair">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="hair">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="hair">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="hair">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom/>
       <diagonal/>
@@ -903,36 +905,36 @@
       <left/>
       <right/>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right/>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right/>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="double">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1062,16 +1064,31 @@
     <xf numFmtId="0" fontId="4" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1111,21 +1128,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1434,143 +1436,143 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U121"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="U17" sqref="U17"/>
+      <selection pane="bottomLeft" activeCell="O18" sqref="O18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="16.5703125" style="20" customWidth="1"/>
-    <col min="2" max="2" width="24.5703125" style="20" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.5" style="20" customWidth="1"/>
+    <col min="2" max="2" width="24.5" style="20" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="31" style="20" customWidth="1"/>
-    <col min="4" max="4" width="22.7109375" style="20" customWidth="1"/>
-    <col min="5" max="5" width="22.140625" style="44" customWidth="1"/>
-    <col min="6" max="6" width="23.5703125" style="43" customWidth="1"/>
-    <col min="7" max="7" width="25.85546875" style="20" customWidth="1"/>
-    <col min="8" max="8" width="12.28515625" style="43" customWidth="1"/>
+    <col min="4" max="4" width="22.6640625" style="20" customWidth="1"/>
+    <col min="5" max="5" width="22.1640625" style="44" customWidth="1"/>
+    <col min="6" max="6" width="23.5" style="43" customWidth="1"/>
+    <col min="7" max="7" width="25.83203125" style="20" customWidth="1"/>
+    <col min="8" max="8" width="12.33203125" style="43" customWidth="1"/>
     <col min="9" max="9" width="11" style="43" customWidth="1"/>
-    <col min="10" max="10" width="73.5703125" style="28" customWidth="1"/>
-    <col min="11" max="11" width="13.28515625" style="20" customWidth="1"/>
-    <col min="12" max="12" width="17.42578125" style="20" customWidth="1"/>
-    <col min="13" max="14" width="9.28515625" style="20" customWidth="1"/>
-    <col min="15" max="15" width="58.5703125" style="43" customWidth="1"/>
-    <col min="16" max="16" width="16.5703125" style="43" customWidth="1"/>
-    <col min="17" max="17" width="20.42578125" style="43" customWidth="1"/>
+    <col min="10" max="10" width="73.5" style="28" customWidth="1"/>
+    <col min="11" max="11" width="13.33203125" style="20" customWidth="1"/>
+    <col min="12" max="12" width="17.5" style="20" customWidth="1"/>
+    <col min="13" max="14" width="9.33203125" style="20" customWidth="1"/>
+    <col min="15" max="15" width="58.5" style="43" customWidth="1"/>
+    <col min="16" max="16" width="16.5" style="43" customWidth="1"/>
+    <col min="17" max="17" width="20.5" style="43" customWidth="1"/>
     <col min="18" max="18" width="23" style="20" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="20.7109375" style="20" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="25.85546875" style="20" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="21.7109375" style="20" customWidth="1"/>
-    <col min="22" max="16384" width="11.42578125" style="20"/>
+    <col min="19" max="19" width="20.6640625" style="20" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="25.83203125" style="20" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="21.6640625" style="20" customWidth="1"/>
+    <col min="22" max="16384" width="10.83203125" style="20"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="57" t="s">
+    <row r="1" spans="1:21" ht="33.75" customHeight="1">
+      <c r="A1" s="62" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="55" t="s">
+      <c r="B1" s="60" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="66" t="s">
+      <c r="C1" s="71" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="57" t="s">
+      <c r="D1" s="62" t="s">
         <v>110</v>
       </c>
-      <c r="E1" s="55" t="s">
+      <c r="E1" s="60" t="s">
         <v>111</v>
       </c>
-      <c r="F1" s="51" t="s">
+      <c r="F1" s="58" t="s">
         <v>112</v>
       </c>
-      <c r="G1" s="59" t="s">
+      <c r="G1" s="64" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="51" t="s">
+      <c r="H1" s="58" t="s">
         <v>113</v>
       </c>
-      <c r="I1" s="51" t="s">
+      <c r="I1" s="58" t="s">
         <v>107</v>
       </c>
-      <c r="J1" s="63" t="s">
+      <c r="J1" s="68" t="s">
         <v>4</v>
       </c>
-      <c r="K1" s="61" t="s">
+      <c r="K1" s="66" t="s">
         <v>108</v>
       </c>
-      <c r="L1" s="59" t="s">
+      <c r="L1" s="64" t="s">
         <v>14</v>
       </c>
-      <c r="M1" s="65" t="s">
+      <c r="M1" s="70" t="s">
         <v>21</v>
       </c>
-      <c r="N1" s="65"/>
-      <c r="O1" s="53" t="s">
+      <c r="N1" s="70"/>
+      <c r="O1" s="51" t="s">
         <v>109</v>
       </c>
-      <c r="P1" s="53" t="s">
+      <c r="P1" s="51" t="s">
         <v>114</v>
       </c>
-      <c r="Q1" s="68" t="s">
+      <c r="Q1" s="53" t="s">
         <v>85</v>
       </c>
-      <c r="R1" s="72" t="s">
+      <c r="R1" s="57" t="s">
         <v>86</v>
       </c>
-      <c r="S1" s="68" t="s">
+      <c r="S1" s="53" t="s">
         <v>87</v>
       </c>
-      <c r="T1" s="69" t="s">
+      <c r="T1" s="54" t="s">
         <v>88</v>
       </c>
-      <c r="U1" s="68" t="s">
+      <c r="U1" s="53" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="2" spans="1:21" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="58"/>
-      <c r="B2" s="56"/>
-      <c r="C2" s="67"/>
-      <c r="D2" s="58"/>
-      <c r="E2" s="56"/>
-      <c r="F2" s="52"/>
-      <c r="G2" s="60"/>
-      <c r="H2" s="52"/>
-      <c r="I2" s="52"/>
-      <c r="J2" s="64"/>
-      <c r="K2" s="62"/>
-      <c r="L2" s="60"/>
+    <row r="2" spans="1:21" ht="15.75" customHeight="1" thickBot="1">
+      <c r="A2" s="63"/>
+      <c r="B2" s="61"/>
+      <c r="C2" s="72"/>
+      <c r="D2" s="63"/>
+      <c r="E2" s="61"/>
+      <c r="F2" s="59"/>
+      <c r="G2" s="65"/>
+      <c r="H2" s="59"/>
+      <c r="I2" s="59"/>
+      <c r="J2" s="69"/>
+      <c r="K2" s="67"/>
+      <c r="L2" s="65"/>
       <c r="M2" s="33" t="s">
         <v>90</v>
       </c>
       <c r="N2" s="33" t="s">
         <v>91</v>
       </c>
-      <c r="O2" s="54"/>
-      <c r="P2" s="54"/>
-      <c r="Q2" s="71"/>
-      <c r="R2" s="72"/>
-      <c r="S2" s="71"/>
-      <c r="T2" s="70"/>
-      <c r="U2" s="68"/>
-    </row>
-    <row r="3" spans="1:21" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="O2" s="52"/>
+      <c r="P2" s="52"/>
+      <c r="Q2" s="56"/>
+      <c r="R2" s="57"/>
+      <c r="S2" s="56"/>
+      <c r="T2" s="55"/>
+      <c r="U2" s="53"/>
+    </row>
+    <row r="3" spans="1:21" ht="16" thickTop="1">
       <c r="A3" s="8" t="s">
         <v>15</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="E3" s="9"/>
       <c r="F3" s="11"/>
       <c r="G3" s="16" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="H3" s="11">
         <v>1</v>
@@ -1579,7 +1581,7 @@
         <v>19</v>
       </c>
       <c r="J3" s="24" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="K3" s="13" t="s">
         <v>19</v>
@@ -1597,30 +1599,30 @@
         <v>7</v>
       </c>
       <c r="R3" s="49" t="s">
+        <v>145</v>
+      </c>
+      <c r="S3" s="47" t="s">
+        <v>146</v>
+      </c>
+      <c r="T3" s="50" t="s">
+        <v>147</v>
+      </c>
+      <c r="U3" s="47" t="s">
         <v>148</v>
       </c>
-      <c r="S3" s="47" t="s">
-        <v>149</v>
-      </c>
-      <c r="T3" s="50" t="s">
-        <v>150</v>
-      </c>
-      <c r="U3" s="47" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="4" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:21" ht="15">
       <c r="A4" s="8" t="s">
         <v>15</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="E4" s="35"/>
       <c r="F4" s="36"/>
@@ -1634,7 +1636,7 @@
         <v>19</v>
       </c>
       <c r="J4" s="24" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="K4" s="13" t="s">
         <v>19</v>
@@ -1652,35 +1654,35 @@
         <v>7</v>
       </c>
       <c r="R4" s="49" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="S4" s="47" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="T4" s="50" t="s">
         <v>126</v>
       </c>
       <c r="U4" s="47" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="5" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" ht="15">
       <c r="A5" s="8" t="s">
         <v>15</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="E5" s="35"/>
       <c r="F5" s="36"/>
       <c r="G5" s="16" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="H5" s="11">
         <v>3</v>
@@ -1689,7 +1691,7 @@
         <v>20</v>
       </c>
       <c r="J5" s="24" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="K5" s="13" t="s">
         <v>19</v>
@@ -1707,35 +1709,35 @@
         <v>7</v>
       </c>
       <c r="R5" s="49" t="s">
+        <v>145</v>
+      </c>
+      <c r="S5" s="47" t="s">
+        <v>146</v>
+      </c>
+      <c r="T5" s="50" t="s">
+        <v>149</v>
+      </c>
+      <c r="U5" s="47" t="s">
         <v>148</v>
       </c>
-      <c r="S5" s="47" t="s">
-        <v>149</v>
-      </c>
-      <c r="T5" s="50" t="s">
-        <v>152</v>
-      </c>
-      <c r="U5" s="47" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="6" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:21" ht="15">
       <c r="A6" s="8" t="s">
         <v>15</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="E6" s="35"/>
       <c r="F6" s="36"/>
       <c r="G6" s="16" t="s">
-        <v>127</v>
+        <v>211</v>
       </c>
       <c r="H6" s="15">
         <v>4</v>
@@ -1744,7 +1746,7 @@
         <v>20</v>
       </c>
       <c r="J6" s="24" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="K6" s="13" t="s">
         <v>20</v>
@@ -1757,7 +1759,7 @@
         <v>40</v>
       </c>
       <c r="O6" s="36" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="P6" s="45" t="s">
         <v>20</v>
@@ -1766,35 +1768,35 @@
         <v>6</v>
       </c>
       <c r="R6" s="22" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="S6" s="21" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="T6" s="48" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="U6" s="21" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="7" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" ht="15">
       <c r="A7" s="8" t="s">
         <v>15</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="D7" s="31" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="E7" s="35"/>
       <c r="F7" s="36"/>
       <c r="G7" s="16" t="s">
-        <v>128</v>
+        <v>212</v>
       </c>
       <c r="H7" s="11">
         <v>5</v>
@@ -1803,7 +1805,7 @@
         <v>20</v>
       </c>
       <c r="J7" s="24" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="K7" s="6" t="s">
         <v>20</v>
@@ -1816,7 +1818,7 @@
         <v>29</v>
       </c>
       <c r="O7" s="36" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="P7" s="45" t="s">
         <v>20</v>
@@ -1825,35 +1827,35 @@
         <v>6</v>
       </c>
       <c r="R7" s="22" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="S7" s="21" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="T7" s="48" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="U7" s="21" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="8" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" ht="15">
       <c r="A8" s="8" t="s">
         <v>15</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="D8" s="31" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="E8" s="35"/>
       <c r="F8" s="36"/>
       <c r="G8" s="16" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="H8" s="15">
         <v>6</v>
@@ -1862,7 +1864,7 @@
         <v>20</v>
       </c>
       <c r="J8" s="24" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="K8" s="6" t="s">
         <v>19</v>
@@ -1880,35 +1882,35 @@
         <v>7</v>
       </c>
       <c r="R8" s="49" t="s">
+        <v>145</v>
+      </c>
+      <c r="S8" s="47" t="s">
+        <v>146</v>
+      </c>
+      <c r="T8" s="50" t="s">
+        <v>127</v>
+      </c>
+      <c r="U8" s="47" t="s">
         <v>148</v>
       </c>
-      <c r="S8" s="47" t="s">
-        <v>149</v>
-      </c>
-      <c r="T8" s="50" t="s">
-        <v>129</v>
-      </c>
-      <c r="U8" s="47" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="9" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:21" ht="15">
       <c r="A9" s="8" t="s">
         <v>15</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="D9" s="31" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="E9" s="35"/>
       <c r="F9" s="36"/>
       <c r="G9" s="16" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="H9" s="11">
         <v>7</v>
@@ -1917,7 +1919,7 @@
         <v>20</v>
       </c>
       <c r="J9" s="24" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="K9" s="6" t="s">
         <v>20</v>
@@ -1930,7 +1932,7 @@
         <v>44</v>
       </c>
       <c r="O9" s="36" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="P9" s="45" t="s">
         <v>19</v>
@@ -1939,35 +1941,35 @@
         <v>6</v>
       </c>
       <c r="R9" s="22" t="s">
+        <v>150</v>
+      </c>
+      <c r="S9" s="21" t="s">
+        <v>151</v>
+      </c>
+      <c r="T9" s="48" t="s">
         <v>153</v>
       </c>
-      <c r="S9" s="21" t="s">
-        <v>154</v>
-      </c>
-      <c r="T9" s="48" t="s">
-        <v>156</v>
-      </c>
       <c r="U9" s="21" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="10" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21" ht="15">
       <c r="A10" s="8" t="s">
         <v>15</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="D10" s="31" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="E10" s="35"/>
       <c r="F10" s="36"/>
       <c r="G10" s="16" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="H10" s="15">
         <v>8</v>
@@ -1976,7 +1978,7 @@
         <v>20</v>
       </c>
       <c r="J10" s="24" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="K10" s="6" t="s">
         <v>19</v>
@@ -1994,35 +1996,35 @@
         <v>7</v>
       </c>
       <c r="R10" s="49" t="s">
+        <v>145</v>
+      </c>
+      <c r="S10" s="47" t="s">
+        <v>146</v>
+      </c>
+      <c r="T10" s="50" t="s">
+        <v>154</v>
+      </c>
+      <c r="U10" s="47" t="s">
         <v>148</v>
       </c>
-      <c r="S10" s="47" t="s">
-        <v>149</v>
-      </c>
-      <c r="T10" s="50" t="s">
-        <v>157</v>
-      </c>
-      <c r="U10" s="47" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="11" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:21" ht="15.75" customHeight="1">
       <c r="A11" s="8" t="s">
         <v>15</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="C11" s="10" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="D11" s="31" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="E11" s="35"/>
       <c r="F11" s="36"/>
       <c r="G11" s="16" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="H11" s="11">
         <v>9</v>
@@ -2031,7 +2033,7 @@
         <v>19</v>
       </c>
       <c r="J11" s="24" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="K11" s="6" t="s">
         <v>20</v>
@@ -2044,7 +2046,7 @@
       </c>
       <c r="N11" s="7"/>
       <c r="O11" s="36" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="P11" s="45" t="s">
         <v>19</v>
@@ -2053,37 +2055,37 @@
         <v>6</v>
       </c>
       <c r="R11" s="22" t="s">
+        <v>155</v>
+      </c>
+      <c r="S11" s="21" t="s">
+        <v>156</v>
+      </c>
+      <c r="T11" s="48" t="s">
+        <v>157</v>
+      </c>
+      <c r="U11" s="21" t="s">
         <v>158</v>
       </c>
-      <c r="S11" s="21" t="s">
-        <v>159</v>
-      </c>
-      <c r="T11" s="48" t="s">
-        <v>160</v>
-      </c>
-      <c r="U11" s="21" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="12" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:21" ht="15">
       <c r="A12" s="8" t="s">
         <v>15</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="C12" s="10" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="D12" s="31" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="E12" s="35" t="s">
         <v>125</v>
       </c>
       <c r="F12" s="36"/>
       <c r="G12" s="17" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="H12" s="15">
         <v>10</v>
@@ -2092,7 +2094,7 @@
         <v>20</v>
       </c>
       <c r="J12" s="25" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="K12" s="6" t="s">
         <v>19</v>
@@ -2110,35 +2112,35 @@
         <v>7</v>
       </c>
       <c r="R12" s="49" t="s">
+        <v>145</v>
+      </c>
+      <c r="S12" s="47" t="s">
+        <v>146</v>
+      </c>
+      <c r="T12" s="50" t="s">
+        <v>130</v>
+      </c>
+      <c r="U12" s="47" t="s">
         <v>148</v>
       </c>
-      <c r="S12" s="47" t="s">
-        <v>149</v>
-      </c>
-      <c r="T12" s="50" t="s">
-        <v>132</v>
-      </c>
-      <c r="U12" s="47" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="13" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:21" ht="15">
       <c r="A13" s="8" t="s">
         <v>15</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="C13" s="10" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="D13" s="31" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="E13" s="35"/>
       <c r="F13" s="36"/>
       <c r="G13" s="18" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="H13" s="11">
         <v>11</v>
@@ -2147,7 +2149,7 @@
         <v>20</v>
       </c>
       <c r="J13" s="24" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="K13" s="6" t="s">
         <v>19</v>
@@ -2158,7 +2160,7 @@
       <c r="M13" s="7"/>
       <c r="N13" s="7"/>
       <c r="O13" s="36" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
       <c r="P13" s="45" t="s">
         <v>19</v>
@@ -2167,35 +2169,35 @@
         <v>7</v>
       </c>
       <c r="R13" s="49" t="s">
+        <v>145</v>
+      </c>
+      <c r="S13" s="47" t="s">
+        <v>146</v>
+      </c>
+      <c r="T13" s="50" t="s">
+        <v>131</v>
+      </c>
+      <c r="U13" s="47" t="s">
         <v>148</v>
       </c>
-      <c r="S13" s="47" t="s">
-        <v>149</v>
-      </c>
-      <c r="T13" s="50" t="s">
-        <v>133</v>
-      </c>
-      <c r="U13" s="47" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="14" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:21" ht="15">
       <c r="A14" s="8" t="s">
         <v>15</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="C14" s="10" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="D14" s="31" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="E14" s="35"/>
       <c r="F14" s="36"/>
       <c r="G14" s="18" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="H14" s="15">
         <v>12</v>
@@ -2204,7 +2206,7 @@
         <v>20</v>
       </c>
       <c r="J14" s="24" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="K14" s="6" t="s">
         <v>20</v>
@@ -2217,7 +2219,7 @@
         <v>45</v>
       </c>
       <c r="O14" s="36" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
       <c r="P14" s="45" t="s">
         <v>19</v>
@@ -2226,35 +2228,35 @@
         <v>6</v>
       </c>
       <c r="R14" s="22" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="S14" s="21" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="T14" s="48" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="U14" s="21" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="15" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21" ht="15">
       <c r="A15" s="8" t="s">
         <v>15</v>
       </c>
       <c r="B15" s="9" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="C15" s="10" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="D15" s="31" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="E15" s="35"/>
       <c r="F15" s="36"/>
       <c r="G15" s="18" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="H15" s="11">
         <v>13</v>
@@ -2263,7 +2265,7 @@
         <v>19</v>
       </c>
       <c r="J15" s="26" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="K15" s="6" t="s">
         <v>20</v>
@@ -2276,7 +2278,7 @@
       </c>
       <c r="N15" s="7"/>
       <c r="O15" s="36" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="P15" s="45" t="s">
         <v>19</v>
@@ -2285,37 +2287,37 @@
         <v>6</v>
       </c>
       <c r="R15" s="22" t="s">
+        <v>155</v>
+      </c>
+      <c r="S15" s="21" t="s">
+        <v>156</v>
+      </c>
+      <c r="T15" s="48" t="s">
+        <v>159</v>
+      </c>
+      <c r="U15" s="21" t="s">
         <v>158</v>
       </c>
-      <c r="S15" s="21" t="s">
-        <v>159</v>
-      </c>
-      <c r="T15" s="48" t="s">
-        <v>162</v>
-      </c>
-      <c r="U15" s="21" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="16" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:21" ht="15">
       <c r="A16" s="8" t="s">
         <v>15</v>
       </c>
       <c r="B16" s="9" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="C16" s="10" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="D16" s="31" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="E16" s="35" t="s">
         <v>125</v>
       </c>
       <c r="F16" s="36"/>
       <c r="G16" s="17" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="H16" s="15">
         <v>14</v>
@@ -2324,7 +2326,7 @@
         <v>20</v>
       </c>
       <c r="J16" s="27" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="K16" s="6" t="s">
         <v>19</v>
@@ -2342,35 +2344,35 @@
         <v>7</v>
       </c>
       <c r="R16" s="49" t="s">
+        <v>145</v>
+      </c>
+      <c r="S16" s="47" t="s">
+        <v>146</v>
+      </c>
+      <c r="T16" s="50" t="s">
+        <v>134</v>
+      </c>
+      <c r="U16" s="47" t="s">
         <v>148</v>
       </c>
-      <c r="S16" s="47" t="s">
-        <v>149</v>
-      </c>
-      <c r="T16" s="50" t="s">
-        <v>136</v>
-      </c>
-      <c r="U16" s="47" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="17" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:21" ht="15">
       <c r="A17" s="8" t="s">
         <v>15</v>
       </c>
       <c r="B17" s="9" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="C17" s="10" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="D17" s="32" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="E17" s="35"/>
       <c r="F17" s="36"/>
       <c r="G17" s="18" t="s">
-        <v>137</v>
+        <v>214</v>
       </c>
       <c r="H17" s="11">
         <v>15</v>
@@ -2379,7 +2381,7 @@
         <v>20</v>
       </c>
       <c r="J17" s="24" t="s">
-        <v>184</v>
+        <v>213</v>
       </c>
       <c r="K17" s="6" t="s">
         <v>20</v>
@@ -2392,7 +2394,7 @@
         <v>27</v>
       </c>
       <c r="O17" s="36" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
       <c r="P17" s="45" t="s">
         <v>19</v>
@@ -2401,35 +2403,35 @@
         <v>6</v>
       </c>
       <c r="R17" s="22" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="S17" s="21" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="T17" s="48" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="U17" s="21" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="18" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="18" spans="1:21" ht="15">
       <c r="A18" s="8" t="s">
         <v>15</v>
       </c>
       <c r="B18" s="9" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="C18" s="10" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="D18" s="32" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="E18" s="35"/>
       <c r="F18" s="36"/>
       <c r="G18" s="18" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="H18" s="15">
         <v>16</v>
@@ -2438,7 +2440,7 @@
         <v>20</v>
       </c>
       <c r="J18" s="24" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="K18" s="6" t="s">
         <v>20</v>
@@ -2451,7 +2453,7 @@
         <v>37</v>
       </c>
       <c r="O18" s="36" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="P18" s="45" t="s">
         <v>19</v>
@@ -2460,35 +2462,35 @@
         <v>6</v>
       </c>
       <c r="R18" s="22" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="S18" s="21" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="T18" s="48" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="U18" s="21" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="19" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="19" spans="1:21" ht="15">
       <c r="A19" s="8" t="s">
         <v>15</v>
       </c>
       <c r="B19" s="9" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="C19" s="10" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="D19" s="32" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="E19" s="35"/>
       <c r="F19" s="36"/>
       <c r="G19" s="18" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="H19" s="11">
         <v>17</v>
@@ -2497,7 +2499,7 @@
         <v>20</v>
       </c>
       <c r="J19" s="24" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="K19" s="6" t="s">
         <v>20</v>
@@ -2510,7 +2512,7 @@
         <v>40</v>
       </c>
       <c r="O19" s="36" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="P19" s="45" t="s">
         <v>19</v>
@@ -2519,37 +2521,37 @@
         <v>6</v>
       </c>
       <c r="R19" s="22" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="S19" s="21" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="T19" s="48" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="U19" s="21" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="20" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="20" spans="1:21" ht="15">
       <c r="A20" s="8" t="s">
         <v>15</v>
       </c>
       <c r="B20" s="9" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="C20" s="10" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="D20" s="32" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="E20" s="35" t="s">
         <v>125</v>
       </c>
       <c r="F20" s="36"/>
       <c r="G20" s="17" t="s">
-        <v>190</v>
+        <v>162</v>
       </c>
       <c r="H20" s="15">
         <v>18</v>
@@ -2558,7 +2560,7 @@
         <v>20</v>
       </c>
       <c r="J20" s="24" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="K20" s="6" t="s">
         <v>19</v>
@@ -2576,35 +2578,35 @@
         <v>7</v>
       </c>
       <c r="R20" s="49" t="s">
+        <v>145</v>
+      </c>
+      <c r="S20" s="47" t="s">
+        <v>146</v>
+      </c>
+      <c r="T20" s="50" t="s">
+        <v>162</v>
+      </c>
+      <c r="U20" s="47" t="s">
         <v>148</v>
       </c>
-      <c r="S20" s="47" t="s">
-        <v>149</v>
-      </c>
-      <c r="T20" s="50" t="s">
-        <v>165</v>
-      </c>
-      <c r="U20" s="47" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="21" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="1:21" ht="15">
       <c r="A21" s="8" t="s">
         <v>15</v>
       </c>
       <c r="B21" s="9" t="s">
+        <v>200</v>
+      </c>
+      <c r="C21" s="10" t="s">
+        <v>201</v>
+      </c>
+      <c r="D21" s="32" t="s">
         <v>205</v>
-      </c>
-      <c r="C21" s="10" t="s">
-        <v>206</v>
-      </c>
-      <c r="D21" s="32" t="s">
-        <v>210</v>
       </c>
       <c r="E21" s="35"/>
       <c r="F21" s="36"/>
       <c r="G21" s="17" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="H21" s="11">
         <v>19</v>
@@ -2613,7 +2615,7 @@
         <v>19</v>
       </c>
       <c r="J21" s="24" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="K21" s="6" t="s">
         <v>19</v>
@@ -2631,35 +2633,35 @@
         <v>7</v>
       </c>
       <c r="R21" s="49" t="s">
+        <v>145</v>
+      </c>
+      <c r="S21" s="47" t="s">
+        <v>146</v>
+      </c>
+      <c r="T21" s="50" t="s">
+        <v>163</v>
+      </c>
+      <c r="U21" s="47" t="s">
         <v>148</v>
       </c>
-      <c r="S21" s="47" t="s">
-        <v>149</v>
-      </c>
-      <c r="T21" s="50" t="s">
-        <v>166</v>
-      </c>
-      <c r="U21" s="47" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="22" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="1:21" ht="15">
       <c r="A22" s="8" t="s">
         <v>15</v>
       </c>
       <c r="B22" s="9" t="s">
+        <v>200</v>
+      </c>
+      <c r="C22" s="10" t="s">
+        <v>201</v>
+      </c>
+      <c r="D22" s="32" t="s">
         <v>205</v>
-      </c>
-      <c r="C22" s="10" t="s">
-        <v>206</v>
-      </c>
-      <c r="D22" s="32" t="s">
-        <v>210</v>
       </c>
       <c r="E22" s="35"/>
       <c r="F22" s="36"/>
       <c r="G22" s="17" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="H22" s="15">
         <v>20</v>
@@ -2668,7 +2670,7 @@
         <v>20</v>
       </c>
       <c r="J22" s="24" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="K22" s="6" t="s">
         <v>19</v>
@@ -2686,37 +2688,37 @@
         <v>7</v>
       </c>
       <c r="R22" s="49" t="s">
+        <v>145</v>
+      </c>
+      <c r="S22" s="47" t="s">
+        <v>146</v>
+      </c>
+      <c r="T22" s="50" t="s">
+        <v>164</v>
+      </c>
+      <c r="U22" s="47" t="s">
         <v>148</v>
       </c>
-      <c r="S22" s="47" t="s">
-        <v>149</v>
-      </c>
-      <c r="T22" s="50" t="s">
-        <v>167</v>
-      </c>
-      <c r="U22" s="47" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="23" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="23" spans="1:21" ht="15">
       <c r="A23" s="8" t="s">
         <v>15</v>
       </c>
       <c r="B23" s="9" t="s">
+        <v>200</v>
+      </c>
+      <c r="C23" s="10" t="s">
+        <v>201</v>
+      </c>
+      <c r="D23" s="32" t="s">
         <v>205</v>
-      </c>
-      <c r="C23" s="10" t="s">
-        <v>206</v>
-      </c>
-      <c r="D23" s="32" t="s">
-        <v>210</v>
       </c>
       <c r="E23" s="35" t="s">
         <v>125</v>
       </c>
       <c r="F23" s="36"/>
       <c r="G23" s="17" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="H23" s="15">
         <v>21</v>
@@ -2725,7 +2727,7 @@
         <v>20</v>
       </c>
       <c r="J23" s="24" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="K23" s="6" t="s">
         <v>19</v>
@@ -2743,27 +2745,27 @@
         <v>7</v>
       </c>
       <c r="R23" s="49" t="s">
+        <v>145</v>
+      </c>
+      <c r="S23" s="47" t="s">
+        <v>146</v>
+      </c>
+      <c r="T23" s="50" t="s">
+        <v>139</v>
+      </c>
+      <c r="U23" s="47" t="s">
         <v>148</v>
       </c>
-      <c r="S23" s="47" t="s">
-        <v>149</v>
-      </c>
-      <c r="T23" s="50" t="s">
-        <v>142</v>
-      </c>
-      <c r="U23" s="47" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="24" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="24" spans="1:21" ht="15">
       <c r="A24" s="8" t="s">
         <v>15</v>
       </c>
       <c r="B24" s="9" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="C24" s="10" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="D24" s="32" t="s">
         <v>123</v>
@@ -2771,7 +2773,7 @@
       <c r="E24" s="35"/>
       <c r="F24" s="36"/>
       <c r="G24" s="17" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="H24" s="11">
         <v>22</v>
@@ -2780,7 +2782,7 @@
         <v>20</v>
       </c>
       <c r="J24" s="24" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="K24" s="6" t="s">
         <v>19</v>
@@ -2798,27 +2800,27 @@
         <v>7</v>
       </c>
       <c r="R24" s="49" t="s">
+        <v>145</v>
+      </c>
+      <c r="S24" s="47" t="s">
+        <v>146</v>
+      </c>
+      <c r="T24" s="50" t="s">
+        <v>140</v>
+      </c>
+      <c r="U24" s="47" t="s">
         <v>148</v>
       </c>
-      <c r="S24" s="47" t="s">
-        <v>149</v>
-      </c>
-      <c r="T24" s="50" t="s">
-        <v>143</v>
-      </c>
-      <c r="U24" s="47" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="25" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="25" spans="1:21" ht="15">
       <c r="A25" s="8" t="s">
         <v>15</v>
       </c>
       <c r="B25" s="9" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="C25" s="10" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="D25" s="32" t="s">
         <v>123</v>
@@ -2826,7 +2828,7 @@
       <c r="E25" s="35"/>
       <c r="F25" s="36"/>
       <c r="G25" s="17" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="H25" s="15">
         <v>23</v>
@@ -2835,7 +2837,7 @@
         <v>20</v>
       </c>
       <c r="J25" s="24" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="K25" s="6" t="s">
         <v>20</v>
@@ -2848,7 +2850,7 @@
         <v>120</v>
       </c>
       <c r="O25" s="36" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="P25" s="45" t="s">
         <v>20</v>
@@ -2857,27 +2859,27 @@
         <v>6</v>
       </c>
       <c r="R25" s="22" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="S25" s="21" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="T25" s="48" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="U25" s="21" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="26" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="26" spans="1:21" ht="15">
       <c r="A26" s="8" t="s">
         <v>15</v>
       </c>
       <c r="B26" s="9" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="C26" s="10" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="D26" s="32" t="s">
         <v>124</v>
@@ -2894,7 +2896,7 @@
         <v>20</v>
       </c>
       <c r="J26" s="24" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="K26" s="6" t="s">
         <v>20</v>
@@ -2914,15 +2916,15 @@
       <c r="T26" s="48"/>
       <c r="U26" s="21"/>
     </row>
-    <row r="27" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:21" ht="15">
       <c r="A27" s="8" t="s">
         <v>15</v>
       </c>
       <c r="B27" s="9" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="C27" s="10" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="D27" s="32" t="s">
         <v>124</v>
@@ -2939,7 +2941,7 @@
         <v>20</v>
       </c>
       <c r="J27" s="24" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="K27" s="6" t="s">
         <v>20</v>
@@ -2957,30 +2959,30 @@
         <v>6</v>
       </c>
       <c r="R27" s="46" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="S27" s="21" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="T27" s="23" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="U27" s="21" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="28" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="28" spans="1:21" ht="15">
       <c r="A28" s="8" t="s">
         <v>15</v>
       </c>
       <c r="B28" s="9" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="C28" s="10" t="s">
+        <v>201</v>
+      </c>
+      <c r="D28" s="32" t="s">
         <v>206</v>
-      </c>
-      <c r="D28" s="32" t="s">
-        <v>211</v>
       </c>
       <c r="E28" s="35"/>
       <c r="F28" s="36"/>
@@ -3010,19 +3012,19 @@
         <v>6</v>
       </c>
       <c r="R28" s="46" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="S28" s="21" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="T28" s="23" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="U28" s="21" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="29" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="29" spans="1:21" ht="15">
       <c r="A29" s="8"/>
       <c r="B29" s="9"/>
       <c r="C29" s="37"/>
@@ -3045,7 +3047,7 @@
       <c r="T29" s="40"/>
       <c r="U29" s="38"/>
     </row>
-    <row r="30" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:21" ht="15">
       <c r="A30" s="3"/>
       <c r="B30" s="41"/>
       <c r="C30" s="37"/>
@@ -3068,7 +3070,7 @@
       <c r="T30" s="40"/>
       <c r="U30" s="38"/>
     </row>
-    <row r="31" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:21" ht="15">
       <c r="A31" s="3"/>
       <c r="B31" s="41"/>
       <c r="C31" s="37"/>
@@ -3091,7 +3093,7 @@
       <c r="T31" s="40"/>
       <c r="U31" s="38"/>
     </row>
-    <row r="32" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:21" ht="15">
       <c r="A32" s="3"/>
       <c r="B32" s="41"/>
       <c r="C32" s="37"/>
@@ -3114,7 +3116,7 @@
       <c r="T32" s="40"/>
       <c r="U32" s="38"/>
     </row>
-    <row r="33" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:21" ht="15">
       <c r="A33" s="3"/>
       <c r="B33" s="41"/>
       <c r="C33" s="37"/>
@@ -3137,7 +3139,7 @@
       <c r="T33" s="40"/>
       <c r="U33" s="38"/>
     </row>
-    <row r="34" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:21" ht="15">
       <c r="A34" s="3"/>
       <c r="B34" s="41"/>
       <c r="C34" s="37"/>
@@ -3160,7 +3162,7 @@
       <c r="T34" s="40"/>
       <c r="U34" s="38"/>
     </row>
-    <row r="35" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:21" ht="15">
       <c r="A35" s="3"/>
       <c r="B35" s="41"/>
       <c r="C35" s="37"/>
@@ -3183,7 +3185,7 @@
       <c r="T35" s="40"/>
       <c r="U35" s="38"/>
     </row>
-    <row r="36" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:21" ht="15">
       <c r="A36" s="3"/>
       <c r="B36" s="41"/>
       <c r="C36" s="37"/>
@@ -3206,7 +3208,7 @@
       <c r="T36" s="40"/>
       <c r="U36" s="38"/>
     </row>
-    <row r="37" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:21" ht="15">
       <c r="A37" s="3"/>
       <c r="B37" s="41"/>
       <c r="C37" s="37"/>
@@ -3229,7 +3231,7 @@
       <c r="T37" s="40"/>
       <c r="U37" s="38"/>
     </row>
-    <row r="38" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:21" ht="15">
       <c r="A38" s="3"/>
       <c r="B38" s="41"/>
       <c r="C38" s="37"/>
@@ -3252,7 +3254,7 @@
       <c r="T38" s="40"/>
       <c r="U38" s="38"/>
     </row>
-    <row r="39" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:21" ht="15">
       <c r="A39" s="3"/>
       <c r="B39" s="41"/>
       <c r="C39" s="37"/>
@@ -3275,7 +3277,7 @@
       <c r="T39" s="40"/>
       <c r="U39" s="38"/>
     </row>
-    <row r="40" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:21" ht="15">
       <c r="A40" s="3"/>
       <c r="B40" s="41"/>
       <c r="C40" s="37"/>
@@ -3298,7 +3300,7 @@
       <c r="T40" s="40"/>
       <c r="U40" s="38"/>
     </row>
-    <row r="41" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:21" ht="15">
       <c r="A41" s="3"/>
       <c r="B41" s="41"/>
       <c r="C41" s="37"/>
@@ -3321,7 +3323,7 @@
       <c r="T41" s="40"/>
       <c r="U41" s="38"/>
     </row>
-    <row r="42" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:21" ht="15">
       <c r="A42" s="3"/>
       <c r="B42" s="41"/>
       <c r="C42" s="37"/>
@@ -3344,7 +3346,7 @@
       <c r="T42" s="40"/>
       <c r="U42" s="38"/>
     </row>
-    <row r="43" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:21" ht="15">
       <c r="A43" s="3"/>
       <c r="B43" s="41"/>
       <c r="C43" s="37"/>
@@ -3367,7 +3369,7 @@
       <c r="T43" s="40"/>
       <c r="U43" s="38"/>
     </row>
-    <row r="44" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:21" ht="15">
       <c r="A44" s="3"/>
       <c r="B44" s="41"/>
       <c r="C44" s="37"/>
@@ -3390,7 +3392,7 @@
       <c r="T44" s="40"/>
       <c r="U44" s="38"/>
     </row>
-    <row r="45" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:21" ht="15">
       <c r="A45" s="3"/>
       <c r="B45" s="41"/>
       <c r="C45" s="37"/>
@@ -3413,7 +3415,7 @@
       <c r="T45" s="40"/>
       <c r="U45" s="38"/>
     </row>
-    <row r="46" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:21" ht="15">
       <c r="A46" s="3"/>
       <c r="B46" s="41"/>
       <c r="C46" s="37"/>
@@ -3436,7 +3438,7 @@
       <c r="T46" s="40"/>
       <c r="U46" s="38"/>
     </row>
-    <row r="47" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:21" ht="15">
       <c r="A47" s="3"/>
       <c r="B47" s="41"/>
       <c r="C47" s="37"/>
@@ -3459,7 +3461,7 @@
       <c r="T47" s="40"/>
       <c r="U47" s="38"/>
     </row>
-    <row r="48" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:21" ht="15">
       <c r="A48" s="3"/>
       <c r="B48" s="41"/>
       <c r="C48" s="37"/>
@@ -3482,7 +3484,7 @@
       <c r="T48" s="40"/>
       <c r="U48" s="38"/>
     </row>
-    <row r="49" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:21" ht="15">
       <c r="A49" s="3"/>
       <c r="B49" s="41"/>
       <c r="C49" s="37"/>
@@ -3505,7 +3507,7 @@
       <c r="T49" s="40"/>
       <c r="U49" s="38"/>
     </row>
-    <row r="50" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:21" ht="15">
       <c r="A50" s="3"/>
       <c r="B50" s="41"/>
       <c r="C50" s="37"/>
@@ -3528,7 +3530,7 @@
       <c r="T50" s="40"/>
       <c r="U50" s="38"/>
     </row>
-    <row r="51" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:21" ht="15">
       <c r="A51" s="3"/>
       <c r="B51" s="41"/>
       <c r="C51" s="37"/>
@@ -3551,7 +3553,7 @@
       <c r="T51" s="40"/>
       <c r="U51" s="38"/>
     </row>
-    <row r="52" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:21" ht="15">
       <c r="A52" s="3"/>
       <c r="B52" s="41"/>
       <c r="C52" s="37"/>
@@ -3574,7 +3576,7 @@
       <c r="T52" s="40"/>
       <c r="U52" s="38"/>
     </row>
-    <row r="53" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:21" ht="15">
       <c r="A53" s="3"/>
       <c r="B53" s="41"/>
       <c r="C53" s="37"/>
@@ -3597,7 +3599,7 @@
       <c r="T53" s="40"/>
       <c r="U53" s="38"/>
     </row>
-    <row r="54" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:21" ht="15">
       <c r="A54" s="3"/>
       <c r="B54" s="41"/>
       <c r="C54" s="37"/>
@@ -3620,7 +3622,7 @@
       <c r="T54" s="40"/>
       <c r="U54" s="38"/>
     </row>
-    <row r="55" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:21" ht="15">
       <c r="A55" s="3"/>
       <c r="B55" s="41"/>
       <c r="C55" s="37"/>
@@ -3643,7 +3645,7 @@
       <c r="T55" s="40"/>
       <c r="U55" s="38"/>
     </row>
-    <row r="56" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:21" ht="15">
       <c r="A56" s="3"/>
       <c r="B56" s="41"/>
       <c r="C56" s="37"/>
@@ -3666,7 +3668,7 @@
       <c r="T56" s="40"/>
       <c r="U56" s="38"/>
     </row>
-    <row r="57" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:21" ht="15">
       <c r="A57" s="3"/>
       <c r="B57" s="41"/>
       <c r="C57" s="37"/>
@@ -3689,7 +3691,7 @@
       <c r="T57" s="40"/>
       <c r="U57" s="38"/>
     </row>
-    <row r="58" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:21" ht="15">
       <c r="A58" s="3"/>
       <c r="B58" s="41"/>
       <c r="C58" s="37"/>
@@ -3712,7 +3714,7 @@
       <c r="T58" s="40"/>
       <c r="U58" s="38"/>
     </row>
-    <row r="59" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:21" ht="15">
       <c r="A59" s="3"/>
       <c r="B59" s="41"/>
       <c r="C59" s="37"/>
@@ -3735,7 +3737,7 @@
       <c r="T59" s="40"/>
       <c r="U59" s="38"/>
     </row>
-    <row r="60" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:21" ht="15">
       <c r="A60" s="3"/>
       <c r="B60" s="41"/>
       <c r="C60" s="37"/>
@@ -3758,7 +3760,7 @@
       <c r="T60" s="40"/>
       <c r="U60" s="38"/>
     </row>
-    <row r="61" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:21" ht="15">
       <c r="A61" s="3"/>
       <c r="B61" s="41"/>
       <c r="C61" s="37"/>
@@ -3781,7 +3783,7 @@
       <c r="T61" s="40"/>
       <c r="U61" s="38"/>
     </row>
-    <row r="62" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:21" ht="15">
       <c r="A62" s="3"/>
       <c r="B62" s="41"/>
       <c r="C62" s="37"/>
@@ -3804,7 +3806,7 @@
       <c r="T62" s="40"/>
       <c r="U62" s="38"/>
     </row>
-    <row r="63" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:21" ht="15">
       <c r="A63" s="3"/>
       <c r="B63" s="41"/>
       <c r="C63" s="37"/>
@@ -3827,7 +3829,7 @@
       <c r="T63" s="40"/>
       <c r="U63" s="38"/>
     </row>
-    <row r="64" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:21" ht="15">
       <c r="A64" s="3"/>
       <c r="B64" s="41"/>
       <c r="C64" s="37"/>
@@ -3850,7 +3852,7 @@
       <c r="T64" s="40"/>
       <c r="U64" s="38"/>
     </row>
-    <row r="65" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:21" ht="15">
       <c r="A65" s="3"/>
       <c r="B65" s="41"/>
       <c r="C65" s="37"/>
@@ -3873,7 +3875,7 @@
       <c r="T65" s="40"/>
       <c r="U65" s="38"/>
     </row>
-    <row r="66" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:21" ht="15">
       <c r="A66" s="3"/>
       <c r="B66" s="41"/>
       <c r="C66" s="37"/>
@@ -3896,7 +3898,7 @@
       <c r="T66" s="40"/>
       <c r="U66" s="38"/>
     </row>
-    <row r="67" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:21" ht="15">
       <c r="A67" s="3"/>
       <c r="B67" s="41"/>
       <c r="C67" s="37"/>
@@ -3914,7 +3916,7 @@
       <c r="O67" s="36"/>
       <c r="P67" s="36"/>
     </row>
-    <row r="68" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:21" ht="15">
       <c r="A68" s="3"/>
       <c r="B68" s="41"/>
       <c r="C68" s="37"/>
@@ -3932,7 +3934,7 @@
       <c r="O68" s="36"/>
       <c r="P68" s="36"/>
     </row>
-    <row r="69" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:21" ht="15">
       <c r="A69" s="3"/>
       <c r="B69" s="41"/>
       <c r="C69" s="37"/>
@@ -3950,7 +3952,7 @@
       <c r="O69" s="36"/>
       <c r="P69" s="36"/>
     </row>
-    <row r="70" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:21" ht="15">
       <c r="A70" s="3"/>
       <c r="B70" s="41"/>
       <c r="C70" s="37"/>
@@ -3968,199 +3970,193 @@
       <c r="O70" s="36"/>
       <c r="P70" s="36"/>
     </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:1">
       <c r="A85" s="20" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:1">
       <c r="A86" s="20" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:1">
       <c r="A87" s="20" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:1">
       <c r="A88" s="20" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:1">
       <c r="A89" s="20" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:1">
       <c r="A90" s="20" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="91" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:1">
       <c r="A91" s="20" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="92" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:1">
       <c r="A92" s="20" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="93" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:1">
       <c r="A93" s="20" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="94" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:1">
       <c r="A94" s="20" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="95" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:1">
       <c r="A95" s="20" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="96" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:1">
       <c r="A96" s="20" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:1">
       <c r="A97" s="20" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:1">
       <c r="A98" s="20" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:1">
       <c r="A99" s="20" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="100" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:1">
       <c r="A100" s="20" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="101" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:1">
       <c r="A101" s="20" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="102" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:1">
       <c r="A102" s="20" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="103" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:1">
       <c r="A103" s="20" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="104" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:1">
       <c r="A104" s="20" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="105" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:1">
       <c r="A105" s="20" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="106" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:1">
       <c r="A106" s="20" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="107" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:1">
       <c r="A107" s="20" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="108" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:1">
       <c r="A108" s="20" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="109" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:1">
       <c r="A109" s="20" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="110" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:1">
       <c r="A110" s="20" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="111" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:1">
       <c r="A111" s="20" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="112" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:1">
       <c r="A112" s="20" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="113" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:1">
       <c r="A113" s="20" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="114" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:1">
       <c r="A114" s="20" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="115" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:1">
       <c r="A115" s="20" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="116" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:1">
       <c r="A116" s="20" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="117" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:1">
       <c r="A117" s="20" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="118" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:1">
       <c r="A118" s="20" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="119" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:1">
       <c r="A119" s="20" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="120" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:1">
       <c r="A120" s="20" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="121" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:1">
       <c r="A121" s="20" t="s">
         <v>115</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="P1:P2"/>
-    <mergeCell ref="U1:U2"/>
-    <mergeCell ref="T1:T2"/>
-    <mergeCell ref="S1:S2"/>
-    <mergeCell ref="R1:R2"/>
-    <mergeCell ref="Q1:Q2"/>
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="H1:H2"/>
     <mergeCell ref="O1:O2"/>
@@ -4175,9 +4171,14 @@
     <mergeCell ref="D1:D2"/>
     <mergeCell ref="C1:C2"/>
     <mergeCell ref="F1:F2"/>
+    <mergeCell ref="P1:P2"/>
+    <mergeCell ref="U1:U2"/>
+    <mergeCell ref="T1:T2"/>
+    <mergeCell ref="S1:S2"/>
+    <mergeCell ref="R1:R2"/>
+    <mergeCell ref="Q1:Q2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="5">
@@ -4213,6 +4214,9 @@
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
   </extLst>
 </worksheet>
 </file>
@@ -4221,31 +4225,31 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O133"/>
   <sheetViews>
-    <sheetView topLeftCell="C20" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="C20" workbookViewId="0">
       <selection activeCell="E47" sqref="E47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="21.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.85546875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="21.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.83203125" style="1" customWidth="1"/>
     <col min="4" max="4" width="34" style="1" customWidth="1"/>
-    <col min="5" max="5" width="34.85546875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="24.5703125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="34.83203125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="24.5" style="1" customWidth="1"/>
     <col min="7" max="7" width="18" style="1" customWidth="1"/>
-    <col min="8" max="8" width="12.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="21.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.7109375" style="1" customWidth="1"/>
-    <col min="11" max="11" width="15.5703125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="12.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="21.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.6640625" style="1" customWidth="1"/>
+    <col min="11" max="11" width="15.5" style="1" customWidth="1"/>
     <col min="12" max="12" width="17" style="1" customWidth="1"/>
-    <col min="13" max="13" width="11.42578125" style="1"/>
-    <col min="14" max="14" width="24.28515625" style="1" customWidth="1"/>
-    <col min="15" max="15" width="69.85546875" style="1" hidden="1" customWidth="1"/>
-    <col min="16" max="16384" width="11.42578125" style="1"/>
+    <col min="13" max="13" width="11.5" style="1"/>
+    <col min="14" max="14" width="24.33203125" style="1" customWidth="1"/>
+    <col min="15" max="15" width="69.83203125" style="1" hidden="1" customWidth="1"/>
+    <col min="16" max="16384" width="11.5" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" s="2" customFormat="1" ht="15">
       <c r="A1" s="1" t="s">
         <v>15</v>
       </c>
@@ -4262,7 +4266,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" ht="15">
       <c r="A2" s="1" t="s">
         <v>16</v>
       </c>
@@ -4286,7 +4290,7 @@
       <c r="K2" s="2"/>
       <c r="L2" s="2"/>
     </row>
-    <row r="3" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" ht="15">
       <c r="A3" s="1" t="s">
         <v>17</v>
       </c>
@@ -4305,7 +4309,7 @@
       <c r="K3" s="2"/>
       <c r="L3" s="2"/>
     </row>
-    <row r="4" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" ht="15">
       <c r="A4" s="1" t="s">
         <v>18</v>
       </c>
@@ -4324,7 +4328,7 @@
       <c r="K4" s="2"/>
       <c r="L4" s="2"/>
     </row>
-    <row r="5" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" ht="15">
       <c r="B5" s="1" t="s">
         <v>9</v>
       </c>
@@ -4340,7 +4344,7 @@
       <c r="K5" s="2"/>
       <c r="L5" s="2"/>
     </row>
-    <row r="6" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" ht="15">
       <c r="B6" s="1" t="s">
         <v>10</v>
       </c>
@@ -4357,7 +4361,7 @@
       <c r="K6" s="2"/>
       <c r="L6" s="2"/>
     </row>
-    <row r="7" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" ht="15">
       <c r="B7" s="1" t="s">
         <v>11</v>
       </c>
@@ -4374,7 +4378,7 @@
       <c r="K7" s="2"/>
       <c r="L7" s="2"/>
     </row>
-    <row r="8" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" ht="15">
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
@@ -4389,7 +4393,7 @@
       <c r="K8" s="2"/>
       <c r="L8" s="2"/>
     </row>
-    <row r="9" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" ht="15">
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
@@ -4404,7 +4408,7 @@
       <c r="K9" s="2"/>
       <c r="L9" s="2"/>
     </row>
-    <row r="10" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" ht="15">
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
@@ -4419,7 +4423,7 @@
       <c r="K10" s="2"/>
       <c r="L10" s="2"/>
     </row>
-    <row r="11" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" ht="15">
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
@@ -4434,7 +4438,7 @@
       <c r="K11" s="2"/>
       <c r="L11" s="2"/>
     </row>
-    <row r="12" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" ht="15">
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
@@ -4449,7 +4453,7 @@
       <c r="K12" s="2"/>
       <c r="L12" s="2"/>
     </row>
-    <row r="13" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" ht="15">
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
@@ -4464,7 +4468,7 @@
       <c r="K13" s="2"/>
       <c r="L13" s="2"/>
     </row>
-    <row r="14" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" ht="15">
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
@@ -4479,7 +4483,7 @@
       <c r="K14" s="2"/>
       <c r="L14" s="2"/>
     </row>
-    <row r="15" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" ht="15">
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
@@ -4494,7 +4498,7 @@
       <c r="K15" s="2"/>
       <c r="L15" s="2"/>
     </row>
-    <row r="16" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" ht="15">
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
@@ -4509,7 +4513,7 @@
       <c r="K16" s="2"/>
       <c r="L16" s="2"/>
     </row>
-    <row r="17" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:12" ht="15">
       <c r="B17" s="2"/>
       <c r="D17" s="2"/>
       <c r="E17" s="1" t="s">
@@ -4523,7 +4527,7 @@
       <c r="K17" s="2"/>
       <c r="L17" s="2"/>
     </row>
-    <row r="18" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:12" ht="15">
       <c r="B18" s="2"/>
       <c r="D18" s="2"/>
       <c r="E18" s="1" t="s">
@@ -4537,7 +4541,7 @@
       <c r="K18" s="2"/>
       <c r="L18" s="2"/>
     </row>
-    <row r="19" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:12" ht="15">
       <c r="B19" s="2"/>
       <c r="D19" s="2"/>
       <c r="E19" s="1" t="s">
@@ -4551,7 +4555,7 @@
       <c r="K19" s="2"/>
       <c r="L19" s="2"/>
     </row>
-    <row r="20" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:12" ht="15">
       <c r="B20" s="2"/>
       <c r="D20" s="2"/>
       <c r="E20" s="1" t="s">
@@ -4565,7 +4569,7 @@
       <c r="K20" s="2"/>
       <c r="L20" s="2"/>
     </row>
-    <row r="21" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:12" ht="15">
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
@@ -4580,7 +4584,7 @@
       <c r="K21" s="2"/>
       <c r="L21" s="2"/>
     </row>
-    <row r="22" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:12" ht="15">
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
       <c r="D22" s="2"/>
@@ -4595,7 +4599,7 @@
       <c r="K22" s="2"/>
       <c r="L22" s="2"/>
     </row>
-    <row r="23" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:12" ht="15">
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
       <c r="D23" s="2"/>
@@ -4610,7 +4614,7 @@
       <c r="K23" s="2"/>
       <c r="L23" s="2"/>
     </row>
-    <row r="24" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:12" ht="15">
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
       <c r="D24" s="2"/>
@@ -4625,7 +4629,7 @@
       <c r="K24" s="2"/>
       <c r="L24" s="2"/>
     </row>
-    <row r="25" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:12" ht="15">
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
       <c r="D25" s="2"/>
@@ -4640,7 +4644,7 @@
       <c r="K25" s="2"/>
       <c r="L25" s="2"/>
     </row>
-    <row r="26" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:12" ht="15">
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
       <c r="D26" s="2"/>
@@ -4655,7 +4659,7 @@
       <c r="K26" s="2"/>
       <c r="L26" s="2"/>
     </row>
-    <row r="27" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:12" ht="15">
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
       <c r="D27" s="2"/>
@@ -4670,7 +4674,7 @@
       <c r="K27" s="2"/>
       <c r="L27" s="2"/>
     </row>
-    <row r="28" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:12" ht="15">
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
       <c r="D28" s="2"/>
@@ -4685,7 +4689,7 @@
       <c r="K28" s="2"/>
       <c r="L28" s="2"/>
     </row>
-    <row r="29" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:12" ht="15">
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
       <c r="D29" s="2"/>
@@ -4700,7 +4704,7 @@
       <c r="K29" s="2"/>
       <c r="L29" s="2"/>
     </row>
-    <row r="30" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:12" ht="15">
       <c r="B30" s="2"/>
       <c r="C30" s="2"/>
       <c r="D30" s="2"/>
@@ -4715,7 +4719,7 @@
       <c r="K30" s="2"/>
       <c r="L30" s="2"/>
     </row>
-    <row r="31" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:12" ht="15">
       <c r="B31" s="2"/>
       <c r="C31" s="2"/>
       <c r="D31" s="2"/>
@@ -4730,7 +4734,7 @@
       <c r="K31" s="2"/>
       <c r="L31" s="2"/>
     </row>
-    <row r="32" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:12" ht="15">
       <c r="B32" s="2"/>
       <c r="C32" s="2"/>
       <c r="D32" s="2"/>
@@ -4745,7 +4749,7 @@
       <c r="K32" s="2"/>
       <c r="L32" s="2"/>
     </row>
-    <row r="33" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:12" ht="15">
       <c r="B33" s="2"/>
       <c r="C33" s="2"/>
       <c r="D33" s="2"/>
@@ -4760,7 +4764,7 @@
       <c r="K33" s="2"/>
       <c r="L33" s="2"/>
     </row>
-    <row r="34" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:12" ht="15">
       <c r="B34" s="2"/>
       <c r="C34" s="2"/>
       <c r="D34" s="2"/>
@@ -4775,7 +4779,7 @@
       <c r="K34" s="2"/>
       <c r="L34" s="2"/>
     </row>
-    <row r="35" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:12" ht="15">
       <c r="B35" s="2"/>
       <c r="C35" s="2"/>
       <c r="D35" s="2"/>
@@ -4790,7 +4794,7 @@
       <c r="K35" s="2"/>
       <c r="L35" s="2"/>
     </row>
-    <row r="36" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:12" ht="15">
       <c r="B36" s="2"/>
       <c r="C36" s="2"/>
       <c r="D36" s="2"/>
@@ -4805,7 +4809,7 @@
       <c r="K36" s="2"/>
       <c r="L36" s="2"/>
     </row>
-    <row r="37" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:12" ht="15">
       <c r="B37" s="2"/>
       <c r="C37" s="2"/>
       <c r="D37" s="2"/>
@@ -4820,7 +4824,7 @@
       <c r="K37" s="2"/>
       <c r="L37" s="2"/>
     </row>
-    <row r="38" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:12" ht="15">
       <c r="B38" s="2"/>
       <c r="C38" s="2"/>
       <c r="D38" s="2"/>
@@ -4835,7 +4839,7 @@
       <c r="K38" s="2"/>
       <c r="L38" s="2"/>
     </row>
-    <row r="39" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:12" ht="15">
       <c r="B39" s="2"/>
       <c r="C39" s="2"/>
       <c r="D39" s="2"/>
@@ -4850,7 +4854,7 @@
       <c r="K39" s="2"/>
       <c r="L39" s="2"/>
     </row>
-    <row r="40" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:12" ht="15">
       <c r="B40" s="2"/>
       <c r="C40" s="2"/>
       <c r="D40" s="2"/>
@@ -4865,7 +4869,7 @@
       <c r="K40" s="2"/>
       <c r="L40" s="2"/>
     </row>
-    <row r="41" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:12" ht="15">
       <c r="B41" s="2"/>
       <c r="C41" s="2"/>
       <c r="D41" s="2"/>
@@ -4880,7 +4884,7 @@
       <c r="K41" s="2"/>
       <c r="L41" s="2"/>
     </row>
-    <row r="42" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:12" ht="15">
       <c r="B42" s="2"/>
       <c r="C42" s="2"/>
       <c r="D42" s="2"/>
@@ -4895,7 +4899,7 @@
       <c r="K42" s="2"/>
       <c r="L42" s="2"/>
     </row>
-    <row r="43" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:12" ht="15">
       <c r="B43" s="2"/>
       <c r="C43" s="2"/>
       <c r="D43" s="2"/>
@@ -4910,7 +4914,7 @@
       <c r="K43" s="2"/>
       <c r="L43" s="2"/>
     </row>
-    <row r="44" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:12" ht="15">
       <c r="B44" s="2"/>
       <c r="C44" s="2"/>
       <c r="D44" s="2"/>
@@ -4925,7 +4929,7 @@
       <c r="K44" s="2"/>
       <c r="L44" s="2"/>
     </row>
-    <row r="45" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:12" ht="15">
       <c r="B45" s="2"/>
       <c r="C45" s="2"/>
       <c r="D45" s="2"/>
@@ -4940,7 +4944,7 @@
       <c r="K45" s="2"/>
       <c r="L45" s="2"/>
     </row>
-    <row r="46" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:12" ht="15">
       <c r="B46" s="2"/>
       <c r="C46" s="2"/>
       <c r="D46" s="2"/>
@@ -4955,7 +4959,7 @@
       <c r="K46" s="2"/>
       <c r="L46" s="2"/>
     </row>
-    <row r="47" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:12" ht="15">
       <c r="B47" s="2"/>
       <c r="C47" s="2"/>
       <c r="D47" s="2"/>
@@ -4970,7 +4974,7 @@
       <c r="K47" s="2"/>
       <c r="L47" s="2"/>
     </row>
-    <row r="48" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:12" ht="15">
       <c r="B48" s="2"/>
       <c r="C48" s="2"/>
       <c r="D48" s="2"/>
@@ -4985,7 +4989,7 @@
       <c r="K48" s="2"/>
       <c r="L48" s="2"/>
     </row>
-    <row r="49" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:12" ht="15">
       <c r="B49" s="2"/>
       <c r="C49" s="2"/>
       <c r="D49" s="2"/>
@@ -4997,7 +5001,7 @@
       <c r="K49" s="2"/>
       <c r="L49" s="2"/>
     </row>
-    <row r="50" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:12" ht="15">
       <c r="B50" s="2"/>
       <c r="C50" s="2"/>
       <c r="D50" s="2"/>
@@ -5009,7 +5013,7 @@
       <c r="K50" s="2"/>
       <c r="L50" s="2"/>
     </row>
-    <row r="51" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:12" ht="15">
       <c r="B51" s="2"/>
       <c r="C51" s="2"/>
       <c r="D51" s="2"/>
@@ -5022,7 +5026,7 @@
       <c r="K51" s="2"/>
       <c r="L51" s="2"/>
     </row>
-    <row r="52" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:12" ht="15">
       <c r="B52" s="2"/>
       <c r="C52" s="2"/>
       <c r="D52" s="2"/>
@@ -5035,7 +5039,7 @@
       <c r="K52" s="2"/>
       <c r="L52" s="2"/>
     </row>
-    <row r="53" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:12" ht="15">
       <c r="B53" s="2"/>
       <c r="C53" s="2"/>
       <c r="D53" s="2"/>
@@ -5048,7 +5052,7 @@
       <c r="K53" s="2"/>
       <c r="L53" s="2"/>
     </row>
-    <row r="54" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:12" ht="15">
       <c r="B54" s="2"/>
       <c r="C54" s="2"/>
       <c r="D54" s="2"/>
@@ -5061,7 +5065,7 @@
       <c r="K54" s="2"/>
       <c r="L54" s="2"/>
     </row>
-    <row r="55" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:12" ht="15">
       <c r="B55" s="2"/>
       <c r="C55" s="2"/>
       <c r="D55" s="2"/>
@@ -5074,7 +5078,7 @@
       <c r="K55" s="2"/>
       <c r="L55" s="2"/>
     </row>
-    <row r="56" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:12" ht="15">
       <c r="B56" s="2"/>
       <c r="C56" s="2"/>
       <c r="D56" s="2"/>
@@ -5087,7 +5091,7 @@
       <c r="K56" s="2"/>
       <c r="L56" s="2"/>
     </row>
-    <row r="57" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:12" ht="15">
       <c r="B57" s="2"/>
       <c r="C57" s="2"/>
       <c r="D57" s="2"/>
@@ -5100,7 +5104,7 @@
       <c r="K57" s="2"/>
       <c r="L57" s="2"/>
     </row>
-    <row r="58" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:12" ht="15">
       <c r="B58" s="2"/>
       <c r="C58" s="2"/>
       <c r="D58" s="2"/>
@@ -5113,7 +5117,7 @@
       <c r="K58" s="2"/>
       <c r="L58" s="2"/>
     </row>
-    <row r="59" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:12" ht="15">
       <c r="B59" s="2"/>
       <c r="C59" s="2"/>
       <c r="D59" s="2"/>
@@ -5126,7 +5130,7 @@
       <c r="K59" s="2"/>
       <c r="L59" s="2"/>
     </row>
-    <row r="60" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:12" ht="15">
       <c r="B60" s="2"/>
       <c r="C60" s="2"/>
       <c r="D60" s="2"/>
@@ -5139,7 +5143,7 @@
       <c r="K60" s="2"/>
       <c r="L60" s="2"/>
     </row>
-    <row r="61" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:12" ht="15">
       <c r="B61" s="2"/>
       <c r="C61" s="2"/>
       <c r="D61" s="2"/>
@@ -5152,7 +5156,7 @@
       <c r="K61" s="2"/>
       <c r="L61" s="2"/>
     </row>
-    <row r="62" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:12" ht="15">
       <c r="B62" s="2"/>
       <c r="C62" s="2"/>
       <c r="D62" s="2"/>
@@ -5165,7 +5169,7 @@
       <c r="K62" s="2"/>
       <c r="L62" s="2"/>
     </row>
-    <row r="63" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="63" spans="2:12" ht="15">
       <c r="B63" s="2"/>
       <c r="C63" s="2"/>
       <c r="D63" s="2"/>
@@ -5178,7 +5182,7 @@
       <c r="K63" s="2"/>
       <c r="L63" s="2"/>
     </row>
-    <row r="64" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="64" spans="2:12" ht="15">
       <c r="B64" s="2"/>
       <c r="C64" s="2"/>
       <c r="D64" s="2"/>
@@ -5191,7 +5195,7 @@
       <c r="K64" s="2"/>
       <c r="L64" s="2"/>
     </row>
-    <row r="65" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:12" ht="15">
       <c r="B65" s="2"/>
       <c r="C65" s="2"/>
       <c r="D65" s="2"/>
@@ -5204,7 +5208,7 @@
       <c r="K65" s="2"/>
       <c r="L65" s="2"/>
     </row>
-    <row r="66" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:12" ht="15">
       <c r="B66" s="2"/>
       <c r="C66" s="2"/>
       <c r="D66" s="2"/>
@@ -5217,7 +5221,7 @@
       <c r="K66" s="2"/>
       <c r="L66" s="2"/>
     </row>
-    <row r="67" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:12" ht="15">
       <c r="B67" s="2"/>
       <c r="C67" s="2"/>
       <c r="D67" s="2"/>
@@ -5230,7 +5234,7 @@
       <c r="K67" s="2"/>
       <c r="L67" s="2"/>
     </row>
-    <row r="68" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:12" ht="15">
       <c r="B68" s="2"/>
       <c r="C68" s="2"/>
       <c r="D68" s="2"/>
@@ -5243,7 +5247,7 @@
       <c r="K68" s="2"/>
       <c r="L68" s="2"/>
     </row>
-    <row r="69" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:12" ht="15">
       <c r="B69" s="2"/>
       <c r="C69" s="2"/>
       <c r="D69" s="2"/>
@@ -5256,7 +5260,7 @@
       <c r="K69" s="2"/>
       <c r="L69" s="2"/>
     </row>
-    <row r="70" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:12" ht="15">
       <c r="B70" s="2"/>
       <c r="C70" s="2"/>
       <c r="D70" s="2"/>
@@ -5269,7 +5273,7 @@
       <c r="K70" s="2"/>
       <c r="L70" s="2"/>
     </row>
-    <row r="71" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:12" ht="15">
       <c r="A71" s="2"/>
       <c r="B71" s="2"/>
       <c r="C71" s="2"/>
@@ -5283,7 +5287,7 @@
       <c r="K71" s="2"/>
       <c r="L71" s="2"/>
     </row>
-    <row r="72" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:12" ht="15">
       <c r="A72" s="2"/>
       <c r="B72" s="2"/>
       <c r="C72" s="2"/>
@@ -5297,7 +5301,7 @@
       <c r="K72" s="2"/>
       <c r="L72" s="2"/>
     </row>
-    <row r="73" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:12" ht="15">
       <c r="A73" s="2"/>
       <c r="B73" s="2"/>
       <c r="C73" s="2"/>
@@ -5311,7 +5315,7 @@
       <c r="K73" s="2"/>
       <c r="L73" s="2"/>
     </row>
-    <row r="74" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:12" ht="15">
       <c r="A74" s="2"/>
       <c r="B74" s="2"/>
       <c r="C74" s="2"/>
@@ -5325,7 +5329,7 @@
       <c r="K74" s="2"/>
       <c r="L74" s="2"/>
     </row>
-    <row r="75" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:12" ht="15">
       <c r="A75" s="2"/>
       <c r="B75" s="2"/>
       <c r="C75" s="2"/>
@@ -5339,7 +5343,7 @@
       <c r="K75" s="2"/>
       <c r="L75" s="2"/>
     </row>
-    <row r="76" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:12" ht="15">
       <c r="A76" s="2"/>
       <c r="B76" s="2"/>
       <c r="C76" s="2"/>
@@ -5353,7 +5357,7 @@
       <c r="K76" s="2"/>
       <c r="L76" s="2"/>
     </row>
-    <row r="77" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:12" ht="15">
       <c r="A77" s="2"/>
       <c r="B77" s="2"/>
       <c r="C77" s="2"/>
@@ -5367,7 +5371,7 @@
       <c r="K77" s="2"/>
       <c r="L77" s="2"/>
     </row>
-    <row r="78" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:12" ht="15">
       <c r="A78" s="2"/>
       <c r="B78" s="2"/>
       <c r="C78" s="2"/>
@@ -5381,7 +5385,7 @@
       <c r="K78" s="2"/>
       <c r="L78" s="2"/>
     </row>
-    <row r="79" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:12" ht="15">
       <c r="A79" s="2"/>
       <c r="B79" s="2"/>
       <c r="C79" s="2"/>
@@ -5395,7 +5399,7 @@
       <c r="K79" s="2"/>
       <c r="L79" s="2"/>
     </row>
-    <row r="80" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:12" ht="15">
       <c r="A80" s="2"/>
       <c r="B80" s="2"/>
       <c r="C80" s="2"/>
@@ -5409,7 +5413,7 @@
       <c r="K80" s="2"/>
       <c r="L80" s="2"/>
     </row>
-    <row r="81" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:12" ht="15">
       <c r="A81" s="2"/>
       <c r="B81" s="2"/>
       <c r="C81" s="2"/>
@@ -5423,7 +5427,7 @@
       <c r="K81" s="2"/>
       <c r="L81" s="2"/>
     </row>
-    <row r="82" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:12" ht="15">
       <c r="A82" s="2"/>
       <c r="B82" s="2"/>
       <c r="C82" s="2"/>
@@ -5437,7 +5441,7 @@
       <c r="K82" s="2"/>
       <c r="L82" s="2"/>
     </row>
-    <row r="83" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:12" ht="15">
       <c r="A83" s="2"/>
       <c r="B83" s="2"/>
       <c r="C83" s="2"/>
@@ -5451,7 +5455,7 @@
       <c r="K83" s="2"/>
       <c r="L83" s="2"/>
     </row>
-    <row r="84" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:12" ht="15">
       <c r="A84" s="2"/>
       <c r="B84" s="2"/>
       <c r="C84" s="2"/>
@@ -5465,7 +5469,7 @@
       <c r="K84" s="2"/>
       <c r="L84" s="2"/>
     </row>
-    <row r="85" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:12" ht="15">
       <c r="A85" s="2"/>
       <c r="B85" s="2"/>
       <c r="C85" s="2"/>
@@ -5479,7 +5483,7 @@
       <c r="K85" s="2"/>
       <c r="L85" s="2"/>
     </row>
-    <row r="86" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:12" ht="15">
       <c r="A86" s="2"/>
       <c r="B86" s="2"/>
       <c r="C86" s="2"/>
@@ -5493,7 +5497,7 @@
       <c r="K86" s="2"/>
       <c r="L86" s="2"/>
     </row>
-    <row r="87" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:12" ht="15">
       <c r="A87" s="2"/>
       <c r="B87" s="2"/>
       <c r="C87" s="2"/>
@@ -5507,7 +5511,7 @@
       <c r="K87" s="2"/>
       <c r="L87" s="2"/>
     </row>
-    <row r="88" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:12" ht="15">
       <c r="A88" s="2"/>
       <c r="B88" s="2"/>
       <c r="C88" s="2"/>
@@ -5521,7 +5525,7 @@
       <c r="K88" s="2"/>
       <c r="L88" s="2"/>
     </row>
-    <row r="89" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:12" ht="15">
       <c r="A89" s="2"/>
       <c r="B89" s="2"/>
       <c r="C89" s="2"/>
@@ -5535,7 +5539,7 @@
       <c r="K89" s="2"/>
       <c r="L89" s="2"/>
     </row>
-    <row r="90" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:12" ht="15">
       <c r="A90" s="2"/>
       <c r="B90" s="2"/>
       <c r="C90" s="2"/>
@@ -5549,7 +5553,7 @@
       <c r="K90" s="2"/>
       <c r="L90" s="2"/>
     </row>
-    <row r="91" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:12" ht="15">
       <c r="A91" s="2"/>
       <c r="B91" s="2"/>
       <c r="C91" s="2"/>
@@ -5563,7 +5567,7 @@
       <c r="K91" s="2"/>
       <c r="L91" s="2"/>
     </row>
-    <row r="92" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:12" ht="15">
       <c r="A92" s="2"/>
       <c r="B92" s="2"/>
       <c r="C92" s="2"/>
@@ -5577,7 +5581,7 @@
       <c r="K92" s="2"/>
       <c r="L92" s="2"/>
     </row>
-    <row r="93" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:12" ht="15">
       <c r="A93" s="2"/>
       <c r="B93" s="2"/>
       <c r="C93" s="2"/>
@@ -5591,7 +5595,7 @@
       <c r="K93" s="2"/>
       <c r="L93" s="2"/>
     </row>
-    <row r="94" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:12" ht="15">
       <c r="A94" s="2"/>
       <c r="B94" s="2"/>
       <c r="C94" s="2"/>
@@ -5605,7 +5609,7 @@
       <c r="K94" s="2"/>
       <c r="L94" s="2"/>
     </row>
-    <row r="95" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:12" ht="15">
       <c r="A95" s="2"/>
       <c r="B95" s="2"/>
       <c r="C95" s="2"/>
@@ -5619,7 +5623,7 @@
       <c r="K95" s="2"/>
       <c r="L95" s="2"/>
     </row>
-    <row r="96" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:12" ht="15">
       <c r="A96" s="2"/>
       <c r="B96" s="2"/>
       <c r="C96" s="2"/>
@@ -5633,7 +5637,7 @@
       <c r="K96" s="2"/>
       <c r="L96" s="2"/>
     </row>
-    <row r="97" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:12" ht="15">
       <c r="A97" s="2"/>
       <c r="B97" s="2"/>
       <c r="C97" s="2"/>
@@ -5647,7 +5651,7 @@
       <c r="K97" s="2"/>
       <c r="L97" s="2"/>
     </row>
-    <row r="98" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:12" ht="15">
       <c r="A98" s="2"/>
       <c r="B98" s="2"/>
       <c r="C98" s="2"/>
@@ -5661,7 +5665,7 @@
       <c r="K98" s="2"/>
       <c r="L98" s="2"/>
     </row>
-    <row r="99" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:12" ht="15">
       <c r="A99" s="2"/>
       <c r="B99" s="2"/>
       <c r="C99" s="2"/>
@@ -5675,7 +5679,7 @@
       <c r="K99" s="2"/>
       <c r="L99" s="2"/>
     </row>
-    <row r="100" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:12" ht="15">
       <c r="A100" s="2"/>
       <c r="B100" s="2"/>
       <c r="C100" s="2"/>
@@ -5689,7 +5693,7 @@
       <c r="K100" s="2"/>
       <c r="L100" s="2"/>
     </row>
-    <row r="101" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:12" ht="15">
       <c r="A101" s="2"/>
       <c r="B101" s="2"/>
       <c r="C101" s="2"/>
@@ -5703,7 +5707,7 @@
       <c r="K101" s="2"/>
       <c r="L101" s="2"/>
     </row>
-    <row r="102" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:12" ht="15">
       <c r="A102" s="2"/>
       <c r="B102" s="2"/>
       <c r="C102" s="2"/>
@@ -5717,7 +5721,7 @@
       <c r="K102" s="2"/>
       <c r="L102" s="2"/>
     </row>
-    <row r="103" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:12" ht="15">
       <c r="A103" s="2"/>
       <c r="B103" s="2"/>
       <c r="C103" s="2"/>
@@ -5731,7 +5735,7 @@
       <c r="K103" s="2"/>
       <c r="L103" s="2"/>
     </row>
-    <row r="104" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:12" ht="15">
       <c r="A104" s="2"/>
       <c r="B104" s="2"/>
       <c r="C104" s="2"/>
@@ -5745,7 +5749,7 @@
       <c r="K104" s="2"/>
       <c r="L104" s="2"/>
     </row>
-    <row r="105" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:12" ht="15">
       <c r="A105" s="2"/>
       <c r="B105" s="2"/>
       <c r="C105" s="2"/>
@@ -5759,7 +5763,7 @@
       <c r="K105" s="2"/>
       <c r="L105" s="2"/>
     </row>
-    <row r="106" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:12" ht="15">
       <c r="A106" s="2"/>
       <c r="B106" s="2"/>
       <c r="C106" s="2"/>
@@ -5773,7 +5777,7 @@
       <c r="K106" s="2"/>
       <c r="L106" s="2"/>
     </row>
-    <row r="107" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:12" ht="15">
       <c r="A107" s="2"/>
       <c r="B107" s="2"/>
       <c r="C107" s="2"/>
@@ -5787,7 +5791,7 @@
       <c r="K107" s="2"/>
       <c r="L107" s="2"/>
     </row>
-    <row r="108" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:12" ht="15">
       <c r="A108" s="2"/>
       <c r="B108" s="2"/>
       <c r="C108" s="2"/>
@@ -5801,7 +5805,7 @@
       <c r="K108" s="2"/>
       <c r="L108" s="2"/>
     </row>
-    <row r="109" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:12" ht="15">
       <c r="A109" s="2"/>
       <c r="B109" s="2"/>
       <c r="C109" s="2"/>
@@ -5815,7 +5819,7 @@
       <c r="K109" s="2"/>
       <c r="L109" s="2"/>
     </row>
-    <row r="110" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:12" ht="15">
       <c r="A110" s="2"/>
       <c r="B110" s="2"/>
       <c r="C110" s="2"/>
@@ -5829,7 +5833,7 @@
       <c r="K110" s="2"/>
       <c r="L110" s="2"/>
     </row>
-    <row r="111" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:12" ht="15">
       <c r="A111" s="2"/>
       <c r="B111" s="2"/>
       <c r="C111" s="2"/>
@@ -5843,7 +5847,7 @@
       <c r="K111" s="2"/>
       <c r="L111" s="2"/>
     </row>
-    <row r="112" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:12" ht="15">
       <c r="A112" s="2"/>
       <c r="B112" s="2"/>
       <c r="C112" s="2"/>
@@ -5857,7 +5861,7 @@
       <c r="K112" s="2"/>
       <c r="L112" s="2"/>
     </row>
-    <row r="113" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:12" ht="15">
       <c r="A113" s="2"/>
       <c r="B113" s="2"/>
       <c r="C113" s="2"/>
@@ -5871,7 +5875,7 @@
       <c r="K113" s="2"/>
       <c r="L113" s="2"/>
     </row>
-    <row r="114" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:12" ht="15">
       <c r="A114" s="2"/>
       <c r="B114" s="2"/>
       <c r="C114" s="2"/>
@@ -5885,7 +5889,7 @@
       <c r="K114" s="2"/>
       <c r="L114" s="2"/>
     </row>
-    <row r="115" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:12" ht="15">
       <c r="A115" s="2"/>
       <c r="B115" s="2"/>
       <c r="C115" s="2"/>
@@ -5899,7 +5903,7 @@
       <c r="K115" s="2"/>
       <c r="L115" s="2"/>
     </row>
-    <row r="116" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:12" ht="15">
       <c r="A116" s="2"/>
       <c r="B116" s="2"/>
       <c r="C116" s="2"/>
@@ -5913,7 +5917,7 @@
       <c r="K116" s="2"/>
       <c r="L116" s="2"/>
     </row>
-    <row r="117" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:12" ht="15">
       <c r="A117" s="2"/>
       <c r="B117" s="2"/>
       <c r="C117" s="2"/>
@@ -5927,7 +5931,7 @@
       <c r="K117" s="2"/>
       <c r="L117" s="2"/>
     </row>
-    <row r="118" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:12" ht="15">
       <c r="A118" s="2"/>
       <c r="B118" s="2"/>
       <c r="C118" s="2"/>
@@ -5941,7 +5945,7 @@
       <c r="K118" s="2"/>
       <c r="L118" s="2"/>
     </row>
-    <row r="119" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:12" ht="15">
       <c r="A119" s="2"/>
       <c r="B119" s="2"/>
       <c r="C119" s="2"/>
@@ -5955,7 +5959,7 @@
       <c r="K119" s="2"/>
       <c r="L119" s="2"/>
     </row>
-    <row r="120" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:12" ht="15">
       <c r="A120" s="2"/>
       <c r="B120" s="2"/>
       <c r="C120" s="2"/>
@@ -5969,7 +5973,7 @@
       <c r="K120" s="2"/>
       <c r="L120" s="2"/>
     </row>
-    <row r="121" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:12" ht="15">
       <c r="A121" s="2"/>
       <c r="B121" s="2"/>
       <c r="C121" s="2"/>
@@ -5983,7 +5987,7 @@
       <c r="K121" s="2"/>
       <c r="L121" s="2"/>
     </row>
-    <row r="122" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:12" ht="15">
       <c r="A122" s="2"/>
       <c r="B122" s="2"/>
       <c r="C122" s="2"/>
@@ -5997,7 +6001,7 @@
       <c r="K122" s="2"/>
       <c r="L122" s="2"/>
     </row>
-    <row r="123" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:12" ht="15">
       <c r="A123" s="2"/>
       <c r="B123" s="2"/>
       <c r="C123" s="2"/>
@@ -6011,7 +6015,7 @@
       <c r="K123" s="2"/>
       <c r="L123" s="2"/>
     </row>
-    <row r="124" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:12" ht="15">
       <c r="A124" s="2"/>
       <c r="B124" s="2"/>
       <c r="C124" s="2"/>
@@ -6025,7 +6029,7 @@
       <c r="K124" s="2"/>
       <c r="L124" s="2"/>
     </row>
-    <row r="125" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:12" ht="15">
       <c r="A125" s="2"/>
       <c r="B125" s="2"/>
       <c r="C125" s="2"/>
@@ -6039,7 +6043,7 @@
       <c r="K125" s="2"/>
       <c r="L125" s="2"/>
     </row>
-    <row r="126" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:12" ht="15">
       <c r="A126" s="2"/>
       <c r="B126" s="2"/>
       <c r="C126" s="2"/>
@@ -6053,7 +6057,7 @@
       <c r="K126" s="2"/>
       <c r="L126" s="2"/>
     </row>
-    <row r="127" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:12" ht="15">
       <c r="A127" s="2"/>
       <c r="B127" s="2"/>
       <c r="C127" s="2"/>
@@ -6067,7 +6071,7 @@
       <c r="K127" s="2"/>
       <c r="L127" s="2"/>
     </row>
-    <row r="128" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:12" ht="15">
       <c r="A128" s="2"/>
       <c r="B128" s="2"/>
       <c r="C128" s="2"/>
@@ -6081,7 +6085,7 @@
       <c r="K128" s="2"/>
       <c r="L128" s="2"/>
     </row>
-    <row r="129" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:12" ht="15">
       <c r="A129" s="2"/>
       <c r="B129" s="2"/>
       <c r="C129" s="2"/>
@@ -6095,7 +6099,7 @@
       <c r="K129" s="2"/>
       <c r="L129" s="2"/>
     </row>
-    <row r="130" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:12" ht="15">
       <c r="A130" s="2"/>
       <c r="B130" s="2"/>
       <c r="C130" s="2"/>
@@ -6109,7 +6113,7 @@
       <c r="K130" s="2"/>
       <c r="L130" s="2"/>
     </row>
-    <row r="131" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:12" ht="15">
       <c r="A131" s="2"/>
       <c r="B131" s="2"/>
       <c r="C131" s="2"/>
@@ -6123,7 +6127,7 @@
       <c r="K131" s="2"/>
       <c r="L131" s="2"/>
     </row>
-    <row r="132" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:12" ht="15">
       <c r="A132" s="2"/>
       <c r="B132" s="2"/>
       <c r="C132" s="2"/>
@@ -6137,7 +6141,7 @@
       <c r="K132" s="2"/>
       <c r="L132" s="2"/>
     </row>
-    <row r="133" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:12" ht="15">
       <c r="A133" s="2"/>
       <c r="B133" s="2"/>
       <c r="C133" s="2"/>
@@ -6174,6 +6178,10 @@
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Ajuste de escaleta tema 11
Ajuste de escaleta tema 11
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado06/guion11/ESCALETA MA_06_11_CO.xlsx
+++ b/fuentes/contenidos/grado06/guion11/ESCALETA MA_06_11_CO.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060"/>
+    <workbookView xWindow="-2380" yWindow="0" windowWidth="25600" windowHeight="14580"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja2" sheetId="2" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="506" uniqueCount="215">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="506" uniqueCount="216">
   <si>
     <t>Asignatura</t>
   </si>
@@ -533,9 +533,6 @@
     <t>Mapa conceptual sobre el tema Los polígonos y la circunferencia</t>
   </si>
   <si>
-    <t>Secuencia e imágenes que presenta los conceptos básicos de geometría</t>
-  </si>
-  <si>
     <t>Interactivo que muestra diferentes clases de polígonos según sus lados</t>
   </si>
   <si>
@@ -557,12 +554,6 @@
     <t>Actividades sobre Los polígonos</t>
   </si>
   <si>
-    <t>Actividad para indicar los pasos que se sigfuen en la construcción de triánguos a partir de condiciones dadas</t>
-  </si>
-  <si>
-    <t>Interactivo con el cual se explican las líneas notables de los triángulos</t>
-  </si>
-  <si>
     <t>Actividades sobre Los triángulos</t>
   </si>
   <si>
@@ -575,15 +566,6 @@
     <t xml:space="preserve">Actividades sobre Los cuadriláteros </t>
   </si>
   <si>
-    <t>Interactivo sobre los elementos de la circunferencia, las posibles posiciones relativas de una recta, una circunferencia y de dos circunferencias</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Actividad que plantea asociar diferentes posiciones relativas de una cirdunferencia respecto a rectas u otra circunferencia </t>
-  </si>
-  <si>
-    <t>Actividad que propone aplicar los pasos necesarios para reconocer y relacionar los elementos de la circunferencia</t>
-  </si>
-  <si>
     <t>Actividad sobre los polígonos utilizando el tangram</t>
   </si>
   <si>
@@ -659,16 +641,37 @@
     <t>Clasifica polígonos según la medida de sus  ángulos</t>
   </si>
   <si>
-    <t>Actividad para emitir juicios sobre afirmaciones relacionadas con los cuadriláteros</t>
-  </si>
-  <si>
     <t>Reconoce información sobre los cuadriláteros</t>
   </si>
   <si>
-    <t>Actividad para evaluar conocimientos sobre el tema Los poligonos y la circunferencia</t>
-  </si>
-  <si>
     <t>Clasifica polígonos según su número de lados</t>
+  </si>
+  <si>
+    <t>Secuencia de imágenes que presenta los conceptos básicos de geometría</t>
+  </si>
+  <si>
+    <t>Actividad para organizar los pasos en la construcción  de un triángulo</t>
+  </si>
+  <si>
+    <t>Interactivo para explicar las líneas notables en los triángulos</t>
+  </si>
+  <si>
+    <t>Actividad de razonamiento sobre los cuadriláteros</t>
+  </si>
+  <si>
+    <t>Interactivo sobre diferentes conceptos de la circunferencia</t>
+  </si>
+  <si>
+    <t>Actividad sobre las posiciones relativas de una circunferencia y una recta</t>
+  </si>
+  <si>
+    <t>Actividades sobre La circunferencia</t>
+  </si>
+  <si>
+    <t>Actividad relacionada con los conceptos de circunferencia</t>
+  </si>
+  <si>
+    <t>Evaluación sobre el tema Los poligonos y la circunferencia</t>
   </si>
 </sst>
 </file>
@@ -942,7 +945,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="73">
+  <cellXfs count="74">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -985,16 +988,7 @@
     <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
@@ -1064,31 +1058,16 @@
     <xf numFmtId="0" fontId="4" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1129,6 +1108,33 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1436,142 +1442,142 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U121"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O7" sqref="O7"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J28" sqref="J28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="16.5" style="20" customWidth="1"/>
-    <col min="2" max="2" width="24.5" style="20" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="31" style="20" customWidth="1"/>
-    <col min="4" max="4" width="22.6640625" style="20" customWidth="1"/>
-    <col min="5" max="5" width="22.1640625" style="44" customWidth="1"/>
-    <col min="6" max="6" width="23.5" style="43" customWidth="1"/>
-    <col min="7" max="7" width="25.83203125" style="20" customWidth="1"/>
-    <col min="8" max="8" width="12.33203125" style="43" customWidth="1"/>
-    <col min="9" max="9" width="11" style="43" customWidth="1"/>
-    <col min="10" max="10" width="73.5" style="28" customWidth="1"/>
-    <col min="11" max="11" width="13.33203125" style="20" customWidth="1"/>
-    <col min="12" max="12" width="17.5" style="20" customWidth="1"/>
-    <col min="13" max="14" width="9.33203125" style="20" customWidth="1"/>
-    <col min="15" max="15" width="58.5" style="43" customWidth="1"/>
-    <col min="16" max="16" width="16.5" style="43" customWidth="1"/>
-    <col min="17" max="17" width="20.5" style="43" customWidth="1"/>
-    <col min="18" max="18" width="23" style="20" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="20.6640625" style="20" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="25.83203125" style="20" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="21.6640625" style="20" customWidth="1"/>
-    <col min="22" max="16384" width="10.83203125" style="20"/>
+    <col min="1" max="1" width="16.5" style="17" customWidth="1"/>
+    <col min="2" max="2" width="24.5" style="17" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="31" style="17" customWidth="1"/>
+    <col min="4" max="4" width="22.6640625" style="17" customWidth="1"/>
+    <col min="5" max="5" width="19.83203125" style="41" customWidth="1"/>
+    <col min="6" max="6" width="20.33203125" style="40" customWidth="1"/>
+    <col min="7" max="7" width="53.5" style="17" customWidth="1"/>
+    <col min="8" max="8" width="12.33203125" style="40" customWidth="1"/>
+    <col min="9" max="9" width="11" style="40" customWidth="1"/>
+    <col min="10" max="10" width="73.5" style="25" customWidth="1"/>
+    <col min="11" max="11" width="13.33203125" style="17" customWidth="1"/>
+    <col min="12" max="12" width="17.5" style="17" customWidth="1"/>
+    <col min="13" max="14" width="9.33203125" style="17" customWidth="1"/>
+    <col min="15" max="15" width="58.5" style="40" customWidth="1"/>
+    <col min="16" max="16" width="16.5" style="40" customWidth="1"/>
+    <col min="17" max="17" width="20.5" style="40" customWidth="1"/>
+    <col min="18" max="18" width="23" style="17" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="20.6640625" style="17" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="25.83203125" style="17" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="21.6640625" style="17" customWidth="1"/>
+    <col min="22" max="16384" width="10.83203125" style="17"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="33.75" customHeight="1">
-      <c r="A1" s="62" t="s">
+      <c r="A1" s="54" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="60" t="s">
+      <c r="B1" s="52" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="71" t="s">
+      <c r="C1" s="63" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="62" t="s">
+      <c r="D1" s="54" t="s">
         <v>110</v>
       </c>
-      <c r="E1" s="60" t="s">
+      <c r="E1" s="52" t="s">
         <v>111</v>
       </c>
-      <c r="F1" s="58" t="s">
+      <c r="F1" s="48" t="s">
         <v>112</v>
       </c>
-      <c r="G1" s="64" t="s">
+      <c r="G1" s="56" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="58" t="s">
+      <c r="H1" s="48" t="s">
         <v>113</v>
       </c>
-      <c r="I1" s="58" t="s">
+      <c r="I1" s="48" t="s">
         <v>107</v>
       </c>
-      <c r="J1" s="68" t="s">
+      <c r="J1" s="60" t="s">
         <v>4</v>
       </c>
-      <c r="K1" s="66" t="s">
+      <c r="K1" s="58" t="s">
         <v>108</v>
       </c>
-      <c r="L1" s="64" t="s">
+      <c r="L1" s="56" t="s">
         <v>14</v>
       </c>
-      <c r="M1" s="70" t="s">
+      <c r="M1" s="62" t="s">
         <v>21</v>
       </c>
-      <c r="N1" s="70"/>
-      <c r="O1" s="51" t="s">
+      <c r="N1" s="62"/>
+      <c r="O1" s="50" t="s">
         <v>109</v>
       </c>
-      <c r="P1" s="51" t="s">
+      <c r="P1" s="50" t="s">
         <v>114</v>
       </c>
-      <c r="Q1" s="53" t="s">
+      <c r="Q1" s="65" t="s">
         <v>85</v>
       </c>
-      <c r="R1" s="57" t="s">
+      <c r="R1" s="69" t="s">
         <v>86</v>
       </c>
-      <c r="S1" s="53" t="s">
+      <c r="S1" s="65" t="s">
         <v>87</v>
       </c>
-      <c r="T1" s="54" t="s">
+      <c r="T1" s="66" t="s">
         <v>88</v>
       </c>
-      <c r="U1" s="53" t="s">
+      <c r="U1" s="65" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="2" spans="1:21" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A2" s="63"/>
-      <c r="B2" s="61"/>
-      <c r="C2" s="72"/>
-      <c r="D2" s="63"/>
-      <c r="E2" s="61"/>
-      <c r="F2" s="59"/>
-      <c r="G2" s="65"/>
-      <c r="H2" s="59"/>
-      <c r="I2" s="59"/>
-      <c r="J2" s="69"/>
-      <c r="K2" s="67"/>
-      <c r="L2" s="65"/>
-      <c r="M2" s="33" t="s">
+      <c r="A2" s="55"/>
+      <c r="B2" s="53"/>
+      <c r="C2" s="64"/>
+      <c r="D2" s="55"/>
+      <c r="E2" s="53"/>
+      <c r="F2" s="49"/>
+      <c r="G2" s="57"/>
+      <c r="H2" s="49"/>
+      <c r="I2" s="49"/>
+      <c r="J2" s="61"/>
+      <c r="K2" s="59"/>
+      <c r="L2" s="57"/>
+      <c r="M2" s="30" t="s">
         <v>90</v>
       </c>
-      <c r="N2" s="33" t="s">
+      <c r="N2" s="30" t="s">
         <v>91</v>
       </c>
-      <c r="O2" s="52"/>
-      <c r="P2" s="52"/>
-      <c r="Q2" s="56"/>
-      <c r="R2" s="57"/>
-      <c r="S2" s="56"/>
-      <c r="T2" s="55"/>
-      <c r="U2" s="53"/>
+      <c r="O2" s="51"/>
+      <c r="P2" s="51"/>
+      <c r="Q2" s="68"/>
+      <c r="R2" s="69"/>
+      <c r="S2" s="68"/>
+      <c r="T2" s="67"/>
+      <c r="U2" s="65"/>
     </row>
     <row r="3" spans="1:21" ht="16" thickTop="1">
       <c r="A3" s="8" t="s">
         <v>15</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>199</v>
+        <v>193</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>200</v>
+        <v>194</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>201</v>
+        <v>195</v>
       </c>
       <c r="E3" s="9"/>
       <c r="F3" s="11"/>
-      <c r="G3" s="16" t="s">
+      <c r="G3" s="70" t="s">
         <v>147</v>
       </c>
       <c r="H3" s="11">
@@ -1580,8 +1586,8 @@
       <c r="I3" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="J3" s="24" t="s">
-        <v>169</v>
+      <c r="J3" s="21" t="s">
+        <v>207</v>
       </c>
       <c r="K3" s="13" t="s">
         <v>19</v>
@@ -1591,23 +1597,23 @@
       </c>
       <c r="M3" s="14"/>
       <c r="N3" s="14"/>
-      <c r="O3" s="34"/>
-      <c r="P3" s="45" t="s">
+      <c r="O3" s="31"/>
+      <c r="P3" s="42" t="s">
         <v>19</v>
       </c>
-      <c r="Q3" s="47">
+      <c r="Q3" s="44">
         <v>7</v>
       </c>
-      <c r="R3" s="49" t="s">
+      <c r="R3" s="46" t="s">
         <v>145</v>
       </c>
-      <c r="S3" s="47" t="s">
+      <c r="S3" s="44" t="s">
         <v>146</v>
       </c>
-      <c r="T3" s="50" t="s">
+      <c r="T3" s="47" t="s">
         <v>147</v>
       </c>
-      <c r="U3" s="47" t="s">
+      <c r="U3" s="44" t="s">
         <v>148</v>
       </c>
     </row>
@@ -1616,17 +1622,17 @@
         <v>15</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>199</v>
+        <v>193</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>200</v>
+        <v>194</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>201</v>
-      </c>
-      <c r="E4" s="35"/>
-      <c r="F4" s="36"/>
-      <c r="G4" s="16" t="s">
+        <v>195</v>
+      </c>
+      <c r="E4" s="32"/>
+      <c r="F4" s="33"/>
+      <c r="G4" s="70" t="s">
         <v>126</v>
       </c>
       <c r="H4" s="15">
@@ -1635,8 +1641,8 @@
       <c r="I4" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="J4" s="24" t="s">
-        <v>170</v>
+      <c r="J4" s="21" t="s">
+        <v>169</v>
       </c>
       <c r="K4" s="13" t="s">
         <v>19</v>
@@ -1646,23 +1652,23 @@
       </c>
       <c r="M4" s="7"/>
       <c r="N4" s="7"/>
-      <c r="O4" s="36"/>
-      <c r="P4" s="45" t="s">
+      <c r="O4" s="33"/>
+      <c r="P4" s="42" t="s">
         <v>19</v>
       </c>
-      <c r="Q4" s="47">
+      <c r="Q4" s="44">
         <v>7</v>
       </c>
-      <c r="R4" s="49" t="s">
+      <c r="R4" s="46" t="s">
         <v>145</v>
       </c>
-      <c r="S4" s="47" t="s">
+      <c r="S4" s="44" t="s">
         <v>146</v>
       </c>
-      <c r="T4" s="50" t="s">
+      <c r="T4" s="47" t="s">
         <v>126</v>
       </c>
-      <c r="U4" s="47" t="s">
+      <c r="U4" s="44" t="s">
         <v>148</v>
       </c>
     </row>
@@ -1671,17 +1677,17 @@
         <v>15</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>199</v>
+        <v>193</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>200</v>
+        <v>194</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>201</v>
-      </c>
-      <c r="E5" s="35"/>
-      <c r="F5" s="36"/>
-      <c r="G5" s="16" t="s">
+        <v>195</v>
+      </c>
+      <c r="E5" s="32"/>
+      <c r="F5" s="33"/>
+      <c r="G5" s="70" t="s">
         <v>149</v>
       </c>
       <c r="H5" s="11">
@@ -1690,8 +1696,8 @@
       <c r="I5" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="J5" s="24" t="s">
-        <v>173</v>
+      <c r="J5" s="21" t="s">
+        <v>172</v>
       </c>
       <c r="K5" s="13" t="s">
         <v>19</v>
@@ -1701,23 +1707,23 @@
       </c>
       <c r="M5" s="7"/>
       <c r="N5" s="7"/>
-      <c r="O5" s="36"/>
-      <c r="P5" s="45" t="s">
+      <c r="O5" s="33"/>
+      <c r="P5" s="42" t="s">
         <v>19</v>
       </c>
-      <c r="Q5" s="47">
+      <c r="Q5" s="44">
         <v>7</v>
       </c>
-      <c r="R5" s="49" t="s">
+      <c r="R5" s="46" t="s">
         <v>145</v>
       </c>
-      <c r="S5" s="47" t="s">
+      <c r="S5" s="44" t="s">
         <v>146</v>
       </c>
-      <c r="T5" s="50" t="s">
+      <c r="T5" s="47" t="s">
         <v>149</v>
       </c>
-      <c r="U5" s="47" t="s">
+      <c r="U5" s="44" t="s">
         <v>148</v>
       </c>
     </row>
@@ -1726,18 +1732,18 @@
         <v>15</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>199</v>
+        <v>193</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>200</v>
+        <v>194</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>201</v>
-      </c>
-      <c r="E6" s="35"/>
-      <c r="F6" s="36"/>
-      <c r="G6" s="16" t="s">
-        <v>210</v>
+        <v>195</v>
+      </c>
+      <c r="E6" s="32"/>
+      <c r="F6" s="33"/>
+      <c r="G6" s="70" t="s">
+        <v>204</v>
       </c>
       <c r="H6" s="15">
         <v>4</v>
@@ -1745,8 +1751,8 @@
       <c r="I6" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="J6" s="24" t="s">
-        <v>171</v>
+      <c r="J6" s="21" t="s">
+        <v>170</v>
       </c>
       <c r="K6" s="13" t="s">
         <v>20</v>
@@ -1758,26 +1764,26 @@
       <c r="N6" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="O6" s="36" t="s">
-        <v>187</v>
-      </c>
-      <c r="P6" s="45" t="s">
+      <c r="O6" s="33" t="s">
+        <v>181</v>
+      </c>
+      <c r="P6" s="42" t="s">
         <v>20</v>
       </c>
-      <c r="Q6" s="21">
+      <c r="Q6" s="18">
         <v>6</v>
       </c>
-      <c r="R6" s="22" t="s">
+      <c r="R6" s="19" t="s">
         <v>150</v>
       </c>
-      <c r="S6" s="21" t="s">
+      <c r="S6" s="18" t="s">
         <v>151</v>
       </c>
-      <c r="T6" s="48" t="s">
-        <v>206</v>
-      </c>
-      <c r="U6" s="21" t="s">
-        <v>209</v>
+      <c r="T6" s="45" t="s">
+        <v>200</v>
+      </c>
+      <c r="U6" s="18" t="s">
+        <v>203</v>
       </c>
     </row>
     <row r="7" spans="1:21" ht="15">
@@ -1785,18 +1791,18 @@
         <v>15</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>199</v>
+        <v>193</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>200</v>
-      </c>
-      <c r="D7" s="31" t="s">
-        <v>201</v>
-      </c>
-      <c r="E7" s="35"/>
-      <c r="F7" s="36"/>
-      <c r="G7" s="16" t="s">
-        <v>214</v>
+        <v>194</v>
+      </c>
+      <c r="D7" s="28" t="s">
+        <v>195</v>
+      </c>
+      <c r="E7" s="32"/>
+      <c r="F7" s="33"/>
+      <c r="G7" s="70" t="s">
+        <v>206</v>
       </c>
       <c r="H7" s="11">
         <v>5</v>
@@ -1804,7 +1810,7 @@
       <c r="I7" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="J7" s="24" t="s">
+      <c r="J7" s="21" t="s">
         <v>142</v>
       </c>
       <c r="K7" s="6" t="s">
@@ -1817,26 +1823,26 @@
       <c r="N7" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="O7" s="36" t="s">
-        <v>188</v>
-      </c>
-      <c r="P7" s="45" t="s">
+      <c r="O7" s="33" t="s">
+        <v>182</v>
+      </c>
+      <c r="P7" s="42" t="s">
         <v>20</v>
       </c>
-      <c r="Q7" s="21">
+      <c r="Q7" s="18">
         <v>6</v>
       </c>
-      <c r="R7" s="22" t="s">
+      <c r="R7" s="19" t="s">
         <v>150</v>
       </c>
-      <c r="S7" s="21" t="s">
+      <c r="S7" s="18" t="s">
         <v>151</v>
       </c>
-      <c r="T7" s="48" t="s">
+      <c r="T7" s="45" t="s">
         <v>152</v>
       </c>
-      <c r="U7" s="21" t="s">
-        <v>209</v>
+      <c r="U7" s="18" t="s">
+        <v>203</v>
       </c>
     </row>
     <row r="8" spans="1:21" ht="15">
@@ -1844,17 +1850,17 @@
         <v>15</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>199</v>
+        <v>193</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>200</v>
-      </c>
-      <c r="D8" s="31" t="s">
-        <v>201</v>
-      </c>
-      <c r="E8" s="35"/>
-      <c r="F8" s="36"/>
-      <c r="G8" s="16" t="s">
+        <v>194</v>
+      </c>
+      <c r="D8" s="28" t="s">
+        <v>195</v>
+      </c>
+      <c r="E8" s="32"/>
+      <c r="F8" s="33"/>
+      <c r="G8" s="70" t="s">
         <v>127</v>
       </c>
       <c r="H8" s="15">
@@ -1863,8 +1869,8 @@
       <c r="I8" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="J8" s="24" t="s">
-        <v>172</v>
+      <c r="J8" s="21" t="s">
+        <v>171</v>
       </c>
       <c r="K8" s="6" t="s">
         <v>19</v>
@@ -1874,23 +1880,23 @@
       </c>
       <c r="M8" s="7"/>
       <c r="N8" s="7"/>
-      <c r="O8" s="36"/>
-      <c r="P8" s="45" t="s">
+      <c r="O8" s="33"/>
+      <c r="P8" s="42" t="s">
         <v>19</v>
       </c>
-      <c r="Q8" s="47">
+      <c r="Q8" s="44">
         <v>7</v>
       </c>
-      <c r="R8" s="49" t="s">
+      <c r="R8" s="46" t="s">
         <v>145</v>
       </c>
-      <c r="S8" s="47" t="s">
+      <c r="S8" s="44" t="s">
         <v>146</v>
       </c>
-      <c r="T8" s="50" t="s">
+      <c r="T8" s="47" t="s">
         <v>127</v>
       </c>
-      <c r="U8" s="47" t="s">
+      <c r="U8" s="44" t="s">
         <v>148</v>
       </c>
     </row>
@@ -1899,17 +1905,17 @@
         <v>15</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>199</v>
+        <v>193</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>200</v>
-      </c>
-      <c r="D9" s="31" t="s">
-        <v>201</v>
-      </c>
-      <c r="E9" s="35"/>
-      <c r="F9" s="36"/>
-      <c r="G9" s="16" t="s">
+        <v>194</v>
+      </c>
+      <c r="D9" s="28" t="s">
+        <v>195</v>
+      </c>
+      <c r="E9" s="32"/>
+      <c r="F9" s="33"/>
+      <c r="G9" s="70" t="s">
         <v>128</v>
       </c>
       <c r="H9" s="11">
@@ -1918,7 +1924,7 @@
       <c r="I9" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="J9" s="24" t="s">
+      <c r="J9" s="21" t="s">
         <v>143</v>
       </c>
       <c r="K9" s="6" t="s">
@@ -1931,26 +1937,26 @@
       <c r="N9" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="O9" s="36" t="s">
-        <v>189</v>
-      </c>
-      <c r="P9" s="45" t="s">
+      <c r="O9" s="33" t="s">
+        <v>183</v>
+      </c>
+      <c r="P9" s="42" t="s">
         <v>19</v>
       </c>
-      <c r="Q9" s="21">
+      <c r="Q9" s="18">
         <v>6</v>
       </c>
-      <c r="R9" s="22" t="s">
+      <c r="R9" s="19" t="s">
         <v>150</v>
       </c>
-      <c r="S9" s="21" t="s">
+      <c r="S9" s="18" t="s">
         <v>151</v>
       </c>
-      <c r="T9" s="48" t="s">
+      <c r="T9" s="45" t="s">
         <v>153</v>
       </c>
-      <c r="U9" s="21" t="s">
-        <v>209</v>
+      <c r="U9" s="18" t="s">
+        <v>203</v>
       </c>
     </row>
     <row r="10" spans="1:21" ht="15">
@@ -1958,18 +1964,18 @@
         <v>15</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>199</v>
+        <v>193</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>200</v>
-      </c>
-      <c r="D10" s="31" t="s">
-        <v>201</v>
-      </c>
-      <c r="E10" s="35"/>
-      <c r="F10" s="36"/>
-      <c r="G10" s="16" t="s">
-        <v>174</v>
+        <v>194</v>
+      </c>
+      <c r="D10" s="28" t="s">
+        <v>195</v>
+      </c>
+      <c r="E10" s="32"/>
+      <c r="F10" s="33"/>
+      <c r="G10" s="70" t="s">
+        <v>173</v>
       </c>
       <c r="H10" s="15">
         <v>8</v>
@@ -1977,8 +1983,8 @@
       <c r="I10" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="J10" s="24" t="s">
-        <v>175</v>
+      <c r="J10" s="21" t="s">
+        <v>174</v>
       </c>
       <c r="K10" s="6" t="s">
         <v>19</v>
@@ -1988,23 +1994,23 @@
       </c>
       <c r="M10" s="7"/>
       <c r="N10" s="7"/>
-      <c r="O10" s="36"/>
-      <c r="P10" s="45" t="s">
+      <c r="O10" s="33"/>
+      <c r="P10" s="42" t="s">
         <v>19</v>
       </c>
-      <c r="Q10" s="47">
+      <c r="Q10" s="44">
         <v>7</v>
       </c>
-      <c r="R10" s="49" t="s">
+      <c r="R10" s="46" t="s">
         <v>145</v>
       </c>
-      <c r="S10" s="47" t="s">
+      <c r="S10" s="44" t="s">
         <v>146</v>
       </c>
-      <c r="T10" s="50" t="s">
+      <c r="T10" s="47" t="s">
         <v>154</v>
       </c>
-      <c r="U10" s="47" t="s">
+      <c r="U10" s="44" t="s">
         <v>148</v>
       </c>
     </row>
@@ -2013,17 +2019,17 @@
         <v>15</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>199</v>
+        <v>193</v>
       </c>
       <c r="C11" s="10" t="s">
-        <v>200</v>
-      </c>
-      <c r="D11" s="31" t="s">
-        <v>201</v>
-      </c>
-      <c r="E11" s="35"/>
-      <c r="F11" s="36"/>
-      <c r="G11" s="16" t="s">
+        <v>194</v>
+      </c>
+      <c r="D11" s="28" t="s">
+        <v>195</v>
+      </c>
+      <c r="E11" s="32"/>
+      <c r="F11" s="33"/>
+      <c r="G11" s="70" t="s">
         <v>129</v>
       </c>
       <c r="H11" s="11">
@@ -2032,8 +2038,8 @@
       <c r="I11" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="J11" s="24" t="s">
-        <v>190</v>
+      <c r="J11" s="21" t="s">
+        <v>184</v>
       </c>
       <c r="K11" s="6" t="s">
         <v>20</v>
@@ -2045,25 +2051,25 @@
         <v>56</v>
       </c>
       <c r="N11" s="7"/>
-      <c r="O11" s="36" t="s">
-        <v>191</v>
-      </c>
-      <c r="P11" s="45" t="s">
+      <c r="O11" s="33" t="s">
+        <v>185</v>
+      </c>
+      <c r="P11" s="42" t="s">
         <v>19</v>
       </c>
-      <c r="Q11" s="21">
+      <c r="Q11" s="18">
         <v>6</v>
       </c>
-      <c r="R11" s="22" t="s">
+      <c r="R11" s="19" t="s">
         <v>155</v>
       </c>
-      <c r="S11" s="21" t="s">
+      <c r="S11" s="18" t="s">
         <v>156</v>
       </c>
-      <c r="T11" s="48" t="s">
+      <c r="T11" s="45" t="s">
         <v>157</v>
       </c>
-      <c r="U11" s="21" t="s">
+      <c r="U11" s="18" t="s">
         <v>158</v>
       </c>
     </row>
@@ -2072,19 +2078,19 @@
         <v>15</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>199</v>
+        <v>193</v>
       </c>
       <c r="C12" s="10" t="s">
-        <v>200</v>
-      </c>
-      <c r="D12" s="31" t="s">
-        <v>201</v>
-      </c>
-      <c r="E12" s="35" t="s">
+        <v>194</v>
+      </c>
+      <c r="D12" s="28" t="s">
+        <v>195</v>
+      </c>
+      <c r="E12" s="32" t="s">
         <v>125</v>
       </c>
-      <c r="F12" s="36"/>
-      <c r="G12" s="17" t="s">
+      <c r="F12" s="33"/>
+      <c r="G12" s="71" t="s">
         <v>130</v>
       </c>
       <c r="H12" s="15">
@@ -2093,8 +2099,8 @@
       <c r="I12" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="J12" s="25" t="s">
-        <v>176</v>
+      <c r="J12" s="22" t="s">
+        <v>175</v>
       </c>
       <c r="K12" s="6" t="s">
         <v>19</v>
@@ -2104,23 +2110,23 @@
       </c>
       <c r="M12" s="7"/>
       <c r="N12" s="7"/>
-      <c r="O12" s="36"/>
-      <c r="P12" s="45" t="s">
+      <c r="O12" s="33"/>
+      <c r="P12" s="42" t="s">
         <v>19</v>
       </c>
-      <c r="Q12" s="47">
+      <c r="Q12" s="44">
         <v>7</v>
       </c>
-      <c r="R12" s="49" t="s">
+      <c r="R12" s="46" t="s">
         <v>145</v>
       </c>
-      <c r="S12" s="47" t="s">
+      <c r="S12" s="44" t="s">
         <v>146</v>
       </c>
-      <c r="T12" s="50" t="s">
+      <c r="T12" s="47" t="s">
         <v>130</v>
       </c>
-      <c r="U12" s="47" t="s">
+      <c r="U12" s="44" t="s">
         <v>148</v>
       </c>
     </row>
@@ -2129,17 +2135,17 @@
         <v>15</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>199</v>
+        <v>193</v>
       </c>
       <c r="C13" s="10" t="s">
-        <v>200</v>
-      </c>
-      <c r="D13" s="31" t="s">
-        <v>202</v>
-      </c>
-      <c r="E13" s="35"/>
-      <c r="F13" s="36"/>
-      <c r="G13" s="18" t="s">
+        <v>194</v>
+      </c>
+      <c r="D13" s="28" t="s">
+        <v>196</v>
+      </c>
+      <c r="E13" s="32"/>
+      <c r="F13" s="33"/>
+      <c r="G13" s="72" t="s">
         <v>131</v>
       </c>
       <c r="H13" s="11">
@@ -2148,7 +2154,7 @@
       <c r="I13" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="J13" s="24" t="s">
+      <c r="J13" s="21" t="s">
         <v>144</v>
       </c>
       <c r="K13" s="6" t="s">
@@ -2159,25 +2165,25 @@
       </c>
       <c r="M13" s="7"/>
       <c r="N13" s="7"/>
-      <c r="O13" s="36" t="s">
-        <v>193</v>
-      </c>
-      <c r="P13" s="45" t="s">
+      <c r="O13" s="33" t="s">
+        <v>187</v>
+      </c>
+      <c r="P13" s="42" t="s">
         <v>19</v>
       </c>
-      <c r="Q13" s="47">
+      <c r="Q13" s="44">
         <v>7</v>
       </c>
-      <c r="R13" s="49" t="s">
+      <c r="R13" s="46" t="s">
         <v>145</v>
       </c>
-      <c r="S13" s="47" t="s">
+      <c r="S13" s="44" t="s">
         <v>146</v>
       </c>
-      <c r="T13" s="50" t="s">
+      <c r="T13" s="47" t="s">
         <v>131</v>
       </c>
-      <c r="U13" s="47" t="s">
+      <c r="U13" s="44" t="s">
         <v>148</v>
       </c>
     </row>
@@ -2186,17 +2192,17 @@
         <v>15</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>199</v>
+        <v>193</v>
       </c>
       <c r="C14" s="10" t="s">
-        <v>200</v>
-      </c>
-      <c r="D14" s="31" t="s">
-        <v>202</v>
-      </c>
-      <c r="E14" s="35"/>
-      <c r="F14" s="36"/>
-      <c r="G14" s="18" t="s">
+        <v>194</v>
+      </c>
+      <c r="D14" s="28" t="s">
+        <v>196</v>
+      </c>
+      <c r="E14" s="32"/>
+      <c r="F14" s="33"/>
+      <c r="G14" s="72" t="s">
         <v>132</v>
       </c>
       <c r="H14" s="15">
@@ -2205,8 +2211,8 @@
       <c r="I14" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="J14" s="24" t="s">
-        <v>177</v>
+      <c r="J14" s="21" t="s">
+        <v>208</v>
       </c>
       <c r="K14" s="6" t="s">
         <v>20</v>
@@ -2218,26 +2224,26 @@
       <c r="N14" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="O14" s="36" t="s">
-        <v>192</v>
-      </c>
-      <c r="P14" s="45" t="s">
+      <c r="O14" s="33" t="s">
+        <v>186</v>
+      </c>
+      <c r="P14" s="42" t="s">
         <v>19</v>
       </c>
-      <c r="Q14" s="21">
+      <c r="Q14" s="18">
         <v>6</v>
       </c>
-      <c r="R14" s="22" t="s">
+      <c r="R14" s="19" t="s">
         <v>150</v>
       </c>
-      <c r="S14" s="21" t="s">
+      <c r="S14" s="18" t="s">
         <v>151</v>
       </c>
-      <c r="T14" s="48" t="s">
-        <v>208</v>
-      </c>
-      <c r="U14" s="21" t="s">
-        <v>209</v>
+      <c r="T14" s="45" t="s">
+        <v>202</v>
+      </c>
+      <c r="U14" s="18" t="s">
+        <v>203</v>
       </c>
     </row>
     <row r="15" spans="1:21" ht="15">
@@ -2245,17 +2251,17 @@
         <v>15</v>
       </c>
       <c r="B15" s="9" t="s">
-        <v>199</v>
+        <v>193</v>
       </c>
       <c r="C15" s="10" t="s">
-        <v>200</v>
-      </c>
-      <c r="D15" s="31" t="s">
-        <v>202</v>
-      </c>
-      <c r="E15" s="35"/>
-      <c r="F15" s="36"/>
-      <c r="G15" s="18" t="s">
+        <v>194</v>
+      </c>
+      <c r="D15" s="28" t="s">
+        <v>196</v>
+      </c>
+      <c r="E15" s="32"/>
+      <c r="F15" s="33"/>
+      <c r="G15" s="72" t="s">
         <v>133</v>
       </c>
       <c r="H15" s="11">
@@ -2264,8 +2270,8 @@
       <c r="I15" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="J15" s="26" t="s">
-        <v>178</v>
+      <c r="J15" s="23" t="s">
+        <v>209</v>
       </c>
       <c r="K15" s="6" t="s">
         <v>20</v>
@@ -2277,25 +2283,25 @@
         <v>63</v>
       </c>
       <c r="N15" s="7"/>
-      <c r="O15" s="36" t="s">
-        <v>194</v>
-      </c>
-      <c r="P15" s="45" t="s">
+      <c r="O15" s="33" t="s">
+        <v>188</v>
+      </c>
+      <c r="P15" s="42" t="s">
         <v>19</v>
       </c>
-      <c r="Q15" s="21">
+      <c r="Q15" s="18">
         <v>6</v>
       </c>
-      <c r="R15" s="22" t="s">
+      <c r="R15" s="19" t="s">
         <v>155</v>
       </c>
-      <c r="S15" s="21" t="s">
+      <c r="S15" s="18" t="s">
         <v>156</v>
       </c>
-      <c r="T15" s="48" t="s">
+      <c r="T15" s="45" t="s">
         <v>159</v>
       </c>
-      <c r="U15" s="21" t="s">
+      <c r="U15" s="18" t="s">
         <v>158</v>
       </c>
     </row>
@@ -2304,19 +2310,19 @@
         <v>15</v>
       </c>
       <c r="B16" s="9" t="s">
-        <v>199</v>
+        <v>193</v>
       </c>
       <c r="C16" s="10" t="s">
-        <v>200</v>
-      </c>
-      <c r="D16" s="31" t="s">
-        <v>202</v>
-      </c>
-      <c r="E16" s="35" t="s">
+        <v>194</v>
+      </c>
+      <c r="D16" s="28" t="s">
+        <v>196</v>
+      </c>
+      <c r="E16" s="32" t="s">
         <v>125</v>
       </c>
-      <c r="F16" s="36"/>
-      <c r="G16" s="17" t="s">
+      <c r="F16" s="33"/>
+      <c r="G16" s="71" t="s">
         <v>134</v>
       </c>
       <c r="H16" s="15">
@@ -2325,8 +2331,8 @@
       <c r="I16" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="J16" s="27" t="s">
-        <v>179</v>
+      <c r="J16" s="24" t="s">
+        <v>176</v>
       </c>
       <c r="K16" s="6" t="s">
         <v>19</v>
@@ -2336,23 +2342,23 @@
       </c>
       <c r="M16" s="7"/>
       <c r="N16" s="7"/>
-      <c r="O16" s="36"/>
-      <c r="P16" s="45" t="s">
+      <c r="O16" s="33"/>
+      <c r="P16" s="42" t="s">
         <v>19</v>
       </c>
-      <c r="Q16" s="47">
+      <c r="Q16" s="44">
         <v>7</v>
       </c>
-      <c r="R16" s="49" t="s">
+      <c r="R16" s="46" t="s">
         <v>145</v>
       </c>
-      <c r="S16" s="47" t="s">
+      <c r="S16" s="44" t="s">
         <v>146</v>
       </c>
-      <c r="T16" s="50" t="s">
+      <c r="T16" s="47" t="s">
         <v>134</v>
       </c>
-      <c r="U16" s="47" t="s">
+      <c r="U16" s="44" t="s">
         <v>148</v>
       </c>
     </row>
@@ -2361,18 +2367,18 @@
         <v>15</v>
       </c>
       <c r="B17" s="9" t="s">
-        <v>199</v>
+        <v>193</v>
       </c>
       <c r="C17" s="10" t="s">
-        <v>200</v>
-      </c>
-      <c r="D17" s="32" t="s">
-        <v>203</v>
-      </c>
-      <c r="E17" s="35"/>
-      <c r="F17" s="36"/>
-      <c r="G17" s="18" t="s">
-        <v>212</v>
+        <v>194</v>
+      </c>
+      <c r="D17" s="29" t="s">
+        <v>197</v>
+      </c>
+      <c r="E17" s="32"/>
+      <c r="F17" s="33"/>
+      <c r="G17" s="72" t="s">
+        <v>205</v>
       </c>
       <c r="H17" s="11">
         <v>15</v>
@@ -2380,8 +2386,8 @@
       <c r="I17" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="J17" s="24" t="s">
-        <v>211</v>
+      <c r="J17" s="21" t="s">
+        <v>210</v>
       </c>
       <c r="K17" s="6" t="s">
         <v>20</v>
@@ -2393,26 +2399,26 @@
       <c r="N17" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="O17" s="36" t="s">
-        <v>195</v>
-      </c>
-      <c r="P17" s="45" t="s">
+      <c r="O17" s="33" t="s">
+        <v>189</v>
+      </c>
+      <c r="P17" s="42" t="s">
         <v>19</v>
       </c>
-      <c r="Q17" s="21">
+      <c r="Q17" s="18">
         <v>6</v>
       </c>
-      <c r="R17" s="22" t="s">
+      <c r="R17" s="19" t="s">
         <v>150</v>
       </c>
-      <c r="S17" s="21" t="s">
+      <c r="S17" s="18" t="s">
         <v>151</v>
       </c>
-      <c r="T17" s="48" t="s">
+      <c r="T17" s="45" t="s">
         <v>160</v>
       </c>
-      <c r="U17" s="21" t="s">
-        <v>209</v>
+      <c r="U17" s="18" t="s">
+        <v>203</v>
       </c>
     </row>
     <row r="18" spans="1:21" ht="15">
@@ -2420,17 +2426,17 @@
         <v>15</v>
       </c>
       <c r="B18" s="9" t="s">
-        <v>199</v>
+        <v>193</v>
       </c>
       <c r="C18" s="10" t="s">
-        <v>200</v>
-      </c>
-      <c r="D18" s="32" t="s">
-        <v>203</v>
-      </c>
-      <c r="E18" s="35"/>
-      <c r="F18" s="36"/>
-      <c r="G18" s="18" t="s">
+        <v>194</v>
+      </c>
+      <c r="D18" s="29" t="s">
+        <v>197</v>
+      </c>
+      <c r="E18" s="32"/>
+      <c r="F18" s="33"/>
+      <c r="G18" s="72" t="s">
         <v>135</v>
       </c>
       <c r="H18" s="15">
@@ -2439,8 +2445,8 @@
       <c r="I18" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="J18" s="24" t="s">
-        <v>180</v>
+      <c r="J18" s="21" t="s">
+        <v>177</v>
       </c>
       <c r="K18" s="6" t="s">
         <v>20</v>
@@ -2452,26 +2458,26 @@
       <c r="N18" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="O18" s="36" t="s">
-        <v>196</v>
-      </c>
-      <c r="P18" s="45" t="s">
+      <c r="O18" s="33" t="s">
+        <v>190</v>
+      </c>
+      <c r="P18" s="42" t="s">
         <v>19</v>
       </c>
-      <c r="Q18" s="21">
+      <c r="Q18" s="18">
         <v>6</v>
       </c>
-      <c r="R18" s="22" t="s">
+      <c r="R18" s="19" t="s">
         <v>150</v>
       </c>
-      <c r="S18" s="21" t="s">
+      <c r="S18" s="18" t="s">
         <v>151</v>
       </c>
-      <c r="T18" s="48" t="s">
+      <c r="T18" s="45" t="s">
         <v>161</v>
       </c>
-      <c r="U18" s="21" t="s">
-        <v>209</v>
+      <c r="U18" s="18" t="s">
+        <v>203</v>
       </c>
     </row>
     <row r="19" spans="1:21" ht="15">
@@ -2479,17 +2485,17 @@
         <v>15</v>
       </c>
       <c r="B19" s="9" t="s">
-        <v>199</v>
+        <v>193</v>
       </c>
       <c r="C19" s="10" t="s">
-        <v>200</v>
-      </c>
-      <c r="D19" s="32" t="s">
-        <v>203</v>
-      </c>
-      <c r="E19" s="35"/>
-      <c r="F19" s="36"/>
-      <c r="G19" s="18" t="s">
+        <v>194</v>
+      </c>
+      <c r="D19" s="29" t="s">
+        <v>197</v>
+      </c>
+      <c r="E19" s="32"/>
+      <c r="F19" s="33"/>
+      <c r="G19" s="72" t="s">
         <v>136</v>
       </c>
       <c r="H19" s="11">
@@ -2498,8 +2504,8 @@
       <c r="I19" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="J19" s="24" t="s">
-        <v>181</v>
+      <c r="J19" s="21" t="s">
+        <v>178</v>
       </c>
       <c r="K19" s="6" t="s">
         <v>20</v>
@@ -2511,26 +2517,26 @@
       <c r="N19" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="O19" s="36" t="s">
-        <v>197</v>
-      </c>
-      <c r="P19" s="45" t="s">
+      <c r="O19" s="33" t="s">
+        <v>191</v>
+      </c>
+      <c r="P19" s="42" t="s">
         <v>19</v>
       </c>
-      <c r="Q19" s="21">
+      <c r="Q19" s="18">
         <v>6</v>
       </c>
-      <c r="R19" s="22" t="s">
+      <c r="R19" s="19" t="s">
         <v>150</v>
       </c>
-      <c r="S19" s="21" t="s">
+      <c r="S19" s="18" t="s">
         <v>151</v>
       </c>
-      <c r="T19" s="48" t="s">
-        <v>207</v>
-      </c>
-      <c r="U19" s="21" t="s">
-        <v>209</v>
+      <c r="T19" s="45" t="s">
+        <v>201</v>
+      </c>
+      <c r="U19" s="18" t="s">
+        <v>203</v>
       </c>
     </row>
     <row r="20" spans="1:21" ht="15">
@@ -2538,19 +2544,19 @@
         <v>15</v>
       </c>
       <c r="B20" s="9" t="s">
-        <v>199</v>
+        <v>193</v>
       </c>
       <c r="C20" s="10" t="s">
-        <v>200</v>
-      </c>
-      <c r="D20" s="32" t="s">
-        <v>203</v>
-      </c>
-      <c r="E20" s="35" t="s">
+        <v>194</v>
+      </c>
+      <c r="D20" s="29" t="s">
+        <v>197</v>
+      </c>
+      <c r="E20" s="32" t="s">
         <v>125</v>
       </c>
-      <c r="F20" s="36"/>
-      <c r="G20" s="17" t="s">
+      <c r="F20" s="33"/>
+      <c r="G20" s="71" t="s">
         <v>162</v>
       </c>
       <c r="H20" s="15">
@@ -2559,8 +2565,8 @@
       <c r="I20" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="J20" s="24" t="s">
-        <v>182</v>
+      <c r="J20" s="21" t="s">
+        <v>179</v>
       </c>
       <c r="K20" s="6" t="s">
         <v>19</v>
@@ -2570,23 +2576,23 @@
       </c>
       <c r="M20" s="7"/>
       <c r="N20" s="7"/>
-      <c r="O20" s="36"/>
-      <c r="P20" s="45" t="s">
+      <c r="O20" s="33"/>
+      <c r="P20" s="42" t="s">
         <v>19</v>
       </c>
-      <c r="Q20" s="47">
+      <c r="Q20" s="44">
         <v>7</v>
       </c>
-      <c r="R20" s="49" t="s">
+      <c r="R20" s="46" t="s">
         <v>145</v>
       </c>
-      <c r="S20" s="47" t="s">
+      <c r="S20" s="44" t="s">
         <v>146</v>
       </c>
-      <c r="T20" s="50" t="s">
+      <c r="T20" s="47" t="s">
         <v>162</v>
       </c>
-      <c r="U20" s="47" t="s">
+      <c r="U20" s="44" t="s">
         <v>148</v>
       </c>
     </row>
@@ -2595,17 +2601,17 @@
         <v>15</v>
       </c>
       <c r="B21" s="9" t="s">
-        <v>199</v>
+        <v>193</v>
       </c>
       <c r="C21" s="10" t="s">
-        <v>200</v>
-      </c>
-      <c r="D21" s="32" t="s">
-        <v>204</v>
-      </c>
-      <c r="E21" s="35"/>
-      <c r="F21" s="36"/>
-      <c r="G21" s="17" t="s">
+        <v>194</v>
+      </c>
+      <c r="D21" s="29" t="s">
+        <v>198</v>
+      </c>
+      <c r="E21" s="32"/>
+      <c r="F21" s="33"/>
+      <c r="G21" s="73" t="s">
         <v>137</v>
       </c>
       <c r="H21" s="11">
@@ -2614,8 +2620,8 @@
       <c r="I21" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="J21" s="24" t="s">
-        <v>183</v>
+      <c r="J21" s="21" t="s">
+        <v>211</v>
       </c>
       <c r="K21" s="6" t="s">
         <v>19</v>
@@ -2625,23 +2631,23 @@
       </c>
       <c r="M21" s="7"/>
       <c r="N21" s="7"/>
-      <c r="O21" s="36"/>
-      <c r="P21" s="45" t="s">
+      <c r="O21" s="33"/>
+      <c r="P21" s="42" t="s">
         <v>19</v>
       </c>
-      <c r="Q21" s="47">
+      <c r="Q21" s="44">
         <v>7</v>
       </c>
-      <c r="R21" s="49" t="s">
+      <c r="R21" s="46" t="s">
         <v>145</v>
       </c>
-      <c r="S21" s="47" t="s">
+      <c r="S21" s="44" t="s">
         <v>146</v>
       </c>
-      <c r="T21" s="50" t="s">
+      <c r="T21" s="47" t="s">
         <v>163</v>
       </c>
-      <c r="U21" s="47" t="s">
+      <c r="U21" s="44" t="s">
         <v>148</v>
       </c>
     </row>
@@ -2650,17 +2656,17 @@
         <v>15</v>
       </c>
       <c r="B22" s="9" t="s">
-        <v>199</v>
+        <v>193</v>
       </c>
       <c r="C22" s="10" t="s">
-        <v>200</v>
-      </c>
-      <c r="D22" s="32" t="s">
-        <v>204</v>
-      </c>
-      <c r="E22" s="35"/>
-      <c r="F22" s="36"/>
-      <c r="G22" s="17" t="s">
+        <v>194</v>
+      </c>
+      <c r="D22" s="29" t="s">
+        <v>198</v>
+      </c>
+      <c r="E22" s="32"/>
+      <c r="F22" s="33"/>
+      <c r="G22" s="73" t="s">
         <v>138</v>
       </c>
       <c r="H22" s="15">
@@ -2669,8 +2675,8 @@
       <c r="I22" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="J22" s="24" t="s">
-        <v>184</v>
+      <c r="J22" s="21" t="s">
+        <v>212</v>
       </c>
       <c r="K22" s="6" t="s">
         <v>19</v>
@@ -2680,23 +2686,23 @@
       </c>
       <c r="M22" s="7"/>
       <c r="N22" s="7"/>
-      <c r="O22" s="36"/>
-      <c r="P22" s="45" t="s">
+      <c r="O22" s="33"/>
+      <c r="P22" s="42" t="s">
         <v>19</v>
       </c>
-      <c r="Q22" s="47">
+      <c r="Q22" s="44">
         <v>7</v>
       </c>
-      <c r="R22" s="49" t="s">
+      <c r="R22" s="46" t="s">
         <v>145</v>
       </c>
-      <c r="S22" s="47" t="s">
+      <c r="S22" s="44" t="s">
         <v>146</v>
       </c>
-      <c r="T22" s="50" t="s">
+      <c r="T22" s="47" t="s">
         <v>164</v>
       </c>
-      <c r="U22" s="47" t="s">
+      <c r="U22" s="44" t="s">
         <v>148</v>
       </c>
     </row>
@@ -2705,19 +2711,19 @@
         <v>15</v>
       </c>
       <c r="B23" s="9" t="s">
-        <v>199</v>
+        <v>193</v>
       </c>
       <c r="C23" s="10" t="s">
-        <v>200</v>
-      </c>
-      <c r="D23" s="32" t="s">
-        <v>204</v>
-      </c>
-      <c r="E23" s="35" t="s">
+        <v>194</v>
+      </c>
+      <c r="D23" s="29" t="s">
+        <v>198</v>
+      </c>
+      <c r="E23" s="32" t="s">
         <v>125</v>
       </c>
-      <c r="F23" s="36"/>
-      <c r="G23" s="17" t="s">
+      <c r="F23" s="33"/>
+      <c r="G23" s="71" t="s">
         <v>139</v>
       </c>
       <c r="H23" s="15">
@@ -2726,8 +2732,8 @@
       <c r="I23" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="J23" s="24" t="s">
-        <v>139</v>
+      <c r="J23" s="21" t="s">
+        <v>213</v>
       </c>
       <c r="K23" s="6" t="s">
         <v>19</v>
@@ -2737,23 +2743,23 @@
       </c>
       <c r="M23" s="7"/>
       <c r="N23" s="7"/>
-      <c r="O23" s="36"/>
-      <c r="P23" s="45" t="s">
+      <c r="O23" s="33"/>
+      <c r="P23" s="42" t="s">
         <v>19</v>
       </c>
-      <c r="Q23" s="47">
+      <c r="Q23" s="44">
         <v>7</v>
       </c>
-      <c r="R23" s="49" t="s">
+      <c r="R23" s="46" t="s">
         <v>145</v>
       </c>
-      <c r="S23" s="47" t="s">
+      <c r="S23" s="44" t="s">
         <v>146</v>
       </c>
-      <c r="T23" s="50" t="s">
+      <c r="T23" s="47" t="s">
         <v>139</v>
       </c>
-      <c r="U23" s="47" t="s">
+      <c r="U23" s="44" t="s">
         <v>148</v>
       </c>
     </row>
@@ -2762,17 +2768,17 @@
         <v>15</v>
       </c>
       <c r="B24" s="9" t="s">
-        <v>199</v>
+        <v>193</v>
       </c>
       <c r="C24" s="10" t="s">
-        <v>200</v>
-      </c>
-      <c r="D24" s="32" t="s">
+        <v>194</v>
+      </c>
+      <c r="D24" s="29" t="s">
         <v>123</v>
       </c>
-      <c r="E24" s="35"/>
-      <c r="F24" s="36"/>
-      <c r="G24" s="17" t="s">
+      <c r="E24" s="32"/>
+      <c r="F24" s="33"/>
+      <c r="G24" s="71" t="s">
         <v>140</v>
       </c>
       <c r="H24" s="11">
@@ -2781,8 +2787,8 @@
       <c r="I24" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="J24" s="24" t="s">
-        <v>185</v>
+      <c r="J24" s="21" t="s">
+        <v>214</v>
       </c>
       <c r="K24" s="6" t="s">
         <v>19</v>
@@ -2792,23 +2798,23 @@
       </c>
       <c r="M24" s="7"/>
       <c r="N24" s="7"/>
-      <c r="O24" s="36"/>
-      <c r="P24" s="45" t="s">
+      <c r="O24" s="33"/>
+      <c r="P24" s="42" t="s">
         <v>19</v>
       </c>
-      <c r="Q24" s="47">
+      <c r="Q24" s="44">
         <v>7</v>
       </c>
-      <c r="R24" s="49" t="s">
+      <c r="R24" s="46" t="s">
         <v>145</v>
       </c>
-      <c r="S24" s="47" t="s">
+      <c r="S24" s="44" t="s">
         <v>146</v>
       </c>
-      <c r="T24" s="50" t="s">
+      <c r="T24" s="47" t="s">
         <v>140</v>
       </c>
-      <c r="U24" s="47" t="s">
+      <c r="U24" s="44" t="s">
         <v>148</v>
       </c>
     </row>
@@ -2817,17 +2823,17 @@
         <v>15</v>
       </c>
       <c r="B25" s="9" t="s">
-        <v>199</v>
+        <v>193</v>
       </c>
       <c r="C25" s="10" t="s">
-        <v>200</v>
-      </c>
-      <c r="D25" s="32" t="s">
+        <v>194</v>
+      </c>
+      <c r="D25" s="29" t="s">
         <v>123</v>
       </c>
-      <c r="E25" s="35"/>
-      <c r="F25" s="36"/>
-      <c r="G25" s="17" t="s">
+      <c r="E25" s="32"/>
+      <c r="F25" s="33"/>
+      <c r="G25" s="71" t="s">
         <v>141</v>
       </c>
       <c r="H25" s="15">
@@ -2836,8 +2842,8 @@
       <c r="I25" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="J25" s="24" t="s">
-        <v>186</v>
+      <c r="J25" s="21" t="s">
+        <v>180</v>
       </c>
       <c r="K25" s="6" t="s">
         <v>20</v>
@@ -2849,26 +2855,26 @@
       <c r="N25" s="7" t="s">
         <v>120</v>
       </c>
-      <c r="O25" s="36" t="s">
-        <v>198</v>
-      </c>
-      <c r="P25" s="45" t="s">
+      <c r="O25" s="33" t="s">
+        <v>192</v>
+      </c>
+      <c r="P25" s="42" t="s">
         <v>20</v>
       </c>
-      <c r="Q25" s="21">
+      <c r="Q25" s="18">
         <v>6</v>
       </c>
-      <c r="R25" s="22" t="s">
+      <c r="R25" s="19" t="s">
         <v>150</v>
       </c>
-      <c r="S25" s="21" t="s">
+      <c r="S25" s="18" t="s">
         <v>151</v>
       </c>
-      <c r="T25" s="48" t="s">
+      <c r="T25" s="45" t="s">
         <v>165</v>
       </c>
-      <c r="U25" s="21" t="s">
-        <v>209</v>
+      <c r="U25" s="18" t="s">
+        <v>203</v>
       </c>
     </row>
     <row r="26" spans="1:21" ht="15">
@@ -2876,17 +2882,17 @@
         <v>15</v>
       </c>
       <c r="B26" s="9" t="s">
-        <v>199</v>
+        <v>193</v>
       </c>
       <c r="C26" s="10" t="s">
-        <v>200</v>
-      </c>
-      <c r="D26" s="32" t="s">
+        <v>194</v>
+      </c>
+      <c r="D26" s="29" t="s">
         <v>124</v>
       </c>
-      <c r="E26" s="35"/>
-      <c r="F26" s="36"/>
-      <c r="G26" s="19" t="s">
+      <c r="E26" s="32"/>
+      <c r="F26" s="33"/>
+      <c r="G26" s="73" t="s">
         <v>10</v>
       </c>
       <c r="H26" s="11">
@@ -2895,7 +2901,7 @@
       <c r="I26" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="J26" s="24" t="s">
+      <c r="J26" s="21" t="s">
         <v>168</v>
       </c>
       <c r="K26" s="6" t="s">
@@ -2906,32 +2912,32 @@
       </c>
       <c r="M26" s="7"/>
       <c r="N26" s="7"/>
-      <c r="O26" s="36"/>
-      <c r="P26" s="45" t="s">
+      <c r="O26" s="33"/>
+      <c r="P26" s="42" t="s">
         <v>19</v>
       </c>
-      <c r="Q26" s="21"/>
-      <c r="R26" s="22"/>
-      <c r="S26" s="21"/>
-      <c r="T26" s="48"/>
-      <c r="U26" s="21"/>
+      <c r="Q26" s="18"/>
+      <c r="R26" s="19"/>
+      <c r="S26" s="18"/>
+      <c r="T26" s="45"/>
+      <c r="U26" s="18"/>
     </row>
     <row r="27" spans="1:21" ht="15">
       <c r="A27" s="8" t="s">
         <v>15</v>
       </c>
       <c r="B27" s="9" t="s">
-        <v>199</v>
+        <v>193</v>
       </c>
       <c r="C27" s="10" t="s">
-        <v>200</v>
-      </c>
-      <c r="D27" s="32" t="s">
+        <v>194</v>
+      </c>
+      <c r="D27" s="29" t="s">
         <v>124</v>
       </c>
-      <c r="E27" s="35"/>
-      <c r="F27" s="36"/>
-      <c r="G27" s="18" t="s">
+      <c r="E27" s="32"/>
+      <c r="F27" s="33"/>
+      <c r="G27" s="72" t="s">
         <v>122</v>
       </c>
       <c r="H27" s="15">
@@ -2940,8 +2946,8 @@
       <c r="I27" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="J27" s="24" t="s">
-        <v>213</v>
+      <c r="J27" s="21" t="s">
+        <v>215</v>
       </c>
       <c r="K27" s="6" t="s">
         <v>20</v>
@@ -2951,24 +2957,24 @@
       <c r="N27" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="O27" s="36"/>
-      <c r="P27" s="45" t="s">
+      <c r="O27" s="33"/>
+      <c r="P27" s="42" t="s">
         <v>19</v>
       </c>
-      <c r="Q27" s="21">
+      <c r="Q27" s="18">
         <v>6</v>
       </c>
-      <c r="R27" s="46" t="s">
+      <c r="R27" s="43" t="s">
         <v>150</v>
       </c>
-      <c r="S27" s="21" t="s">
+      <c r="S27" s="18" t="s">
         <v>151</v>
       </c>
-      <c r="T27" s="23" t="s">
+      <c r="T27" s="20" t="s">
         <v>166</v>
       </c>
-      <c r="U27" s="21" t="s">
-        <v>209</v>
+      <c r="U27" s="18" t="s">
+        <v>203</v>
       </c>
     </row>
     <row r="28" spans="1:21" ht="15">
@@ -2976,24 +2982,24 @@
         <v>15</v>
       </c>
       <c r="B28" s="9" t="s">
+        <v>193</v>
+      </c>
+      <c r="C28" s="10" t="s">
+        <v>194</v>
+      </c>
+      <c r="D28" s="29" t="s">
         <v>199</v>
       </c>
-      <c r="C28" s="10" t="s">
-        <v>200</v>
-      </c>
-      <c r="D28" s="32" t="s">
-        <v>205</v>
-      </c>
-      <c r="E28" s="35"/>
-      <c r="F28" s="36"/>
-      <c r="G28" s="18"/>
+      <c r="E28" s="32"/>
+      <c r="F28" s="33"/>
+      <c r="G28" s="16"/>
       <c r="H28" s="15">
         <v>26</v>
       </c>
       <c r="I28" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="J28" s="24"/>
+      <c r="J28" s="21"/>
       <c r="K28" s="6" t="s">
         <v>20</v>
       </c>
@@ -3004,1159 +3010,1165 @@
       <c r="N28" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="O28" s="36"/>
-      <c r="P28" s="45" t="s">
+      <c r="O28" s="33"/>
+      <c r="P28" s="42" t="s">
         <v>20</v>
       </c>
-      <c r="Q28" s="21">
+      <c r="Q28" s="18">
         <v>6</v>
       </c>
-      <c r="R28" s="46" t="s">
+      <c r="R28" s="43" t="s">
         <v>150</v>
       </c>
-      <c r="S28" s="21" t="s">
+      <c r="S28" s="18" t="s">
         <v>151</v>
       </c>
-      <c r="T28" s="23" t="s">
+      <c r="T28" s="20" t="s">
         <v>167</v>
       </c>
-      <c r="U28" s="21" t="s">
-        <v>209</v>
+      <c r="U28" s="18" t="s">
+        <v>203</v>
       </c>
     </row>
     <row r="29" spans="1:21" ht="15">
       <c r="A29" s="8"/>
       <c r="B29" s="9"/>
-      <c r="C29" s="37"/>
-      <c r="D29" s="32"/>
-      <c r="E29" s="35"/>
-      <c r="F29" s="36"/>
-      <c r="G29" s="18"/>
+      <c r="C29" s="34"/>
+      <c r="D29" s="29"/>
+      <c r="E29" s="32"/>
+      <c r="F29" s="33"/>
+      <c r="G29" s="16"/>
       <c r="H29" s="11"/>
       <c r="I29" s="4"/>
-      <c r="J29" s="24"/>
+      <c r="J29" s="21"/>
       <c r="K29" s="6"/>
       <c r="L29" s="5"/>
       <c r="M29" s="7"/>
       <c r="N29" s="7"/>
-      <c r="O29" s="36"/>
-      <c r="P29" s="45"/>
-      <c r="Q29" s="38"/>
-      <c r="R29" s="39"/>
-      <c r="S29" s="38"/>
-      <c r="T29" s="40"/>
-      <c r="U29" s="38"/>
+      <c r="O29" s="33"/>
+      <c r="P29" s="42"/>
+      <c r="Q29" s="35"/>
+      <c r="R29" s="36"/>
+      <c r="S29" s="35"/>
+      <c r="T29" s="37"/>
+      <c r="U29" s="35"/>
     </row>
     <row r="30" spans="1:21" ht="15">
       <c r="A30" s="3"/>
-      <c r="B30" s="41"/>
-      <c r="C30" s="37"/>
-      <c r="D30" s="30"/>
-      <c r="E30" s="35"/>
-      <c r="F30" s="36"/>
-      <c r="G30" s="42"/>
-      <c r="H30" s="36"/>
+      <c r="B30" s="38"/>
+      <c r="C30" s="34"/>
+      <c r="D30" s="27"/>
+      <c r="E30" s="32"/>
+      <c r="F30" s="33"/>
+      <c r="G30" s="39"/>
+      <c r="H30" s="33"/>
       <c r="I30" s="4"/>
-      <c r="J30" s="24"/>
+      <c r="J30" s="21"/>
       <c r="K30" s="6"/>
       <c r="L30" s="5"/>
       <c r="M30" s="7"/>
       <c r="N30" s="7"/>
-      <c r="O30" s="36"/>
-      <c r="P30" s="34"/>
-      <c r="Q30" s="38"/>
-      <c r="R30" s="39"/>
-      <c r="S30" s="38"/>
-      <c r="T30" s="40"/>
-      <c r="U30" s="38"/>
+      <c r="O30" s="33"/>
+      <c r="P30" s="31"/>
+      <c r="Q30" s="35"/>
+      <c r="R30" s="36"/>
+      <c r="S30" s="35"/>
+      <c r="T30" s="37"/>
+      <c r="U30" s="35"/>
     </row>
     <row r="31" spans="1:21" ht="15">
       <c r="A31" s="3"/>
-      <c r="B31" s="41"/>
-      <c r="C31" s="37"/>
-      <c r="D31" s="30"/>
-      <c r="E31" s="35"/>
-      <c r="F31" s="36"/>
-      <c r="G31" s="42"/>
-      <c r="H31" s="36"/>
+      <c r="B31" s="38"/>
+      <c r="C31" s="34"/>
+      <c r="D31" s="27"/>
+      <c r="E31" s="32"/>
+      <c r="F31" s="33"/>
+      <c r="G31" s="39"/>
+      <c r="H31" s="33"/>
       <c r="I31" s="4"/>
-      <c r="J31" s="24"/>
+      <c r="J31" s="21"/>
       <c r="K31" s="6"/>
       <c r="L31" s="5"/>
       <c r="M31" s="7"/>
       <c r="N31" s="7"/>
-      <c r="O31" s="36"/>
-      <c r="P31" s="34"/>
-      <c r="Q31" s="38"/>
-      <c r="R31" s="39"/>
-      <c r="S31" s="38"/>
-      <c r="T31" s="40"/>
-      <c r="U31" s="38"/>
+      <c r="O31" s="33"/>
+      <c r="P31" s="31"/>
+      <c r="Q31" s="35"/>
+      <c r="R31" s="36"/>
+      <c r="S31" s="35"/>
+      <c r="T31" s="37"/>
+      <c r="U31" s="35"/>
     </row>
     <row r="32" spans="1:21" ht="15">
       <c r="A32" s="3"/>
-      <c r="B32" s="41"/>
-      <c r="C32" s="37"/>
-      <c r="D32" s="30"/>
-      <c r="E32" s="35"/>
-      <c r="F32" s="36"/>
-      <c r="G32" s="42"/>
-      <c r="H32" s="36"/>
+      <c r="B32" s="38"/>
+      <c r="C32" s="34"/>
+      <c r="D32" s="27"/>
+      <c r="E32" s="32"/>
+      <c r="F32" s="33"/>
+      <c r="G32" s="39"/>
+      <c r="H32" s="33"/>
       <c r="I32" s="4"/>
-      <c r="J32" s="24"/>
+      <c r="J32" s="21"/>
       <c r="K32" s="6"/>
       <c r="L32" s="5"/>
       <c r="M32" s="7"/>
       <c r="N32" s="7"/>
-      <c r="O32" s="36"/>
-      <c r="P32" s="36"/>
-      <c r="Q32" s="38"/>
-      <c r="R32" s="39"/>
-      <c r="S32" s="38"/>
-      <c r="T32" s="40"/>
-      <c r="U32" s="38"/>
+      <c r="O32" s="33"/>
+      <c r="P32" s="33"/>
+      <c r="Q32" s="35"/>
+      <c r="R32" s="36"/>
+      <c r="S32" s="35"/>
+      <c r="T32" s="37"/>
+      <c r="U32" s="35"/>
     </row>
     <row r="33" spans="1:21" ht="15">
       <c r="A33" s="3"/>
-      <c r="B33" s="41"/>
-      <c r="C33" s="37"/>
-      <c r="D33" s="30"/>
-      <c r="E33" s="35"/>
-      <c r="F33" s="36"/>
-      <c r="G33" s="42"/>
-      <c r="H33" s="36"/>
+      <c r="B33" s="38"/>
+      <c r="C33" s="34"/>
+      <c r="D33" s="27"/>
+      <c r="E33" s="32"/>
+      <c r="F33" s="33"/>
+      <c r="G33" s="39"/>
+      <c r="H33" s="33"/>
       <c r="I33" s="4"/>
-      <c r="J33" s="24"/>
+      <c r="J33" s="21"/>
       <c r="K33" s="6"/>
       <c r="L33" s="5"/>
       <c r="M33" s="7"/>
       <c r="N33" s="7"/>
-      <c r="O33" s="36"/>
-      <c r="P33" s="36"/>
-      <c r="Q33" s="38"/>
-      <c r="R33" s="39"/>
-      <c r="S33" s="38"/>
-      <c r="T33" s="40"/>
-      <c r="U33" s="38"/>
+      <c r="O33" s="33"/>
+      <c r="P33" s="33"/>
+      <c r="Q33" s="35"/>
+      <c r="R33" s="36"/>
+      <c r="S33" s="35"/>
+      <c r="T33" s="37"/>
+      <c r="U33" s="35"/>
     </row>
     <row r="34" spans="1:21" ht="15">
       <c r="A34" s="3"/>
-      <c r="B34" s="41"/>
-      <c r="C34" s="37"/>
-      <c r="D34" s="30"/>
-      <c r="E34" s="35"/>
-      <c r="F34" s="36"/>
-      <c r="G34" s="42"/>
-      <c r="H34" s="36"/>
+      <c r="B34" s="38"/>
+      <c r="C34" s="34"/>
+      <c r="D34" s="27"/>
+      <c r="E34" s="32"/>
+      <c r="F34" s="33"/>
+      <c r="G34" s="39"/>
+      <c r="H34" s="33"/>
       <c r="I34" s="4"/>
-      <c r="J34" s="29"/>
+      <c r="J34" s="26"/>
       <c r="K34" s="6"/>
       <c r="L34" s="5"/>
       <c r="M34" s="7"/>
       <c r="N34" s="7"/>
-      <c r="O34" s="36"/>
-      <c r="P34" s="36"/>
-      <c r="Q34" s="38"/>
-      <c r="R34" s="39"/>
-      <c r="S34" s="38"/>
-      <c r="T34" s="40"/>
-      <c r="U34" s="38"/>
+      <c r="O34" s="33"/>
+      <c r="P34" s="33"/>
+      <c r="Q34" s="35"/>
+      <c r="R34" s="36"/>
+      <c r="S34" s="35"/>
+      <c r="T34" s="37"/>
+      <c r="U34" s="35"/>
     </row>
     <row r="35" spans="1:21" ht="15">
       <c r="A35" s="3"/>
-      <c r="B35" s="41"/>
-      <c r="C35" s="37"/>
-      <c r="D35" s="30"/>
-      <c r="E35" s="35"/>
-      <c r="F35" s="36"/>
-      <c r="G35" s="42"/>
-      <c r="H35" s="36"/>
+      <c r="B35" s="38"/>
+      <c r="C35" s="34"/>
+      <c r="D35" s="27"/>
+      <c r="E35" s="32"/>
+      <c r="F35" s="33"/>
+      <c r="G35" s="39"/>
+      <c r="H35" s="33"/>
       <c r="I35" s="4"/>
-      <c r="J35" s="29"/>
+      <c r="J35" s="26"/>
       <c r="K35" s="6"/>
       <c r="L35" s="5"/>
       <c r="M35" s="7"/>
       <c r="N35" s="7"/>
-      <c r="O35" s="36"/>
-      <c r="P35" s="36"/>
-      <c r="Q35" s="38"/>
-      <c r="R35" s="39"/>
-      <c r="S35" s="38"/>
-      <c r="T35" s="40"/>
-      <c r="U35" s="38"/>
+      <c r="O35" s="33"/>
+      <c r="P35" s="33"/>
+      <c r="Q35" s="35"/>
+      <c r="R35" s="36"/>
+      <c r="S35" s="35"/>
+      <c r="T35" s="37"/>
+      <c r="U35" s="35"/>
     </row>
     <row r="36" spans="1:21" ht="15">
       <c r="A36" s="3"/>
-      <c r="B36" s="41"/>
-      <c r="C36" s="37"/>
-      <c r="D36" s="30"/>
-      <c r="E36" s="35"/>
-      <c r="F36" s="36"/>
-      <c r="G36" s="42"/>
-      <c r="H36" s="36"/>
+      <c r="B36" s="38"/>
+      <c r="C36" s="34"/>
+      <c r="D36" s="27"/>
+      <c r="E36" s="32"/>
+      <c r="F36" s="33"/>
+      <c r="G36" s="39"/>
+      <c r="H36" s="33"/>
       <c r="I36" s="4"/>
-      <c r="J36" s="29"/>
+      <c r="J36" s="26"/>
       <c r="K36" s="6"/>
       <c r="L36" s="5"/>
       <c r="M36" s="7"/>
       <c r="N36" s="7"/>
-      <c r="O36" s="36"/>
-      <c r="P36" s="36"/>
-      <c r="Q36" s="38"/>
-      <c r="R36" s="39"/>
-      <c r="S36" s="38"/>
-      <c r="T36" s="40"/>
-      <c r="U36" s="38"/>
+      <c r="O36" s="33"/>
+      <c r="P36" s="33"/>
+      <c r="Q36" s="35"/>
+      <c r="R36" s="36"/>
+      <c r="S36" s="35"/>
+      <c r="T36" s="37"/>
+      <c r="U36" s="35"/>
     </row>
     <row r="37" spans="1:21" ht="15">
       <c r="A37" s="3"/>
-      <c r="B37" s="41"/>
-      <c r="C37" s="37"/>
-      <c r="D37" s="30"/>
-      <c r="E37" s="35"/>
-      <c r="F37" s="36"/>
-      <c r="G37" s="42"/>
-      <c r="H37" s="36"/>
+      <c r="B37" s="38"/>
+      <c r="C37" s="34"/>
+      <c r="D37" s="27"/>
+      <c r="E37" s="32"/>
+      <c r="F37" s="33"/>
+      <c r="G37" s="39"/>
+      <c r="H37" s="33"/>
       <c r="I37" s="4"/>
-      <c r="J37" s="29"/>
+      <c r="J37" s="26"/>
       <c r="K37" s="6"/>
       <c r="L37" s="5"/>
       <c r="M37" s="7"/>
       <c r="N37" s="7"/>
-      <c r="O37" s="36"/>
-      <c r="P37" s="36"/>
-      <c r="Q37" s="38"/>
-      <c r="R37" s="39"/>
-      <c r="S37" s="38"/>
-      <c r="T37" s="40"/>
-      <c r="U37" s="38"/>
+      <c r="O37" s="33"/>
+      <c r="P37" s="33"/>
+      <c r="Q37" s="35"/>
+      <c r="R37" s="36"/>
+      <c r="S37" s="35"/>
+      <c r="T37" s="37"/>
+      <c r="U37" s="35"/>
     </row>
     <row r="38" spans="1:21" ht="15">
       <c r="A38" s="3"/>
-      <c r="B38" s="41"/>
-      <c r="C38" s="37"/>
-      <c r="D38" s="30"/>
-      <c r="E38" s="35"/>
-      <c r="F38" s="36"/>
-      <c r="G38" s="42"/>
-      <c r="H38" s="36"/>
+      <c r="B38" s="38"/>
+      <c r="C38" s="34"/>
+      <c r="D38" s="27"/>
+      <c r="E38" s="32"/>
+      <c r="F38" s="33"/>
+      <c r="G38" s="39"/>
+      <c r="H38" s="33"/>
       <c r="I38" s="4"/>
-      <c r="J38" s="29"/>
+      <c r="J38" s="26"/>
       <c r="K38" s="6"/>
       <c r="L38" s="5"/>
       <c r="M38" s="7"/>
       <c r="N38" s="7"/>
-      <c r="O38" s="36"/>
-      <c r="P38" s="36"/>
-      <c r="Q38" s="38"/>
-      <c r="R38" s="39"/>
-      <c r="S38" s="38"/>
-      <c r="T38" s="40"/>
-      <c r="U38" s="38"/>
+      <c r="O38" s="33"/>
+      <c r="P38" s="33"/>
+      <c r="Q38" s="35"/>
+      <c r="R38" s="36"/>
+      <c r="S38" s="35"/>
+      <c r="T38" s="37"/>
+      <c r="U38" s="35"/>
     </row>
     <row r="39" spans="1:21" ht="15">
       <c r="A39" s="3"/>
-      <c r="B39" s="41"/>
-      <c r="C39" s="37"/>
-      <c r="D39" s="30"/>
-      <c r="E39" s="35"/>
-      <c r="F39" s="36"/>
-      <c r="G39" s="42"/>
-      <c r="H39" s="36"/>
+      <c r="B39" s="38"/>
+      <c r="C39" s="34"/>
+      <c r="D39" s="27"/>
+      <c r="E39" s="32"/>
+      <c r="F39" s="33"/>
+      <c r="G39" s="39"/>
+      <c r="H39" s="33"/>
       <c r="I39" s="4"/>
-      <c r="J39" s="29"/>
+      <c r="J39" s="26"/>
       <c r="K39" s="6"/>
       <c r="L39" s="5"/>
       <c r="M39" s="7"/>
       <c r="N39" s="7"/>
-      <c r="O39" s="36"/>
-      <c r="P39" s="36"/>
-      <c r="Q39" s="38"/>
-      <c r="R39" s="39"/>
-      <c r="S39" s="38"/>
-      <c r="T39" s="40"/>
-      <c r="U39" s="38"/>
+      <c r="O39" s="33"/>
+      <c r="P39" s="33"/>
+      <c r="Q39" s="35"/>
+      <c r="R39" s="36"/>
+      <c r="S39" s="35"/>
+      <c r="T39" s="37"/>
+      <c r="U39" s="35"/>
     </row>
     <row r="40" spans="1:21" ht="15">
       <c r="A40" s="3"/>
-      <c r="B40" s="41"/>
-      <c r="C40" s="37"/>
-      <c r="D40" s="30"/>
-      <c r="E40" s="35"/>
-      <c r="F40" s="36"/>
-      <c r="G40" s="42"/>
-      <c r="H40" s="36"/>
+      <c r="B40" s="38"/>
+      <c r="C40" s="34"/>
+      <c r="D40" s="27"/>
+      <c r="E40" s="32"/>
+      <c r="F40" s="33"/>
+      <c r="G40" s="39"/>
+      <c r="H40" s="33"/>
       <c r="I40" s="4"/>
-      <c r="J40" s="29"/>
+      <c r="J40" s="26"/>
       <c r="K40" s="6"/>
       <c r="L40" s="5"/>
       <c r="M40" s="7"/>
       <c r="N40" s="7"/>
-      <c r="O40" s="36"/>
-      <c r="P40" s="36"/>
-      <c r="Q40" s="38"/>
-      <c r="R40" s="39"/>
-      <c r="S40" s="38"/>
-      <c r="T40" s="40"/>
-      <c r="U40" s="38"/>
+      <c r="O40" s="33"/>
+      <c r="P40" s="33"/>
+      <c r="Q40" s="35"/>
+      <c r="R40" s="36"/>
+      <c r="S40" s="35"/>
+      <c r="T40" s="37"/>
+      <c r="U40" s="35"/>
     </row>
     <row r="41" spans="1:21" ht="15">
       <c r="A41" s="3"/>
-      <c r="B41" s="41"/>
-      <c r="C41" s="37"/>
-      <c r="D41" s="30"/>
-      <c r="E41" s="35"/>
-      <c r="F41" s="36"/>
-      <c r="G41" s="42"/>
-      <c r="H41" s="36"/>
+      <c r="B41" s="38"/>
+      <c r="C41" s="34"/>
+      <c r="D41" s="27"/>
+      <c r="E41" s="32"/>
+      <c r="F41" s="33"/>
+      <c r="G41" s="39"/>
+      <c r="H41" s="33"/>
       <c r="I41" s="4"/>
-      <c r="J41" s="29"/>
+      <c r="J41" s="26"/>
       <c r="K41" s="6"/>
       <c r="L41" s="5"/>
       <c r="M41" s="7"/>
       <c r="N41" s="7"/>
-      <c r="O41" s="36"/>
-      <c r="P41" s="36"/>
-      <c r="Q41" s="38"/>
-      <c r="R41" s="39"/>
-      <c r="S41" s="38"/>
-      <c r="T41" s="40"/>
-      <c r="U41" s="38"/>
+      <c r="O41" s="33"/>
+      <c r="P41" s="33"/>
+      <c r="Q41" s="35"/>
+      <c r="R41" s="36"/>
+      <c r="S41" s="35"/>
+      <c r="T41" s="37"/>
+      <c r="U41" s="35"/>
     </row>
     <row r="42" spans="1:21" ht="15">
       <c r="A42" s="3"/>
-      <c r="B42" s="41"/>
-      <c r="C42" s="37"/>
-      <c r="D42" s="30"/>
-      <c r="E42" s="35"/>
-      <c r="F42" s="36"/>
-      <c r="G42" s="42"/>
-      <c r="H42" s="36"/>
+      <c r="B42" s="38"/>
+      <c r="C42" s="34"/>
+      <c r="D42" s="27"/>
+      <c r="E42" s="32"/>
+      <c r="F42" s="33"/>
+      <c r="G42" s="39"/>
+      <c r="H42" s="33"/>
       <c r="I42" s="4"/>
-      <c r="J42" s="29"/>
+      <c r="J42" s="26"/>
       <c r="K42" s="6"/>
       <c r="L42" s="5"/>
       <c r="M42" s="7"/>
       <c r="N42" s="7"/>
-      <c r="O42" s="36"/>
-      <c r="P42" s="36"/>
-      <c r="Q42" s="38"/>
-      <c r="R42" s="39"/>
-      <c r="S42" s="38"/>
-      <c r="T42" s="40"/>
-      <c r="U42" s="38"/>
+      <c r="O42" s="33"/>
+      <c r="P42" s="33"/>
+      <c r="Q42" s="35"/>
+      <c r="R42" s="36"/>
+      <c r="S42" s="35"/>
+      <c r="T42" s="37"/>
+      <c r="U42" s="35"/>
     </row>
     <row r="43" spans="1:21" ht="15">
       <c r="A43" s="3"/>
-      <c r="B43" s="41"/>
-      <c r="C43" s="37"/>
-      <c r="D43" s="30"/>
-      <c r="E43" s="35"/>
-      <c r="F43" s="36"/>
-      <c r="G43" s="42"/>
-      <c r="H43" s="36"/>
+      <c r="B43" s="38"/>
+      <c r="C43" s="34"/>
+      <c r="D43" s="27"/>
+      <c r="E43" s="32"/>
+      <c r="F43" s="33"/>
+      <c r="G43" s="39"/>
+      <c r="H43" s="33"/>
       <c r="I43" s="4"/>
-      <c r="J43" s="29"/>
+      <c r="J43" s="26"/>
       <c r="K43" s="6"/>
       <c r="L43" s="5"/>
       <c r="M43" s="7"/>
       <c r="N43" s="7"/>
-      <c r="O43" s="36"/>
-      <c r="P43" s="36"/>
-      <c r="Q43" s="38"/>
-      <c r="R43" s="39"/>
-      <c r="S43" s="38"/>
-      <c r="T43" s="40"/>
-      <c r="U43" s="38"/>
+      <c r="O43" s="33"/>
+      <c r="P43" s="33"/>
+      <c r="Q43" s="35"/>
+      <c r="R43" s="36"/>
+      <c r="S43" s="35"/>
+      <c r="T43" s="37"/>
+      <c r="U43" s="35"/>
     </row>
     <row r="44" spans="1:21" ht="15">
       <c r="A44" s="3"/>
-      <c r="B44" s="41"/>
-      <c r="C44" s="37"/>
-      <c r="D44" s="30"/>
-      <c r="E44" s="35"/>
-      <c r="F44" s="36"/>
-      <c r="G44" s="42"/>
-      <c r="H44" s="36"/>
+      <c r="B44" s="38"/>
+      <c r="C44" s="34"/>
+      <c r="D44" s="27"/>
+      <c r="E44" s="32"/>
+      <c r="F44" s="33"/>
+      <c r="G44" s="39"/>
+      <c r="H44" s="33"/>
       <c r="I44" s="4"/>
-      <c r="J44" s="29"/>
+      <c r="J44" s="26"/>
       <c r="K44" s="6"/>
       <c r="L44" s="5"/>
       <c r="M44" s="7"/>
       <c r="N44" s="7"/>
-      <c r="O44" s="36"/>
-      <c r="P44" s="36"/>
-      <c r="Q44" s="38"/>
-      <c r="R44" s="39"/>
-      <c r="S44" s="38"/>
-      <c r="T44" s="40"/>
-      <c r="U44" s="38"/>
+      <c r="O44" s="33"/>
+      <c r="P44" s="33"/>
+      <c r="Q44" s="35"/>
+      <c r="R44" s="36"/>
+      <c r="S44" s="35"/>
+      <c r="T44" s="37"/>
+      <c r="U44" s="35"/>
     </row>
     <row r="45" spans="1:21" ht="15">
       <c r="A45" s="3"/>
-      <c r="B45" s="41"/>
-      <c r="C45" s="37"/>
-      <c r="D45" s="30"/>
-      <c r="E45" s="35"/>
-      <c r="F45" s="36"/>
-      <c r="G45" s="42"/>
-      <c r="H45" s="36"/>
+      <c r="B45" s="38"/>
+      <c r="C45" s="34"/>
+      <c r="D45" s="27"/>
+      <c r="E45" s="32"/>
+      <c r="F45" s="33"/>
+      <c r="G45" s="39"/>
+      <c r="H45" s="33"/>
       <c r="I45" s="4"/>
-      <c r="J45" s="29"/>
+      <c r="J45" s="26"/>
       <c r="K45" s="6"/>
       <c r="L45" s="5"/>
       <c r="M45" s="7"/>
       <c r="N45" s="7"/>
-      <c r="O45" s="36"/>
-      <c r="P45" s="36"/>
-      <c r="Q45" s="38"/>
-      <c r="R45" s="39"/>
-      <c r="S45" s="38"/>
-      <c r="T45" s="40"/>
-      <c r="U45" s="38"/>
+      <c r="O45" s="33"/>
+      <c r="P45" s="33"/>
+      <c r="Q45" s="35"/>
+      <c r="R45" s="36"/>
+      <c r="S45" s="35"/>
+      <c r="T45" s="37"/>
+      <c r="U45" s="35"/>
     </row>
     <row r="46" spans="1:21" ht="15">
       <c r="A46" s="3"/>
-      <c r="B46" s="41"/>
-      <c r="C46" s="37"/>
-      <c r="D46" s="30"/>
-      <c r="E46" s="35"/>
-      <c r="F46" s="36"/>
-      <c r="G46" s="42"/>
-      <c r="H46" s="36"/>
+      <c r="B46" s="38"/>
+      <c r="C46" s="34"/>
+      <c r="D46" s="27"/>
+      <c r="E46" s="32"/>
+      <c r="F46" s="33"/>
+      <c r="G46" s="39"/>
+      <c r="H46" s="33"/>
       <c r="I46" s="4"/>
-      <c r="J46" s="29"/>
+      <c r="J46" s="26"/>
       <c r="K46" s="6"/>
       <c r="L46" s="5"/>
       <c r="M46" s="7"/>
       <c r="N46" s="7"/>
-      <c r="O46" s="36"/>
-      <c r="P46" s="36"/>
-      <c r="Q46" s="38"/>
-      <c r="R46" s="39"/>
-      <c r="S46" s="38"/>
-      <c r="T46" s="40"/>
-      <c r="U46" s="38"/>
+      <c r="O46" s="33"/>
+      <c r="P46" s="33"/>
+      <c r="Q46" s="35"/>
+      <c r="R46" s="36"/>
+      <c r="S46" s="35"/>
+      <c r="T46" s="37"/>
+      <c r="U46" s="35"/>
     </row>
     <row r="47" spans="1:21" ht="15">
       <c r="A47" s="3"/>
-      <c r="B47" s="41"/>
-      <c r="C47" s="37"/>
-      <c r="D47" s="30"/>
-      <c r="E47" s="35"/>
-      <c r="F47" s="36"/>
-      <c r="G47" s="42"/>
-      <c r="H47" s="36"/>
+      <c r="B47" s="38"/>
+      <c r="C47" s="34"/>
+      <c r="D47" s="27"/>
+      <c r="E47" s="32"/>
+      <c r="F47" s="33"/>
+      <c r="G47" s="39"/>
+      <c r="H47" s="33"/>
       <c r="I47" s="4"/>
-      <c r="J47" s="29"/>
+      <c r="J47" s="26"/>
       <c r="K47" s="6"/>
       <c r="L47" s="5"/>
       <c r="M47" s="7"/>
       <c r="N47" s="7"/>
-      <c r="O47" s="36"/>
-      <c r="P47" s="36"/>
-      <c r="Q47" s="38"/>
-      <c r="R47" s="39"/>
-      <c r="S47" s="38"/>
-      <c r="T47" s="40"/>
-      <c r="U47" s="38"/>
+      <c r="O47" s="33"/>
+      <c r="P47" s="33"/>
+      <c r="Q47" s="35"/>
+      <c r="R47" s="36"/>
+      <c r="S47" s="35"/>
+      <c r="T47" s="37"/>
+      <c r="U47" s="35"/>
     </row>
     <row r="48" spans="1:21" ht="15">
       <c r="A48" s="3"/>
-      <c r="B48" s="41"/>
-      <c r="C48" s="37"/>
-      <c r="D48" s="30"/>
-      <c r="E48" s="35"/>
-      <c r="F48" s="36"/>
-      <c r="G48" s="42"/>
-      <c r="H48" s="36"/>
+      <c r="B48" s="38"/>
+      <c r="C48" s="34"/>
+      <c r="D48" s="27"/>
+      <c r="E48" s="32"/>
+      <c r="F48" s="33"/>
+      <c r="G48" s="39"/>
+      <c r="H48" s="33"/>
       <c r="I48" s="4"/>
-      <c r="J48" s="29"/>
+      <c r="J48" s="26"/>
       <c r="K48" s="6"/>
       <c r="L48" s="5"/>
       <c r="M48" s="7"/>
       <c r="N48" s="7"/>
-      <c r="O48" s="36"/>
-      <c r="P48" s="36"/>
-      <c r="Q48" s="38"/>
-      <c r="R48" s="39"/>
-      <c r="S48" s="38"/>
-      <c r="T48" s="40"/>
-      <c r="U48" s="38"/>
+      <c r="O48" s="33"/>
+      <c r="P48" s="33"/>
+      <c r="Q48" s="35"/>
+      <c r="R48" s="36"/>
+      <c r="S48" s="35"/>
+      <c r="T48" s="37"/>
+      <c r="U48" s="35"/>
     </row>
     <row r="49" spans="1:21" ht="15">
       <c r="A49" s="3"/>
-      <c r="B49" s="41"/>
-      <c r="C49" s="37"/>
-      <c r="D49" s="30"/>
-      <c r="E49" s="35"/>
-      <c r="F49" s="36"/>
-      <c r="G49" s="42"/>
-      <c r="H49" s="36"/>
+      <c r="B49" s="38"/>
+      <c r="C49" s="34"/>
+      <c r="D49" s="27"/>
+      <c r="E49" s="32"/>
+      <c r="F49" s="33"/>
+      <c r="G49" s="39"/>
+      <c r="H49" s="33"/>
       <c r="I49" s="4"/>
-      <c r="J49" s="29"/>
+      <c r="J49" s="26"/>
       <c r="K49" s="6"/>
       <c r="L49" s="5"/>
       <c r="M49" s="7"/>
       <c r="N49" s="7"/>
-      <c r="O49" s="36"/>
-      <c r="P49" s="36"/>
-      <c r="Q49" s="38"/>
-      <c r="R49" s="39"/>
-      <c r="S49" s="38"/>
-      <c r="T49" s="40"/>
-      <c r="U49" s="38"/>
+      <c r="O49" s="33"/>
+      <c r="P49" s="33"/>
+      <c r="Q49" s="35"/>
+      <c r="R49" s="36"/>
+      <c r="S49" s="35"/>
+      <c r="T49" s="37"/>
+      <c r="U49" s="35"/>
     </row>
     <row r="50" spans="1:21" ht="15">
       <c r="A50" s="3"/>
-      <c r="B50" s="41"/>
-      <c r="C50" s="37"/>
-      <c r="D50" s="30"/>
-      <c r="E50" s="35"/>
-      <c r="F50" s="36"/>
-      <c r="G50" s="42"/>
-      <c r="H50" s="36"/>
+      <c r="B50" s="38"/>
+      <c r="C50" s="34"/>
+      <c r="D50" s="27"/>
+      <c r="E50" s="32"/>
+      <c r="F50" s="33"/>
+      <c r="G50" s="39"/>
+      <c r="H50" s="33"/>
       <c r="I50" s="4"/>
-      <c r="J50" s="29"/>
+      <c r="J50" s="26"/>
       <c r="K50" s="6"/>
       <c r="L50" s="5"/>
       <c r="M50" s="7"/>
       <c r="N50" s="7"/>
-      <c r="O50" s="36"/>
-      <c r="P50" s="36"/>
-      <c r="Q50" s="38"/>
-      <c r="R50" s="39"/>
-      <c r="S50" s="38"/>
-      <c r="T50" s="40"/>
-      <c r="U50" s="38"/>
+      <c r="O50" s="33"/>
+      <c r="P50" s="33"/>
+      <c r="Q50" s="35"/>
+      <c r="R50" s="36"/>
+      <c r="S50" s="35"/>
+      <c r="T50" s="37"/>
+      <c r="U50" s="35"/>
     </row>
     <row r="51" spans="1:21" ht="15">
       <c r="A51" s="3"/>
-      <c r="B51" s="41"/>
-      <c r="C51" s="37"/>
-      <c r="D51" s="30"/>
-      <c r="E51" s="35"/>
-      <c r="F51" s="36"/>
-      <c r="G51" s="42"/>
-      <c r="H51" s="36"/>
+      <c r="B51" s="38"/>
+      <c r="C51" s="34"/>
+      <c r="D51" s="27"/>
+      <c r="E51" s="32"/>
+      <c r="F51" s="33"/>
+      <c r="G51" s="39"/>
+      <c r="H51" s="33"/>
       <c r="I51" s="4"/>
-      <c r="J51" s="29"/>
+      <c r="J51" s="26"/>
       <c r="K51" s="6"/>
       <c r="L51" s="5"/>
       <c r="M51" s="7"/>
       <c r="N51" s="7"/>
-      <c r="O51" s="36"/>
-      <c r="P51" s="36"/>
-      <c r="Q51" s="38"/>
-      <c r="R51" s="39"/>
-      <c r="S51" s="38"/>
-      <c r="T51" s="40"/>
-      <c r="U51" s="38"/>
+      <c r="O51" s="33"/>
+      <c r="P51" s="33"/>
+      <c r="Q51" s="35"/>
+      <c r="R51" s="36"/>
+      <c r="S51" s="35"/>
+      <c r="T51" s="37"/>
+      <c r="U51" s="35"/>
     </row>
     <row r="52" spans="1:21" ht="15">
       <c r="A52" s="3"/>
-      <c r="B52" s="41"/>
-      <c r="C52" s="37"/>
-      <c r="D52" s="30"/>
-      <c r="E52" s="35"/>
-      <c r="F52" s="36"/>
-      <c r="G52" s="42"/>
-      <c r="H52" s="36"/>
+      <c r="B52" s="38"/>
+      <c r="C52" s="34"/>
+      <c r="D52" s="27"/>
+      <c r="E52" s="32"/>
+      <c r="F52" s="33"/>
+      <c r="G52" s="39"/>
+      <c r="H52" s="33"/>
       <c r="I52" s="4"/>
-      <c r="J52" s="29"/>
+      <c r="J52" s="26"/>
       <c r="K52" s="6"/>
       <c r="L52" s="5"/>
       <c r="M52" s="7"/>
       <c r="N52" s="7"/>
-      <c r="O52" s="36"/>
-      <c r="P52" s="36"/>
-      <c r="Q52" s="38"/>
-      <c r="R52" s="39"/>
-      <c r="S52" s="38"/>
-      <c r="T52" s="40"/>
-      <c r="U52" s="38"/>
+      <c r="O52" s="33"/>
+      <c r="P52" s="33"/>
+      <c r="Q52" s="35"/>
+      <c r="R52" s="36"/>
+      <c r="S52" s="35"/>
+      <c r="T52" s="37"/>
+      <c r="U52" s="35"/>
     </row>
     <row r="53" spans="1:21" ht="15">
       <c r="A53" s="3"/>
-      <c r="B53" s="41"/>
-      <c r="C53" s="37"/>
-      <c r="D53" s="30"/>
-      <c r="E53" s="35"/>
-      <c r="F53" s="36"/>
-      <c r="G53" s="42"/>
-      <c r="H53" s="36"/>
+      <c r="B53" s="38"/>
+      <c r="C53" s="34"/>
+      <c r="D53" s="27"/>
+      <c r="E53" s="32"/>
+      <c r="F53" s="33"/>
+      <c r="G53" s="39"/>
+      <c r="H53" s="33"/>
       <c r="I53" s="4"/>
-      <c r="J53" s="29"/>
+      <c r="J53" s="26"/>
       <c r="K53" s="6"/>
       <c r="L53" s="5"/>
       <c r="M53" s="7"/>
       <c r="N53" s="7"/>
-      <c r="O53" s="36"/>
-      <c r="P53" s="36"/>
-      <c r="Q53" s="38"/>
-      <c r="R53" s="39"/>
-      <c r="S53" s="38"/>
-      <c r="T53" s="40"/>
-      <c r="U53" s="38"/>
+      <c r="O53" s="33"/>
+      <c r="P53" s="33"/>
+      <c r="Q53" s="35"/>
+      <c r="R53" s="36"/>
+      <c r="S53" s="35"/>
+      <c r="T53" s="37"/>
+      <c r="U53" s="35"/>
     </row>
     <row r="54" spans="1:21" ht="15">
       <c r="A54" s="3"/>
-      <c r="B54" s="41"/>
-      <c r="C54" s="37"/>
-      <c r="D54" s="30"/>
-      <c r="E54" s="35"/>
-      <c r="F54" s="36"/>
-      <c r="G54" s="42"/>
-      <c r="H54" s="36"/>
+      <c r="B54" s="38"/>
+      <c r="C54" s="34"/>
+      <c r="D54" s="27"/>
+      <c r="E54" s="32"/>
+      <c r="F54" s="33"/>
+      <c r="G54" s="39"/>
+      <c r="H54" s="33"/>
       <c r="I54" s="4"/>
-      <c r="J54" s="29"/>
+      <c r="J54" s="26"/>
       <c r="K54" s="6"/>
       <c r="L54" s="5"/>
       <c r="M54" s="7"/>
       <c r="N54" s="7"/>
-      <c r="O54" s="36"/>
-      <c r="P54" s="36"/>
-      <c r="Q54" s="38"/>
-      <c r="R54" s="39"/>
-      <c r="S54" s="38"/>
-      <c r="T54" s="40"/>
-      <c r="U54" s="38"/>
+      <c r="O54" s="33"/>
+      <c r="P54" s="33"/>
+      <c r="Q54" s="35"/>
+      <c r="R54" s="36"/>
+      <c r="S54" s="35"/>
+      <c r="T54" s="37"/>
+      <c r="U54" s="35"/>
     </row>
     <row r="55" spans="1:21" ht="15">
       <c r="A55" s="3"/>
-      <c r="B55" s="41"/>
-      <c r="C55" s="37"/>
-      <c r="D55" s="30"/>
-      <c r="E55" s="35"/>
-      <c r="F55" s="36"/>
-      <c r="G55" s="42"/>
-      <c r="H55" s="36"/>
+      <c r="B55" s="38"/>
+      <c r="C55" s="34"/>
+      <c r="D55" s="27"/>
+      <c r="E55" s="32"/>
+      <c r="F55" s="33"/>
+      <c r="G55" s="39"/>
+      <c r="H55" s="33"/>
       <c r="I55" s="4"/>
-      <c r="J55" s="29"/>
+      <c r="J55" s="26"/>
       <c r="K55" s="6"/>
       <c r="L55" s="5"/>
       <c r="M55" s="7"/>
       <c r="N55" s="7"/>
-      <c r="O55" s="36"/>
-      <c r="P55" s="36"/>
-      <c r="Q55" s="38"/>
-      <c r="R55" s="39"/>
-      <c r="S55" s="38"/>
-      <c r="T55" s="40"/>
-      <c r="U55" s="38"/>
+      <c r="O55" s="33"/>
+      <c r="P55" s="33"/>
+      <c r="Q55" s="35"/>
+      <c r="R55" s="36"/>
+      <c r="S55" s="35"/>
+      <c r="T55" s="37"/>
+      <c r="U55" s="35"/>
     </row>
     <row r="56" spans="1:21" ht="15">
       <c r="A56" s="3"/>
-      <c r="B56" s="41"/>
-      <c r="C56" s="37"/>
-      <c r="D56" s="30"/>
-      <c r="E56" s="35"/>
-      <c r="F56" s="36"/>
-      <c r="G56" s="42"/>
-      <c r="H56" s="36"/>
+      <c r="B56" s="38"/>
+      <c r="C56" s="34"/>
+      <c r="D56" s="27"/>
+      <c r="E56" s="32"/>
+      <c r="F56" s="33"/>
+      <c r="G56" s="39"/>
+      <c r="H56" s="33"/>
       <c r="I56" s="4"/>
-      <c r="J56" s="29"/>
+      <c r="J56" s="26"/>
       <c r="K56" s="6"/>
       <c r="L56" s="5"/>
       <c r="M56" s="7"/>
       <c r="N56" s="7"/>
-      <c r="O56" s="36"/>
-      <c r="P56" s="36"/>
-      <c r="Q56" s="38"/>
-      <c r="R56" s="39"/>
-      <c r="S56" s="38"/>
-      <c r="T56" s="40"/>
-      <c r="U56" s="38"/>
+      <c r="O56" s="33"/>
+      <c r="P56" s="33"/>
+      <c r="Q56" s="35"/>
+      <c r="R56" s="36"/>
+      <c r="S56" s="35"/>
+      <c r="T56" s="37"/>
+      <c r="U56" s="35"/>
     </row>
     <row r="57" spans="1:21" ht="15">
       <c r="A57" s="3"/>
-      <c r="B57" s="41"/>
-      <c r="C57" s="37"/>
-      <c r="D57" s="30"/>
-      <c r="E57" s="35"/>
-      <c r="F57" s="36"/>
-      <c r="G57" s="42"/>
-      <c r="H57" s="36"/>
+      <c r="B57" s="38"/>
+      <c r="C57" s="34"/>
+      <c r="D57" s="27"/>
+      <c r="E57" s="32"/>
+      <c r="F57" s="33"/>
+      <c r="G57" s="39"/>
+      <c r="H57" s="33"/>
       <c r="I57" s="4"/>
-      <c r="J57" s="29"/>
+      <c r="J57" s="26"/>
       <c r="K57" s="6"/>
       <c r="L57" s="5"/>
       <c r="M57" s="7"/>
       <c r="N57" s="7"/>
-      <c r="O57" s="36"/>
-      <c r="P57" s="36"/>
-      <c r="Q57" s="38"/>
-      <c r="R57" s="39"/>
-      <c r="S57" s="38"/>
-      <c r="T57" s="40"/>
-      <c r="U57" s="38"/>
+      <c r="O57" s="33"/>
+      <c r="P57" s="33"/>
+      <c r="Q57" s="35"/>
+      <c r="R57" s="36"/>
+      <c r="S57" s="35"/>
+      <c r="T57" s="37"/>
+      <c r="U57" s="35"/>
     </row>
     <row r="58" spans="1:21" ht="15">
       <c r="A58" s="3"/>
-      <c r="B58" s="41"/>
-      <c r="C58" s="37"/>
-      <c r="D58" s="30"/>
-      <c r="E58" s="35"/>
-      <c r="F58" s="36"/>
-      <c r="G58" s="42"/>
-      <c r="H58" s="36"/>
+      <c r="B58" s="38"/>
+      <c r="C58" s="34"/>
+      <c r="D58" s="27"/>
+      <c r="E58" s="32"/>
+      <c r="F58" s="33"/>
+      <c r="G58" s="39"/>
+      <c r="H58" s="33"/>
       <c r="I58" s="4"/>
-      <c r="J58" s="29"/>
+      <c r="J58" s="26"/>
       <c r="K58" s="6"/>
       <c r="L58" s="5"/>
       <c r="M58" s="7"/>
       <c r="N58" s="7"/>
-      <c r="O58" s="36"/>
-      <c r="P58" s="36"/>
-      <c r="Q58" s="38"/>
-      <c r="R58" s="39"/>
-      <c r="S58" s="38"/>
-      <c r="T58" s="40"/>
-      <c r="U58" s="38"/>
+      <c r="O58" s="33"/>
+      <c r="P58" s="33"/>
+      <c r="Q58" s="35"/>
+      <c r="R58" s="36"/>
+      <c r="S58" s="35"/>
+      <c r="T58" s="37"/>
+      <c r="U58" s="35"/>
     </row>
     <row r="59" spans="1:21" ht="15">
       <c r="A59" s="3"/>
-      <c r="B59" s="41"/>
-      <c r="C59" s="37"/>
-      <c r="D59" s="30"/>
-      <c r="E59" s="35"/>
-      <c r="F59" s="36"/>
-      <c r="G59" s="42"/>
-      <c r="H59" s="36"/>
+      <c r="B59" s="38"/>
+      <c r="C59" s="34"/>
+      <c r="D59" s="27"/>
+      <c r="E59" s="32"/>
+      <c r="F59" s="33"/>
+      <c r="G59" s="39"/>
+      <c r="H59" s="33"/>
       <c r="I59" s="4"/>
-      <c r="J59" s="29"/>
+      <c r="J59" s="26"/>
       <c r="K59" s="6"/>
       <c r="L59" s="5"/>
       <c r="M59" s="7"/>
       <c r="N59" s="7"/>
-      <c r="O59" s="36"/>
-      <c r="P59" s="36"/>
-      <c r="Q59" s="38"/>
-      <c r="R59" s="39"/>
-      <c r="S59" s="38"/>
-      <c r="T59" s="40"/>
-      <c r="U59" s="38"/>
+      <c r="O59" s="33"/>
+      <c r="P59" s="33"/>
+      <c r="Q59" s="35"/>
+      <c r="R59" s="36"/>
+      <c r="S59" s="35"/>
+      <c r="T59" s="37"/>
+      <c r="U59" s="35"/>
     </row>
     <row r="60" spans="1:21" ht="15">
       <c r="A60" s="3"/>
-      <c r="B60" s="41"/>
-      <c r="C60" s="37"/>
-      <c r="D60" s="30"/>
-      <c r="E60" s="35"/>
-      <c r="F60" s="36"/>
-      <c r="G60" s="42"/>
-      <c r="H60" s="36"/>
+      <c r="B60" s="38"/>
+      <c r="C60" s="34"/>
+      <c r="D60" s="27"/>
+      <c r="E60" s="32"/>
+      <c r="F60" s="33"/>
+      <c r="G60" s="39"/>
+      <c r="H60" s="33"/>
       <c r="I60" s="4"/>
-      <c r="J60" s="29"/>
+      <c r="J60" s="26"/>
       <c r="K60" s="6"/>
       <c r="L60" s="5"/>
       <c r="M60" s="7"/>
       <c r="N60" s="7"/>
-      <c r="O60" s="36"/>
-      <c r="P60" s="36"/>
-      <c r="Q60" s="38"/>
-      <c r="R60" s="39"/>
-      <c r="S60" s="38"/>
-      <c r="T60" s="40"/>
-      <c r="U60" s="38"/>
+      <c r="O60" s="33"/>
+      <c r="P60" s="33"/>
+      <c r="Q60" s="35"/>
+      <c r="R60" s="36"/>
+      <c r="S60" s="35"/>
+      <c r="T60" s="37"/>
+      <c r="U60" s="35"/>
     </row>
     <row r="61" spans="1:21" ht="15">
       <c r="A61" s="3"/>
-      <c r="B61" s="41"/>
-      <c r="C61" s="37"/>
-      <c r="D61" s="30"/>
-      <c r="E61" s="35"/>
-      <c r="F61" s="36"/>
-      <c r="G61" s="42"/>
-      <c r="H61" s="36"/>
+      <c r="B61" s="38"/>
+      <c r="C61" s="34"/>
+      <c r="D61" s="27"/>
+      <c r="E61" s="32"/>
+      <c r="F61" s="33"/>
+      <c r="G61" s="39"/>
+      <c r="H61" s="33"/>
       <c r="I61" s="4"/>
-      <c r="J61" s="29"/>
+      <c r="J61" s="26"/>
       <c r="K61" s="6"/>
       <c r="L61" s="5"/>
       <c r="M61" s="7"/>
       <c r="N61" s="7"/>
-      <c r="O61" s="36"/>
-      <c r="P61" s="36"/>
-      <c r="Q61" s="38"/>
-      <c r="R61" s="39"/>
-      <c r="S61" s="38"/>
-      <c r="T61" s="40"/>
-      <c r="U61" s="38"/>
+      <c r="O61" s="33"/>
+      <c r="P61" s="33"/>
+      <c r="Q61" s="35"/>
+      <c r="R61" s="36"/>
+      <c r="S61" s="35"/>
+      <c r="T61" s="37"/>
+      <c r="U61" s="35"/>
     </row>
     <row r="62" spans="1:21" ht="15">
       <c r="A62" s="3"/>
-      <c r="B62" s="41"/>
-      <c r="C62" s="37"/>
-      <c r="D62" s="30"/>
-      <c r="E62" s="35"/>
-      <c r="F62" s="36"/>
-      <c r="G62" s="42"/>
-      <c r="H62" s="36"/>
+      <c r="B62" s="38"/>
+      <c r="C62" s="34"/>
+      <c r="D62" s="27"/>
+      <c r="E62" s="32"/>
+      <c r="F62" s="33"/>
+      <c r="G62" s="39"/>
+      <c r="H62" s="33"/>
       <c r="I62" s="4"/>
-      <c r="J62" s="29"/>
+      <c r="J62" s="26"/>
       <c r="K62" s="6"/>
       <c r="L62" s="5"/>
       <c r="M62" s="7"/>
       <c r="N62" s="7"/>
-      <c r="O62" s="36"/>
-      <c r="P62" s="36"/>
-      <c r="Q62" s="38"/>
-      <c r="R62" s="39"/>
-      <c r="S62" s="38"/>
-      <c r="T62" s="40"/>
-      <c r="U62" s="38"/>
+      <c r="O62" s="33"/>
+      <c r="P62" s="33"/>
+      <c r="Q62" s="35"/>
+      <c r="R62" s="36"/>
+      <c r="S62" s="35"/>
+      <c r="T62" s="37"/>
+      <c r="U62" s="35"/>
     </row>
     <row r="63" spans="1:21" ht="15">
       <c r="A63" s="3"/>
-      <c r="B63" s="41"/>
-      <c r="C63" s="37"/>
-      <c r="D63" s="30"/>
-      <c r="E63" s="35"/>
-      <c r="F63" s="36"/>
-      <c r="G63" s="42"/>
-      <c r="H63" s="36"/>
+      <c r="B63" s="38"/>
+      <c r="C63" s="34"/>
+      <c r="D63" s="27"/>
+      <c r="E63" s="32"/>
+      <c r="F63" s="33"/>
+      <c r="G63" s="39"/>
+      <c r="H63" s="33"/>
       <c r="I63" s="4"/>
-      <c r="J63" s="29"/>
+      <c r="J63" s="26"/>
       <c r="K63" s="6"/>
       <c r="L63" s="5"/>
       <c r="M63" s="7"/>
       <c r="N63" s="7"/>
-      <c r="O63" s="36"/>
-      <c r="P63" s="36"/>
-      <c r="Q63" s="38"/>
-      <c r="R63" s="39"/>
-      <c r="S63" s="38"/>
-      <c r="T63" s="40"/>
-      <c r="U63" s="38"/>
+      <c r="O63" s="33"/>
+      <c r="P63" s="33"/>
+      <c r="Q63" s="35"/>
+      <c r="R63" s="36"/>
+      <c r="S63" s="35"/>
+      <c r="T63" s="37"/>
+      <c r="U63" s="35"/>
     </row>
     <row r="64" spans="1:21" ht="15">
       <c r="A64" s="3"/>
-      <c r="B64" s="41"/>
-      <c r="C64" s="37"/>
-      <c r="D64" s="30"/>
-      <c r="E64" s="35"/>
-      <c r="F64" s="36"/>
-      <c r="G64" s="42"/>
-      <c r="H64" s="36"/>
+      <c r="B64" s="38"/>
+      <c r="C64" s="34"/>
+      <c r="D64" s="27"/>
+      <c r="E64" s="32"/>
+      <c r="F64" s="33"/>
+      <c r="G64" s="39"/>
+      <c r="H64" s="33"/>
       <c r="I64" s="4"/>
-      <c r="J64" s="29"/>
+      <c r="J64" s="26"/>
       <c r="K64" s="6"/>
       <c r="L64" s="5"/>
       <c r="M64" s="7"/>
       <c r="N64" s="7"/>
-      <c r="O64" s="36"/>
-      <c r="P64" s="36"/>
-      <c r="Q64" s="38"/>
-      <c r="R64" s="39"/>
-      <c r="S64" s="38"/>
-      <c r="T64" s="40"/>
-      <c r="U64" s="38"/>
+      <c r="O64" s="33"/>
+      <c r="P64" s="33"/>
+      <c r="Q64" s="35"/>
+      <c r="R64" s="36"/>
+      <c r="S64" s="35"/>
+      <c r="T64" s="37"/>
+      <c r="U64" s="35"/>
     </row>
     <row r="65" spans="1:21" ht="15">
       <c r="A65" s="3"/>
-      <c r="B65" s="41"/>
-      <c r="C65" s="37"/>
-      <c r="D65" s="30"/>
-      <c r="E65" s="35"/>
-      <c r="F65" s="36"/>
-      <c r="G65" s="42"/>
-      <c r="H65" s="36"/>
+      <c r="B65" s="38"/>
+      <c r="C65" s="34"/>
+      <c r="D65" s="27"/>
+      <c r="E65" s="32"/>
+      <c r="F65" s="33"/>
+      <c r="G65" s="39"/>
+      <c r="H65" s="33"/>
       <c r="I65" s="4"/>
-      <c r="J65" s="29"/>
+      <c r="J65" s="26"/>
       <c r="K65" s="6"/>
       <c r="L65" s="5"/>
       <c r="M65" s="7"/>
       <c r="N65" s="7"/>
-      <c r="O65" s="36"/>
-      <c r="P65" s="36"/>
-      <c r="Q65" s="38"/>
-      <c r="R65" s="39"/>
-      <c r="S65" s="38"/>
-      <c r="T65" s="40"/>
-      <c r="U65" s="38"/>
+      <c r="O65" s="33"/>
+      <c r="P65" s="33"/>
+      <c r="Q65" s="35"/>
+      <c r="R65" s="36"/>
+      <c r="S65" s="35"/>
+      <c r="T65" s="37"/>
+      <c r="U65" s="35"/>
     </row>
     <row r="66" spans="1:21" ht="15">
       <c r="A66" s="3"/>
-      <c r="B66" s="41"/>
-      <c r="C66" s="37"/>
-      <c r="D66" s="30"/>
-      <c r="E66" s="35"/>
-      <c r="F66" s="36"/>
-      <c r="G66" s="42"/>
-      <c r="H66" s="36"/>
+      <c r="B66" s="38"/>
+      <c r="C66" s="34"/>
+      <c r="D66" s="27"/>
+      <c r="E66" s="32"/>
+      <c r="F66" s="33"/>
+      <c r="G66" s="39"/>
+      <c r="H66" s="33"/>
       <c r="I66" s="4"/>
-      <c r="J66" s="29"/>
+      <c r="J66" s="26"/>
       <c r="K66" s="6"/>
       <c r="L66" s="5"/>
       <c r="M66" s="7"/>
       <c r="N66" s="7"/>
-      <c r="O66" s="36"/>
-      <c r="P66" s="36"/>
-      <c r="Q66" s="38"/>
-      <c r="R66" s="39"/>
-      <c r="S66" s="38"/>
-      <c r="T66" s="40"/>
-      <c r="U66" s="38"/>
+      <c r="O66" s="33"/>
+      <c r="P66" s="33"/>
+      <c r="Q66" s="35"/>
+      <c r="R66" s="36"/>
+      <c r="S66" s="35"/>
+      <c r="T66" s="37"/>
+      <c r="U66" s="35"/>
     </row>
     <row r="67" spans="1:21" ht="15">
       <c r="A67" s="3"/>
-      <c r="B67" s="41"/>
-      <c r="C67" s="37"/>
-      <c r="D67" s="30"/>
-      <c r="E67" s="35"/>
-      <c r="F67" s="36"/>
-      <c r="G67" s="42"/>
-      <c r="H67" s="36"/>
+      <c r="B67" s="38"/>
+      <c r="C67" s="34"/>
+      <c r="D67" s="27"/>
+      <c r="E67" s="32"/>
+      <c r="F67" s="33"/>
+      <c r="G67" s="39"/>
+      <c r="H67" s="33"/>
       <c r="I67" s="4"/>
-      <c r="J67" s="29"/>
+      <c r="J67" s="26"/>
       <c r="K67" s="6"/>
       <c r="L67" s="5"/>
       <c r="M67" s="7"/>
       <c r="N67" s="7"/>
-      <c r="O67" s="36"/>
-      <c r="P67" s="36"/>
+      <c r="O67" s="33"/>
+      <c r="P67" s="33"/>
     </row>
     <row r="68" spans="1:21" ht="15">
       <c r="A68" s="3"/>
-      <c r="B68" s="41"/>
-      <c r="C68" s="37"/>
-      <c r="D68" s="30"/>
-      <c r="E68" s="35"/>
-      <c r="F68" s="36"/>
-      <c r="G68" s="42"/>
-      <c r="H68" s="36"/>
+      <c r="B68" s="38"/>
+      <c r="C68" s="34"/>
+      <c r="D68" s="27"/>
+      <c r="E68" s="32"/>
+      <c r="F68" s="33"/>
+      <c r="G68" s="39"/>
+      <c r="H68" s="33"/>
       <c r="I68" s="4"/>
-      <c r="J68" s="29"/>
+      <c r="J68" s="26"/>
       <c r="K68" s="6"/>
       <c r="L68" s="5"/>
       <c r="M68" s="7"/>
       <c r="N68" s="7"/>
-      <c r="O68" s="36"/>
-      <c r="P68" s="36"/>
+      <c r="O68" s="33"/>
+      <c r="P68" s="33"/>
     </row>
     <row r="69" spans="1:21" ht="15">
       <c r="A69" s="3"/>
-      <c r="B69" s="41"/>
-      <c r="C69" s="37"/>
-      <c r="D69" s="30"/>
-      <c r="E69" s="35"/>
-      <c r="F69" s="36"/>
-      <c r="G69" s="42"/>
-      <c r="H69" s="36"/>
+      <c r="B69" s="38"/>
+      <c r="C69" s="34"/>
+      <c r="D69" s="27"/>
+      <c r="E69" s="32"/>
+      <c r="F69" s="33"/>
+      <c r="G69" s="39"/>
+      <c r="H69" s="33"/>
       <c r="I69" s="4"/>
-      <c r="J69" s="29"/>
+      <c r="J69" s="26"/>
       <c r="K69" s="6"/>
       <c r="L69" s="5"/>
       <c r="M69" s="7"/>
       <c r="N69" s="7"/>
-      <c r="O69" s="36"/>
-      <c r="P69" s="36"/>
+      <c r="O69" s="33"/>
+      <c r="P69" s="33"/>
     </row>
     <row r="70" spans="1:21" ht="15">
       <c r="A70" s="3"/>
-      <c r="B70" s="41"/>
-      <c r="C70" s="37"/>
-      <c r="D70" s="30"/>
-      <c r="E70" s="35"/>
-      <c r="F70" s="36"/>
-      <c r="G70" s="42"/>
-      <c r="H70" s="36"/>
+      <c r="B70" s="38"/>
+      <c r="C70" s="34"/>
+      <c r="D70" s="27"/>
+      <c r="E70" s="32"/>
+      <c r="F70" s="33"/>
+      <c r="G70" s="39"/>
+      <c r="H70" s="33"/>
       <c r="I70" s="4"/>
-      <c r="J70" s="29"/>
+      <c r="J70" s="26"/>
       <c r="K70" s="6"/>
       <c r="L70" s="5"/>
       <c r="M70" s="7"/>
       <c r="N70" s="7"/>
-      <c r="O70" s="36"/>
-      <c r="P70" s="36"/>
+      <c r="O70" s="33"/>
+      <c r="P70" s="33"/>
     </row>
     <row r="85" spans="1:1">
-      <c r="A85" s="20" t="s">
+      <c r="A85" s="17" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="86" spans="1:1">
-      <c r="A86" s="20" t="s">
+      <c r="A86" s="17" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="87" spans="1:1">
-      <c r="A87" s="20" t="s">
+      <c r="A87" s="17" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="88" spans="1:1">
-      <c r="A88" s="20" t="s">
+      <c r="A88" s="17" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="89" spans="1:1">
-      <c r="A89" s="20" t="s">
+      <c r="A89" s="17" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="90" spans="1:1">
-      <c r="A90" s="20" t="s">
+      <c r="A90" s="17" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="91" spans="1:1">
-      <c r="A91" s="20" t="s">
+      <c r="A91" s="17" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="92" spans="1:1">
-      <c r="A92" s="20" t="s">
+      <c r="A92" s="17" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="93" spans="1:1">
-      <c r="A93" s="20" t="s">
+      <c r="A93" s="17" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="94" spans="1:1">
-      <c r="A94" s="20" t="s">
+      <c r="A94" s="17" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="95" spans="1:1">
-      <c r="A95" s="20" t="s">
+      <c r="A95" s="17" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="96" spans="1:1">
-      <c r="A96" s="20" t="s">
+      <c r="A96" s="17" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="97" spans="1:1">
-      <c r="A97" s="20" t="s">
+      <c r="A97" s="17" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="98" spans="1:1">
-      <c r="A98" s="20" t="s">
+      <c r="A98" s="17" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="99" spans="1:1">
-      <c r="A99" s="20" t="s">
+      <c r="A99" s="17" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="100" spans="1:1">
-      <c r="A100" s="20" t="s">
+      <c r="A100" s="17" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="101" spans="1:1">
-      <c r="A101" s="20" t="s">
+      <c r="A101" s="17" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="102" spans="1:1">
-      <c r="A102" s="20" t="s">
+      <c r="A102" s="17" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="103" spans="1:1">
-      <c r="A103" s="20" t="s">
+      <c r="A103" s="17" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="104" spans="1:1">
-      <c r="A104" s="20" t="s">
+      <c r="A104" s="17" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="105" spans="1:1">
-      <c r="A105" s="20" t="s">
+      <c r="A105" s="17" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="106" spans="1:1">
-      <c r="A106" s="20" t="s">
+      <c r="A106" s="17" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="107" spans="1:1">
-      <c r="A107" s="20" t="s">
+      <c r="A107" s="17" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="108" spans="1:1">
-      <c r="A108" s="20" t="s">
+      <c r="A108" s="17" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="109" spans="1:1">
-      <c r="A109" s="20" t="s">
+      <c r="A109" s="17" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="110" spans="1:1">
-      <c r="A110" s="20" t="s">
+      <c r="A110" s="17" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="111" spans="1:1">
-      <c r="A111" s="20" t="s">
+      <c r="A111" s="17" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="112" spans="1:1">
-      <c r="A112" s="20" t="s">
+      <c r="A112" s="17" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="113" spans="1:1">
-      <c r="A113" s="20" t="s">
+      <c r="A113" s="17" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="114" spans="1:1">
-      <c r="A114" s="20" t="s">
+      <c r="A114" s="17" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="115" spans="1:1">
-      <c r="A115" s="20" t="s">
+      <c r="A115" s="17" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="116" spans="1:1">
-      <c r="A116" s="20" t="s">
+      <c r="A116" s="17" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="117" spans="1:1">
-      <c r="A117" s="20" t="s">
+      <c r="A117" s="17" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="118" spans="1:1">
-      <c r="A118" s="20" t="s">
+      <c r="A118" s="17" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="119" spans="1:1">
-      <c r="A119" s="20" t="s">
+      <c r="A119" s="17" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="120" spans="1:1">
-      <c r="A120" s="20" t="s">
+      <c r="A120" s="17" t="s">
         <v>116</v>
       </c>
     </row>
     <row r="121" spans="1:1">
-      <c r="A121" s="20" t="s">
+      <c r="A121" s="17" t="s">
         <v>115</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="P1:P2"/>
+    <mergeCell ref="U1:U2"/>
+    <mergeCell ref="T1:T2"/>
+    <mergeCell ref="S1:S2"/>
+    <mergeCell ref="R1:R2"/>
+    <mergeCell ref="Q1:Q2"/>
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="H1:H2"/>
     <mergeCell ref="O1:O2"/>
@@ -4171,12 +4183,6 @@
     <mergeCell ref="D1:D2"/>
     <mergeCell ref="C1:C2"/>
     <mergeCell ref="F1:F2"/>
-    <mergeCell ref="P1:P2"/>
-    <mergeCell ref="U1:U2"/>
-    <mergeCell ref="T1:T2"/>
-    <mergeCell ref="S1:S2"/>
-    <mergeCell ref="R1:R2"/>
-    <mergeCell ref="Q1:Q2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>

</xml_diff>